<commit_message>
- rewrote script updater script   - incorporating renaming of `sentry` data variables to the `nexial` counterparts.   - automatically rename / upgrade old scripts to newest standards (v3).   - no longer need an empty project in order to generate command JSON file.   - no longer uses S3 to use generated command JSON file.  Instead, the same JSON file is stored to local directory prior to distribution.   - update script also reset script's zoom to 100%
Signed-off-by: Mike Liu <mliu@ep.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10305"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD656AA-E947-8143-9783-033BB0D4C7C4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605A1988-3204-5245-866B-E13A0FBA7F9A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="40960" windowHeight="12540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="12540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
-    <sheet name="macros" sheetId="2" r:id="rId2"/>
+    <sheet name="MacroLibrary" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>

</xml_diff>

<commit_message>
- shipped with <a href="https://raw.githubusercontent.com/SeleniumHQ/selenium/master/java/CHANGELOG" class="external-link" target="nexial_external">Selenium v3.13.0</a>. - preliminary support for Electron app automation. To use this,   1. set `nexial.browser` to `electron`.   2. set `nexial.browser.electron.appLocation` to the path of the target Electron application binary/executable.   - most web commands should work. The following commands are currently not supported (by either Electron or the     underlying WebDriver):     - [web &raquo; `maximizeWindow()`](../commands/web/maximizeWindow())     - [web &raquo; `resizeWindow(width,height)`](../commands/web/resizeWindow(width,height))     - [web &raquo; `goBack()`](../commands/web/goBack())     - [web &raquo; `goBackAndWait()`](../commands/web/goBackAndWait())
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -17,7 +17,7 @@
     <definedName name="csv">'#system'!$D$2:$D$4</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$E$2:$E$91</definedName>
+    <definedName name="desktop">'#system'!$E$2:$E$92</definedName>
     <definedName name="excel">'#system'!$F$2:$F$8</definedName>
     <definedName name="external">'#system'!$G$2:$G$3</definedName>
     <definedName name="image">'#system'!$H$2:$H$5</definedName>
@@ -28,7 +28,7 @@
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
     <definedName name="nextgen">'#system'!$K$2:$K$28</definedName>
-    <definedName name="number">'#system'!$M$2:$M$14</definedName>
+    <definedName name="number">'#system'!$M$2:$M$15</definedName>
     <definedName name="pdf">'#system'!$N$2:$N$16</definedName>
     <definedName name="rdbms">'#system'!$O$2:$O$7</definedName>
     <definedName name="ssh">'#system'!$S$2:$S$9</definedName>
@@ -42,7 +42,7 @@
     <definedName name="step">'#system'!$T$2:$T$4</definedName>
     <definedName name="sms">'#system'!$Q$2:$Q$2</definedName>
     <definedName name="sound">'#system'!$R$2:$R$5</definedName>
-    <definedName name="ws.async">'#system'!$Y$2:$Y$7</definedName>
+    <definedName name="ws.async">'#system'!$Y$2:$Y$8</definedName>
   </definedNames>
   <calcPr calcId="150000"/>
   <extLst>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2557" uniqueCount="439">
   <si>
     <t>description</t>
   </si>
@@ -1338,6 +1338,42 @@
   </si>
   <si>
     <t>put(url,body,output)</t>
+  </si>
+  <si>
+    <t>sendKeysToTextBox(name,text1,text2,text3,text4)</t>
+  </si>
+  <si>
+    <t>assertBetween(num,minNum,maxNum)</t>
+  </si>
+  <si>
+    <t>assertEqual(num1,num2)</t>
+  </si>
+  <si>
+    <t>average(variableName,array)</t>
+  </si>
+  <si>
+    <t>ceiling(variableName)</t>
+  </si>
+  <si>
+    <t>decrement(variableName,amount)</t>
+  </si>
+  <si>
+    <t>floor(variableName)</t>
+  </si>
+  <si>
+    <t>increment(variableName,amount)</t>
+  </si>
+  <si>
+    <t>max(variableName,array)</t>
+  </si>
+  <si>
+    <t>min(variableName,array)</t>
+  </si>
+  <si>
+    <t>round(variableName,closestDigit)</t>
+  </si>
+  <si>
+    <t>delete(url,body,output)</t>
   </si>
 </sst>
 </file>
@@ -1345,7 +1381,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="59" x14ac:knownFonts="1">
+  <fonts count="74" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1721,8 +1757,102 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="93">
+  <fills count="120">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2245,8 +2375,161 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="90">
+  <borders count="118">
     <border>
       <left/>
       <right/>
@@ -3133,13 +3416,295 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="87">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -3317,49 +3882,94 @@
     <xf applyFont="true" borderId="0" fillId="0" fontId="43" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="68" borderId="69" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="69" fillId="68" fontId="44" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="45" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="71" borderId="73" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="73" fillId="71" fontId="46" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="74" borderId="77" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="77" fillId="74" fontId="47" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="48" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="77" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="77" fontId="49" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="50" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="80" borderId="81" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="81" fillId="80" fontId="51" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="83" borderId="85" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="85" fillId="83" fontId="52" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="86" borderId="89" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="89" fillId="86" fontId="53" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="86" borderId="89" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="89" fillId="86" fontId="54" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="89" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="89" fontId="55" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="92" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="92" fontId="56" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="89" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="89" fontId="57" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="58" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="95" borderId="97" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="98" borderId="101" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="101" borderId="105" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="104" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="107" borderId="109" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="110" borderId="113" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="113" borderId="117" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="113" borderId="117" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="116" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="119" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="116" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3784,7 +4394,7 @@
         <v>415</v>
       </c>
       <c r="M2" t="s">
-        <v>409</v>
+        <v>428</v>
       </c>
       <c r="N2" t="s">
         <v>246</v>
@@ -3820,7 +4430,7 @@
         <v>176</v>
       </c>
       <c r="Y2" t="s">
-        <v>177</v>
+        <v>438</v>
       </c>
       <c r="Z2" t="s">
         <v>221</v>
@@ -3861,7 +4471,7 @@
         <v>18</v>
       </c>
       <c r="M3" t="s">
-        <v>311</v>
+        <v>429</v>
       </c>
       <c r="N3" t="s">
         <v>233</v>
@@ -3894,7 +4504,7 @@
         <v>362</v>
       </c>
       <c r="Y3" t="s">
-        <v>422</v>
+        <v>177</v>
       </c>
       <c r="Z3" t="s">
         <v>222</v>
@@ -3965,7 +4575,7 @@
         <v>177</v>
       </c>
       <c r="Y4" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Z4" t="s">
         <v>223</v>
@@ -4027,7 +4637,7 @@
         <v>178</v>
       </c>
       <c r="Y5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="Z5" t="s">
         <v>224</v>
@@ -4083,7 +4693,7 @@
         <v>179</v>
       </c>
       <c r="Y6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="Z6" t="s">
         <v>225</v>
@@ -4136,7 +4746,7 @@
         <v>180</v>
       </c>
       <c r="Y7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="Z7" t="s">
         <v>226</v>
@@ -4165,7 +4775,7 @@
         <v>29</v>
       </c>
       <c r="M8" t="s">
-        <v>83</v>
+        <v>430</v>
       </c>
       <c r="N8" t="s">
         <v>238</v>
@@ -4184,6 +4794,9 @@
       </c>
       <c r="X8" t="s">
         <v>181</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>426</v>
       </c>
       <c r="Z8" t="s">
         <v>227</v>
@@ -4209,7 +4822,7 @@
         <v>32</v>
       </c>
       <c r="M9" t="s">
-        <v>84</v>
+        <v>431</v>
       </c>
       <c r="N9" t="s">
         <v>239</v>
@@ -4247,7 +4860,7 @@
         <v>33</v>
       </c>
       <c r="M10" t="s">
-        <v>85</v>
+        <v>432</v>
       </c>
       <c r="N10" t="s">
         <v>240</v>
@@ -4282,7 +4895,7 @@
         <v>36</v>
       </c>
       <c r="M11" t="s">
-        <v>34</v>
+        <v>433</v>
       </c>
       <c r="N11" t="s">
         <v>241</v>
@@ -4311,7 +4924,7 @@
         <v>73</v>
       </c>
       <c r="M12" t="s">
-        <v>86</v>
+        <v>434</v>
       </c>
       <c r="N12" t="s">
         <v>242</v>
@@ -4337,7 +4950,7 @@
         <v>74</v>
       </c>
       <c r="M13" t="s">
-        <v>87</v>
+        <v>435</v>
       </c>
       <c r="N13" t="s">
         <v>247</v>
@@ -4363,7 +4976,7 @@
         <v>75</v>
       </c>
       <c r="M14" t="s">
-        <v>88</v>
+        <v>436</v>
       </c>
       <c r="N14" t="s">
         <v>243</v>
@@ -4388,6 +5001,9 @@
       <c r="I15" t="s">
         <v>76</v>
       </c>
+      <c r="M15" t="s">
+        <v>437</v>
+      </c>
       <c r="N15" t="s">
         <v>244</v>
       </c>
@@ -4996,7 +5612,7 @@
     </row>
     <row r="77">
       <c r="E77" t="s">
-        <v>328</v>
+        <v>427</v>
       </c>
       <c r="U77" t="s">
         <v>197</v>
@@ -5004,7 +5620,7 @@
     </row>
     <row r="78">
       <c r="E78" t="s">
-        <v>266</v>
+        <v>328</v>
       </c>
       <c r="U78" t="s">
         <v>141</v>
@@ -5012,7 +5628,7 @@
     </row>
     <row r="79">
       <c r="E79" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="U79" t="s">
         <v>198</v>
@@ -5020,7 +5636,7 @@
     </row>
     <row r="80">
       <c r="E80" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="U80" t="s">
         <v>199</v>
@@ -5028,7 +5644,7 @@
     </row>
     <row r="81">
       <c r="E81" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="U81" t="s">
         <v>200</v>
@@ -5036,7 +5652,7 @@
     </row>
     <row r="82">
       <c r="E82" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="U82" t="s">
         <v>201</v>
@@ -5044,7 +5660,7 @@
     </row>
     <row r="83">
       <c r="E83" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="U83" t="s">
         <v>216</v>
@@ -5052,7 +5668,7 @@
     </row>
     <row r="84">
       <c r="E84" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="U84" t="s">
         <v>202</v>
@@ -5060,7 +5676,7 @@
     </row>
     <row r="85">
       <c r="E85" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="U85" t="s">
         <v>142</v>
@@ -5068,7 +5684,7 @@
     </row>
     <row r="86">
       <c r="E86" t="s">
-        <v>301</v>
+        <v>269</v>
       </c>
       <c r="U86" t="s">
         <v>381</v>
@@ -5076,7 +5692,7 @@
     </row>
     <row r="87">
       <c r="E87" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="U87" t="s">
         <v>143</v>
@@ -5084,7 +5700,7 @@
     </row>
     <row r="88">
       <c r="E88" t="s">
-        <v>291</v>
+        <v>307</v>
       </c>
       <c r="U88" t="s">
         <v>144</v>
@@ -5092,7 +5708,7 @@
     </row>
     <row r="89">
       <c r="E89" t="s">
-        <v>336</v>
+        <v>291</v>
       </c>
       <c r="U89" t="s">
         <v>145</v>
@@ -5100,7 +5716,7 @@
     </row>
     <row r="90">
       <c r="E90" t="s">
-        <v>273</v>
+        <v>336</v>
       </c>
       <c r="U90" t="s">
         <v>146</v>
@@ -5108,13 +5724,16 @@
     </row>
     <row r="91">
       <c r="E91" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="U91" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="92">
+      <c r="E92" t="s">
+        <v>274</v>
+      </c>
       <c r="U92" t="s">
         <v>148</v>
       </c>

</xml_diff>

<commit_message>
- improved the handling of _crypt_ data variable during output generation.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -14,36 +14,38 @@
   <definedNames>
     <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
     <definedName name="aws.ses">'#system'!$C$2:$C$3</definedName>
-    <definedName name="base">'#system'!$D$2:$D$38</definedName>
-    <definedName name="csv">'#system'!$E$2:$E$5</definedName>
+    <definedName name="base">'#system'!$E$2:$E$38</definedName>
+    <definedName name="csv">'#system'!$F$2:$F$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$F$2:$F$92</definedName>
-    <definedName name="excel">'#system'!$G$2:$G$14</definedName>
-    <definedName name="external">'#system'!$H$2:$H$3</definedName>
-    <definedName name="image">'#system'!$I$2:$I$6</definedName>
-    <definedName name="io">'#system'!$J$2:$J$25</definedName>
-    <definedName name="jms">'#system'!$K$2:$K$4</definedName>
-    <definedName name="json">'#system'!$L$2:$L$16</definedName>
-    <definedName name="mail">'#system'!$M$2:$M$2</definedName>
+    <definedName name="desktop">'#system'!$G$2:$G$92</definedName>
+    <definedName name="excel">'#system'!$H$2:$H$14</definedName>
+    <definedName name="external">'#system'!$I$2:$I$4</definedName>
+    <definedName name="image">'#system'!$J$2:$J$6</definedName>
+    <definedName name="io">'#system'!$K$2:$K$28</definedName>
+    <definedName name="jms">'#system'!$L$2:$L$4</definedName>
+    <definedName name="json">'#system'!$M$2:$M$16</definedName>
+    <definedName name="mail">'#system'!$O$2:$O$2</definedName>
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
     <definedName name="nextgen">'#system'!$K$2:$K$28</definedName>
-    <definedName name="number">'#system'!$N$2:$N$15</definedName>
-    <definedName name="pdf">'#system'!$O$2:$O$16</definedName>
-    <definedName name="rdbms">'#system'!$P$2:$P$7</definedName>
-    <definedName name="redis">'#system'!$Q$2:$Q$10</definedName>
-    <definedName name="sms">'#system'!$R$2:$R$2</definedName>
-    <definedName name="sound">'#system'!$S$2:$S$5</definedName>
-    <definedName name="ssh">'#system'!$T$2:$T$9</definedName>
-    <definedName name="step">'#system'!$U$2:$U$4</definedName>
-    <definedName name="target">'#system'!$A$2:$A$27</definedName>
-    <definedName name="web">'#system'!$V$2:$V$120</definedName>
-    <definedName name="webalert">'#system'!$W$2:$W$8</definedName>
-    <definedName name="webcookie">'#system'!$X$2:$X$8</definedName>
-    <definedName name="ws">'#system'!$Y$2:$Y$17</definedName>
-    <definedName name="ws.async">'#system'!$Z$2:$Z$8</definedName>
-    <definedName name="xml">'#system'!$AA$2:$AA$13</definedName>
+    <definedName name="number">'#system'!$P$2:$P$16</definedName>
+    <definedName name="pdf">'#system'!$Q$2:$Q$16</definedName>
+    <definedName name="rdbms">'#system'!$R$2:$R$7</definedName>
+    <definedName name="redis">'#system'!$S$2:$S$10</definedName>
+    <definedName name="sms">'#system'!$T$2:$T$2</definedName>
+    <definedName name="sound">'#system'!$U$2:$U$5</definedName>
+    <definedName name="ssh">'#system'!$V$2:$V$9</definedName>
+    <definedName name="step">'#system'!$W$2:$W$4</definedName>
+    <definedName name="target">'#system'!$A$2:$A$29</definedName>
+    <definedName name="web">'#system'!$X$2:$X$125</definedName>
+    <definedName name="webalert">'#system'!$Y$2:$Y$8</definedName>
+    <definedName name="webcookie">'#system'!$Z$2:$Z$8</definedName>
+    <definedName name="ws">'#system'!$AA$2:$AA$17</definedName>
+    <definedName name="ws.async">'#system'!$AB$2:$AB$8</definedName>
+    <definedName name="xml">'#system'!$AC$2:$AC$21</definedName>
+    <definedName name="aws.sqs">'#system'!$D$2:$D$5</definedName>
+    <definedName name="macro">'#system'!$N$2:$N$4</definedName>
   </definedNames>
   <calcPr calcId="150000"/>
   <extLst>
@@ -58,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="498">
   <si>
     <t>description</t>
   </si>
@@ -1462,6 +1464,96 @@
   </si>
   <si>
     <t>minify(xml,var)</t>
+  </si>
+  <si>
+    <t>aws.sqs</t>
+  </si>
+  <si>
+    <t>deleteMessage(profile,queue,receiptHandle)</t>
+  </si>
+  <si>
+    <t>receiveMessage(profile,queue,var)</t>
+  </si>
+  <si>
+    <t>receiveMessages(profile,queue,var)</t>
+  </si>
+  <si>
+    <t>sendMessage(profile,queue,message,var)</t>
+  </si>
+  <si>
+    <t>toExcel(csvFile,excel,worksheet,startCell)</t>
+  </si>
+  <si>
+    <t>runProgram(programPathAndParams)</t>
+  </si>
+  <si>
+    <t>runProgramNoWait(programPathAndParams)</t>
+  </si>
+  <si>
+    <t>copyFilesByRegex(sourceDir,regex,target)</t>
+  </si>
+  <si>
+    <t>deleteFilesByRegex(sourceDir,regex)</t>
+  </si>
+  <si>
+    <t>moveFilesByRegex(sourceDir,regex,target)</t>
+  </si>
+  <si>
+    <t>description()</t>
+  </si>
+  <si>
+    <t>expects(var,default)</t>
+  </si>
+  <si>
+    <t>produces(var,value)</t>
+  </si>
+  <si>
+    <t>roundTo(var,closestDigit)</t>
+  </si>
+  <si>
+    <t>whole(var)</t>
+  </si>
+  <si>
+    <t>assertElementsPresent(prefix)</t>
+  </si>
+  <si>
+    <t>assertIENativeMode()</t>
+  </si>
+  <si>
+    <t>clickOffset(locator,x,y)</t>
+  </si>
+  <si>
+    <t>rightClick(locator)</t>
+  </si>
+  <si>
+    <t>saveAttributeList(var,locator,attrName)</t>
+  </si>
+  <si>
+    <t>saveValues(var,locator)</t>
+  </si>
+  <si>
+    <t>append(xml,xpath,content,var)</t>
+  </si>
+  <si>
+    <t>clear(xml,xpath,var)</t>
+  </si>
+  <si>
+    <t>delete(xml,xpath,var)</t>
+  </si>
+  <si>
+    <t>insertAfter(xml,xpath,content,var)</t>
+  </si>
+  <si>
+    <t>insertBefore(xml,xpath,content,var)</t>
+  </si>
+  <si>
+    <t>prepend(xml,xpath,content,var)</t>
+  </si>
+  <si>
+    <t>replace(xml,xpath,content,var)</t>
+  </si>
+  <si>
+    <t>replaceIn(xml,xpath,content,var)</t>
   </si>
 </sst>
 </file>
@@ -1469,7 +1561,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1624,8 +1716,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="823C3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="30">
+  <fills count="57">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1791,8 +1984,161 @@
         <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6D7D7"/>
+        <bgColor rgb="E6D7D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="58">
     <border>
       <left/>
       <right/>
@@ -2097,13 +2443,295 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="53">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -2173,52 +2801,100 @@
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="9" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="9" fillId="5" fontId="8" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="13" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="13" fillId="8" fontId="10" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="17" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="17" fillId="11" fontId="11" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="17" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="17" fillId="14" fontId="12" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="17" fontId="14" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="21" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="21" fillId="20" fontId="16" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="25" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="25" fillId="23" fontId="17" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="29" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="29" fillId="26" fontId="18" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="29" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="29" fillId="26" fontId="19" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="14" fontId="20" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="29" fontId="21" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="14" fontId="22" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="37" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="41" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="38" borderId="45" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="41" borderId="45" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="44" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="47" borderId="49" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="50" borderId="53" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="53" borderId="57" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="53" borderId="57" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="41" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="56" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="41" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2516,7 +3192,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB120"/>
+  <dimension ref="A1:AD125"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -2536,75 +3212,81 @@
         <v>446</v>
       </c>
       <c r="D1" t="s">
+        <v>468</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>340</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>326</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>17</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>246</v>
+      </c>
+      <c r="O1" t="s">
         <v>188</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>44</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>230</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>387</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>403</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>404</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>350</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>388</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>46</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>47</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>48</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>49</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>405</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>218</v>
       </c>
     </row>
@@ -2619,76 +3301,82 @@
         <v>447</v>
       </c>
       <c r="D2" t="s">
+        <v>469</v>
+      </c>
+      <c r="E2" t="s">
         <v>50</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>64</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>66</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>441</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>71</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>452</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>308</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>377</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>426</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
+        <v>479</v>
+      </c>
+      <c r="O2" t="s">
         <v>408</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>421</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>244</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>209</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>389</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>410</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>411</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V2" t="s">
         <v>374</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>398</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>89</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>163</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>168</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AA2" t="s">
         <v>175</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>423</v>
       </c>
-      <c r="AA2" t="s">
-        <v>219</v>
+      <c r="AC2" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="3">
@@ -2702,1521 +3390,1609 @@
         <v>448</v>
       </c>
       <c r="D3" t="s">
+        <v>470</v>
+      </c>
+      <c r="E3" t="s">
         <v>449</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>358</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>80</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>41</v>
       </c>
-      <c r="H3" t="s">
-        <v>21</v>
-      </c>
       <c r="I3" t="s">
+        <v>474</v>
+      </c>
+      <c r="J3" t="s">
         <v>342</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>334</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>327</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>78</v>
       </c>
       <c r="N3" t="s">
+        <v>480</v>
+      </c>
+      <c r="P3" t="s">
         <v>422</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>231</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>210</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="S3" t="s">
         <v>390</v>
       </c>
-      <c r="S3" t="s">
+      <c r="U3" t="s">
         <v>412</v>
       </c>
-      <c r="T3" t="s">
+      <c r="V3" t="s">
         <v>375</v>
       </c>
-      <c r="U3" t="s">
+      <c r="W3" t="s">
         <v>399</v>
       </c>
-      <c r="V3" t="s">
+      <c r="X3" t="s">
         <v>90</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Y3" t="s">
         <v>164</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Z3" t="s">
         <v>169</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AA3" t="s">
         <v>357</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AB3" t="s">
         <v>176</v>
       </c>
-      <c r="AA3" t="s">
-        <v>220</v>
+      <c r="AC3" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>468</v>
       </c>
       <c r="B4" t="s">
         <v>367</v>
       </c>
       <c r="D4" t="s">
+        <v>471</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>65</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>380</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>442</v>
       </c>
       <c r="I4" t="s">
+        <v>475</v>
+      </c>
+      <c r="J4" t="s">
         <v>343</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>229</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>328</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>18</v>
       </c>
       <c r="N4" t="s">
+        <v>481</v>
+      </c>
+      <c r="P4" t="s">
         <v>19</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>232</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>211</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
         <v>391</v>
       </c>
-      <c r="S4" t="s">
+      <c r="U4" t="s">
         <v>413</v>
       </c>
-      <c r="T4" t="s">
+      <c r="V4" t="s">
         <v>351</v>
       </c>
-      <c r="U4" t="s">
+      <c r="W4" t="s">
         <v>400</v>
       </c>
-      <c r="V4" t="s">
+      <c r="X4" t="s">
         <v>347</v>
       </c>
-      <c r="W4" t="s">
+      <c r="Y4" t="s">
         <v>165</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Z4" t="s">
         <v>170</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AA4" t="s">
         <v>176</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AB4" t="s">
         <v>415</v>
       </c>
-      <c r="AA4" t="s">
-        <v>221</v>
+      <c r="AC4" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>368</v>
       </c>
       <c r="D5" t="s">
+        <v>472</v>
+      </c>
+      <c r="E5" t="s">
         <v>450</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>424</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>329</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>451</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>344</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>453</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>79</v>
       </c>
-      <c r="N5" t="s">
+      <c r="P5" t="s">
         <v>23</v>
       </c>
-      <c r="O5" t="s">
+      <c r="Q5" t="s">
         <v>233</v>
       </c>
-      <c r="P5" t="s">
+      <c r="R5" t="s">
         <v>212</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="S5" t="s">
         <v>392</v>
       </c>
-      <c r="S5" t="s">
+      <c r="U5" t="s">
         <v>414</v>
       </c>
-      <c r="T5" t="s">
+      <c r="V5" t="s">
         <v>352</v>
       </c>
-      <c r="V5" t="s">
+      <c r="X5" t="s">
         <v>348</v>
       </c>
-      <c r="W5" t="s">
+      <c r="Y5" t="s">
         <v>166</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Z5" t="s">
         <v>171</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="AA5" t="s">
         <v>177</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AB5" t="s">
         <v>416</v>
       </c>
-      <c r="AA5" t="s">
-        <v>222</v>
+      <c r="AC5" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
         <v>369</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>20</v>
       </c>
       <c r="F6" t="s">
+        <v>473</v>
+      </c>
+      <c r="G6" t="s">
         <v>381</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>439</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>341</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>64</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>22</v>
       </c>
-      <c r="N6" t="s">
+      <c r="P6" t="s">
         <v>24</v>
       </c>
-      <c r="O6" t="s">
+      <c r="Q6" t="s">
         <v>234</v>
       </c>
-      <c r="P6" t="s">
+      <c r="R6" t="s">
         <v>384</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="S6" t="s">
         <v>393</v>
       </c>
-      <c r="T6" t="s">
+      <c r="V6" t="s">
         <v>354</v>
       </c>
-      <c r="V6" t="s">
+      <c r="X6" t="s">
         <v>91</v>
       </c>
-      <c r="W6" t="s">
+      <c r="Y6" t="s">
         <v>436</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Z6" t="s">
         <v>172</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="AA6" t="s">
         <v>178</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AB6" t="s">
         <v>417</v>
       </c>
-      <c r="AA6" t="s">
-        <v>223</v>
+      <c r="AC6" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>370</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>215</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>359</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>438</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>12</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>308</v>
       </c>
-      <c r="N7" t="s">
+      <c r="P7" t="s">
         <v>26</v>
       </c>
-      <c r="O7" t="s">
+      <c r="Q7" t="s">
         <v>235</v>
       </c>
-      <c r="P7" t="s">
+      <c r="R7" t="s">
         <v>409</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="S7" t="s">
         <v>394</v>
       </c>
-      <c r="T7" t="s">
+      <c r="V7" t="s">
         <v>353</v>
       </c>
-      <c r="V7" t="s">
+      <c r="X7" t="s">
         <v>92</v>
       </c>
-      <c r="W7" t="s">
+      <c r="Y7" t="s">
         <v>437</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Z7" t="s">
         <v>173</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="AA7" t="s">
         <v>179</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AB7" t="s">
         <v>418</v>
       </c>
-      <c r="AA7" t="s">
-        <v>224</v>
+      <c r="AC7" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>371</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>311</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>360</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>321</v>
       </c>
-      <c r="J8" t="s">
-        <v>72</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="K8" t="s">
+        <v>476</v>
+      </c>
+      <c r="M8" t="s">
         <v>27</v>
       </c>
-      <c r="N8" t="s">
+      <c r="P8" t="s">
         <v>83</v>
       </c>
-      <c r="O8" t="s">
+      <c r="Q8" t="s">
         <v>236</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="S8" t="s">
         <v>395</v>
       </c>
-      <c r="T8" t="s">
+      <c r="V8" t="s">
         <v>355</v>
       </c>
-      <c r="V8" t="s">
+      <c r="X8" t="s">
         <v>93</v>
       </c>
-      <c r="W8" t="s">
+      <c r="Y8" t="s">
         <v>167</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Z8" t="s">
         <v>174</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="AA8" t="s">
         <v>180</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AB8" t="s">
         <v>419</v>
       </c>
-      <c r="AA8" t="s">
-        <v>225</v>
+      <c r="AC8" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>340</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>372</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>25</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>299</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>322</v>
       </c>
-      <c r="J9" t="s">
-        <v>31</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="K9" t="s">
+        <v>72</v>
+      </c>
+      <c r="M9" t="s">
         <v>28</v>
       </c>
-      <c r="N9" t="s">
+      <c r="P9" t="s">
         <v>84</v>
       </c>
-      <c r="O9" t="s">
+      <c r="Q9" t="s">
         <v>237</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="S9" t="s">
         <v>396</v>
       </c>
-      <c r="T9" t="s">
+      <c r="V9" t="s">
         <v>356</v>
       </c>
-      <c r="V9" t="s">
+      <c r="X9" t="s">
         <v>201</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="AA9" t="s">
         <v>181</v>
       </c>
-      <c r="AA9" t="s">
-        <v>466</v>
+      <c r="AC9" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
+        <v>340</v>
+      </c>
+      <c r="E10" t="s">
         <v>308</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>345</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>443</v>
       </c>
-      <c r="J10" t="s">
-        <v>383</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="K10" t="s">
+        <v>31</v>
+      </c>
+      <c r="M10" t="s">
         <v>29</v>
       </c>
-      <c r="N10" t="s">
+      <c r="P10" t="s">
         <v>428</v>
       </c>
-      <c r="O10" t="s">
+      <c r="Q10" t="s">
         <v>238</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="S10" t="s">
         <v>397</v>
       </c>
-      <c r="V10" t="s">
+      <c r="X10" t="s">
         <v>250</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="AA10" t="s">
         <v>182</v>
       </c>
-      <c r="AA10" t="s">
-        <v>467</v>
+      <c r="AC10" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>326</v>
-      </c>
-      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
         <v>249</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>267</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>315</v>
       </c>
-      <c r="J11" t="s">
-        <v>13</v>
-      </c>
-      <c r="L11" t="s">
+      <c r="K11" t="s">
+        <v>477</v>
+      </c>
+      <c r="M11" t="s">
         <v>463</v>
       </c>
-      <c r="N11" t="s">
+      <c r="P11" t="s">
         <v>85</v>
       </c>
-      <c r="O11" t="s">
+      <c r="Q11" t="s">
         <v>239</v>
       </c>
-      <c r="V11" t="s">
+      <c r="X11" t="s">
         <v>251</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="AA11" t="s">
         <v>252</v>
       </c>
-      <c r="AA11" t="s">
-        <v>226</v>
+      <c r="AC11" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
+        <v>326</v>
+      </c>
+      <c r="E12" t="s">
         <v>312</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>256</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>316</v>
       </c>
-      <c r="J12" t="s">
-        <v>35</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="K12" t="s">
+        <v>383</v>
+      </c>
+      <c r="M12" t="s">
         <v>427</v>
       </c>
-      <c r="N12" t="s">
+      <c r="P12" t="s">
         <v>34</v>
       </c>
-      <c r="O12" t="s">
+      <c r="Q12" t="s">
         <v>240</v>
       </c>
-      <c r="V12" t="s">
+      <c r="X12" t="s">
         <v>94</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="AA12" t="s">
         <v>183</v>
       </c>
-      <c r="AA12" t="s">
-        <v>227</v>
+      <c r="AC12" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>188</v>
-      </c>
-      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
         <v>334</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>309</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>317</v>
       </c>
-      <c r="J13" t="s">
-        <v>73</v>
-      </c>
-      <c r="L13" t="s">
+      <c r="K13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M13" t="s">
         <v>464</v>
       </c>
-      <c r="N13" t="s">
+      <c r="P13" t="s">
         <v>86</v>
       </c>
-      <c r="O13" t="s">
+      <c r="Q13" t="s">
         <v>245</v>
       </c>
-      <c r="V13" t="s">
+      <c r="X13" t="s">
         <v>319</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="AA13" t="s">
         <v>184</v>
       </c>
-      <c r="AA13" t="s">
-        <v>228</v>
+      <c r="AC13" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" t="s">
+        <v>246</v>
+      </c>
+      <c r="E14" t="s">
         <v>30</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>257</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>318</v>
       </c>
-      <c r="J14" t="s">
-        <v>74</v>
-      </c>
-      <c r="L14" t="s">
+      <c r="K14" t="s">
+        <v>35</v>
+      </c>
+      <c r="M14" t="s">
         <v>32</v>
       </c>
-      <c r="N14" t="s">
+      <c r="P14" t="s">
         <v>87</v>
       </c>
-      <c r="O14" t="s">
+      <c r="Q14" t="s">
         <v>241</v>
       </c>
-      <c r="V14" t="s">
+      <c r="X14" t="s">
         <v>95</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="AA14" t="s">
         <v>185</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>230</v>
-      </c>
-      <c r="D15" t="s">
+        <v>188</v>
+      </c>
+      <c r="E15" t="s">
         <v>51</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>258</v>
       </c>
-      <c r="J15" t="s">
-        <v>454</v>
-      </c>
-      <c r="L15" t="s">
+      <c r="K15" t="s">
+        <v>478</v>
+      </c>
+      <c r="M15" t="s">
         <v>33</v>
       </c>
-      <c r="N15" t="s">
-        <v>88</v>
-      </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q15" t="s">
         <v>242</v>
       </c>
-      <c r="V15" t="s">
+      <c r="X15" t="s">
         <v>96</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="AA15" t="s">
         <v>186</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" t="s">
         <v>378</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>310</v>
       </c>
-      <c r="J16" t="s">
-        <v>75</v>
-      </c>
-      <c r="L16" t="s">
+      <c r="K16" t="s">
+        <v>73</v>
+      </c>
+      <c r="M16" t="s">
         <v>36</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
+        <v>483</v>
+      </c>
+      <c r="Q16" t="s">
         <v>243</v>
       </c>
-      <c r="V16" t="s">
+      <c r="X16" t="s">
         <v>67</v>
       </c>
-      <c r="Y16" t="s">
+      <c r="AA16" t="s">
         <v>187</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>387</v>
-      </c>
-      <c r="D17" t="s">
+        <v>230</v>
+      </c>
+      <c r="E17" t="s">
         <v>379</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>81</v>
       </c>
-      <c r="J17" t="s">
-        <v>76</v>
-      </c>
-      <c r="V17" t="s">
-        <v>97</v>
-      </c>
-      <c r="Y17" t="s">
+      <c r="K17" t="s">
+        <v>74</v>
+      </c>
+      <c r="X17" t="s">
+        <v>484</v>
+      </c>
+      <c r="AA17" t="s">
         <v>458</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>403</v>
-      </c>
-      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" t="s">
         <v>406</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>82</v>
       </c>
-      <c r="J18" t="s">
-        <v>373</v>
-      </c>
-      <c r="V18" t="s">
-        <v>98</v>
+      <c r="K18" t="s">
+        <v>454</v>
+      </c>
+      <c r="X18" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>404</v>
-      </c>
-      <c r="D19" t="s">
+        <v>387</v>
+      </c>
+      <c r="E19" t="s">
         <v>52</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>289</v>
       </c>
-      <c r="J19" t="s">
-        <v>462</v>
-      </c>
-      <c r="V19" t="s">
-        <v>99</v>
+      <c r="K19" t="s">
+        <v>75</v>
+      </c>
+      <c r="X19" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>350</v>
-      </c>
-      <c r="D20" t="s">
+        <v>403</v>
+      </c>
+      <c r="E20" t="s">
         <v>53</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>290</v>
       </c>
-      <c r="J20" t="s">
-        <v>37</v>
-      </c>
-      <c r="V20" t="s">
-        <v>100</v>
+      <c r="K20" t="s">
+        <v>76</v>
+      </c>
+      <c r="X20" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>388</v>
-      </c>
-      <c r="D21" t="s">
+        <v>404</v>
+      </c>
+      <c r="E21" t="s">
         <v>54</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>291</v>
       </c>
-      <c r="J21" t="s">
-        <v>385</v>
-      </c>
-      <c r="V21" t="s">
-        <v>101</v>
+      <c r="K21" t="s">
+        <v>373</v>
+      </c>
+      <c r="X21" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" t="s">
+        <v>350</v>
+      </c>
+      <c r="E22" t="s">
         <v>314</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>292</v>
       </c>
-      <c r="J22" t="s">
-        <v>77</v>
-      </c>
-      <c r="V22" t="s">
-        <v>102</v>
+      <c r="K22" t="s">
+        <v>462</v>
+      </c>
+      <c r="X22" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" t="s">
+        <v>388</v>
+      </c>
+      <c r="E23" t="s">
         <v>55</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>283</v>
       </c>
-      <c r="J23" t="s">
-        <v>425</v>
-      </c>
-      <c r="V23" t="s">
-        <v>103</v>
+      <c r="K23" t="s">
+        <v>37</v>
+      </c>
+      <c r="X23" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" t="s">
         <v>440</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>272</v>
       </c>
-      <c r="J24" t="s">
-        <v>38</v>
-      </c>
-      <c r="V24" t="s">
-        <v>104</v>
+      <c r="K24" t="s">
+        <v>385</v>
+      </c>
+      <c r="X24" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" t="s">
         <v>216</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>68</v>
       </c>
-      <c r="J25" t="s">
-        <v>39</v>
-      </c>
-      <c r="V25" t="s">
-        <v>105</v>
+      <c r="K25" t="s">
+        <v>77</v>
+      </c>
+      <c r="X25" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>405</v>
-      </c>
-      <c r="D26" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" t="s">
         <v>217</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>275</v>
       </c>
-      <c r="V26" t="s">
-        <v>106</v>
+      <c r="K26" t="s">
+        <v>425</v>
+      </c>
+      <c r="X26" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" t="s">
+        <v>460</v>
+      </c>
+      <c r="G27" t="s">
+        <v>259</v>
+      </c>
+      <c r="K27" t="s">
+        <v>38</v>
+      </c>
+      <c r="X27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>405</v>
+      </c>
+      <c r="E28" t="s">
+        <v>461</v>
+      </c>
+      <c r="G28" t="s">
+        <v>276</v>
+      </c>
+      <c r="K28" t="s">
+        <v>39</v>
+      </c>
+      <c r="X28" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
         <v>218</v>
       </c>
-      <c r="D27" t="s">
-        <v>460</v>
-      </c>
-      <c r="F27" t="s">
-        <v>259</v>
-      </c>
-      <c r="V27" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="D28" t="s">
-        <v>461</v>
-      </c>
-      <c r="F28" t="s">
-        <v>276</v>
-      </c>
-      <c r="V28" t="s">
+      <c r="E29" t="s">
+        <v>407</v>
+      </c>
+      <c r="G29" t="s">
+        <v>277</v>
+      </c>
+      <c r="X29" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="29">
-      <c r="D29" t="s">
-        <v>407</v>
-      </c>
-      <c r="F29" t="s">
-        <v>277</v>
-      </c>
-      <c r="V29" t="s">
+    <row r="30">
+      <c r="E30" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" t="s">
+        <v>208</v>
+      </c>
+      <c r="X30" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="30">
-      <c r="D30" t="s">
-        <v>56</v>
-      </c>
-      <c r="F30" t="s">
-        <v>208</v>
-      </c>
-      <c r="V30" t="s">
+    <row r="31">
+      <c r="E31" t="s">
+        <v>57</v>
+      </c>
+      <c r="G31" t="s">
+        <v>268</v>
+      </c>
+      <c r="X31" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="31">
-      <c r="D31" t="s">
-        <v>57</v>
-      </c>
-      <c r="F31" t="s">
-        <v>268</v>
-      </c>
-      <c r="V31" t="s">
+    <row r="32">
+      <c r="E32" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" t="s">
+        <v>278</v>
+      </c>
+      <c r="X32" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="32">
-      <c r="D32" t="s">
-        <v>58</v>
-      </c>
-      <c r="F32" t="s">
-        <v>278</v>
-      </c>
-      <c r="V32" t="s">
+    <row r="33">
+      <c r="E33" t="s">
+        <v>59</v>
+      </c>
+      <c r="G33" t="s">
+        <v>253</v>
+      </c>
+      <c r="X33" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="33">
-      <c r="D33" t="s">
-        <v>59</v>
-      </c>
-      <c r="F33" t="s">
-        <v>253</v>
-      </c>
-      <c r="V33" t="s">
+    <row r="34">
+      <c r="E34" t="s">
+        <v>60</v>
+      </c>
+      <c r="G34" t="s">
+        <v>323</v>
+      </c>
+      <c r="X34" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="34">
-      <c r="D34" t="s">
-        <v>60</v>
-      </c>
-      <c r="F34" t="s">
-        <v>323</v>
-      </c>
-      <c r="V34" t="s">
+    <row r="35">
+      <c r="E35" t="s">
+        <v>61</v>
+      </c>
+      <c r="G35" t="s">
+        <v>300</v>
+      </c>
+      <c r="X35" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="35">
-      <c r="D35" t="s">
-        <v>61</v>
-      </c>
-      <c r="F35" t="s">
-        <v>300</v>
-      </c>
-      <c r="V35" t="s">
+    <row r="36">
+      <c r="E36" t="s">
+        <v>62</v>
+      </c>
+      <c r="G36" t="s">
+        <v>254</v>
+      </c>
+      <c r="X36" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="36">
-      <c r="D36" t="s">
-        <v>62</v>
-      </c>
-      <c r="F36" t="s">
-        <v>254</v>
-      </c>
-      <c r="V36" t="s">
+    <row r="37">
+      <c r="E37" t="s">
+        <v>63</v>
+      </c>
+      <c r="G37" t="s">
+        <v>301</v>
+      </c>
+      <c r="X37" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="37">
-      <c r="D37" t="s">
-        <v>63</v>
-      </c>
-      <c r="F37" t="s">
-        <v>301</v>
-      </c>
-      <c r="V37" t="s">
+    <row r="38">
+      <c r="G38" t="s">
+        <v>260</v>
+      </c>
+      <c r="X38" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="38">
-      <c r="F38" t="s">
-        <v>260</v>
-      </c>
-      <c r="V38" t="s">
+    <row r="39">
+      <c r="G39" t="s">
+        <v>70</v>
+      </c>
+      <c r="X39" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="39">
-      <c r="F39" t="s">
-        <v>70</v>
-      </c>
-      <c r="V39" t="s">
+    <row r="40">
+      <c r="G40" t="s">
+        <v>204</v>
+      </c>
+      <c r="X40" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="40">
-      <c r="F40" t="s">
-        <v>204</v>
-      </c>
-      <c r="V40" t="s">
+    <row r="41">
+      <c r="G41" t="s">
+        <v>282</v>
+      </c>
+      <c r="X41" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="41">
-      <c r="F41" t="s">
-        <v>282</v>
-      </c>
-      <c r="V41" t="s">
+    <row r="42">
+      <c r="G42" t="s">
+        <v>293</v>
+      </c>
+      <c r="X42" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="42">
-      <c r="F42" t="s">
-        <v>293</v>
-      </c>
-      <c r="V42" t="s">
+    <row r="43">
+      <c r="G43" t="s">
+        <v>294</v>
+      </c>
+      <c r="X43" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="43">
-      <c r="F43" t="s">
-        <v>294</v>
-      </c>
-      <c r="V43" t="s">
+    <row r="44">
+      <c r="G44" t="s">
+        <v>336</v>
+      </c>
+      <c r="X44" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="44">
-      <c r="F44" t="s">
-        <v>336</v>
-      </c>
-      <c r="V44" t="s">
+    <row r="45">
+      <c r="G45" t="s">
+        <v>335</v>
+      </c>
+      <c r="X45" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="45">
-      <c r="F45" t="s">
-        <v>335</v>
-      </c>
-      <c r="V45" t="s">
+    <row r="46">
+      <c r="G46" t="s">
+        <v>203</v>
+      </c>
+      <c r="X46" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="46">
-      <c r="F46" t="s">
-        <v>203</v>
-      </c>
-      <c r="V46" t="s">
+    <row r="47">
+      <c r="G47" t="s">
+        <v>313</v>
+      </c>
+      <c r="X47" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="47">
-      <c r="F47" t="s">
-        <v>313</v>
-      </c>
-      <c r="V47" t="s">
+    <row r="48">
+      <c r="G48" t="s">
+        <v>332</v>
+      </c>
+      <c r="X48" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="48">
-      <c r="F48" t="s">
-        <v>332</v>
-      </c>
-      <c r="V48" t="s">
+    <row r="49">
+      <c r="G49" t="s">
+        <v>361</v>
+      </c>
+      <c r="X49" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="49">
-      <c r="F49" t="s">
-        <v>361</v>
-      </c>
-      <c r="V49" t="s">
+    <row r="50">
+      <c r="G50" t="s">
+        <v>295</v>
+      </c>
+      <c r="X50" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="50">
-      <c r="F50" t="s">
-        <v>295</v>
-      </c>
-      <c r="V50" t="s">
+    <row r="51">
+      <c r="G51" t="s">
+        <v>349</v>
+      </c>
+      <c r="X51" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="51">
-      <c r="F51" t="s">
-        <v>349</v>
-      </c>
-      <c r="V51" t="s">
+    <row r="52">
+      <c r="G52" t="s">
+        <v>324</v>
+      </c>
+      <c r="X52" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="G53" t="s">
+        <v>261</v>
+      </c>
+      <c r="X53" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="52">
-      <c r="F52" t="s">
-        <v>324</v>
-      </c>
-      <c r="V52" t="s">
+    <row r="54">
+      <c r="G54" t="s">
+        <v>285</v>
+      </c>
+      <c r="X54" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="53">
-      <c r="F53" t="s">
-        <v>261</v>
-      </c>
-      <c r="V53" t="s">
+    <row r="55">
+      <c r="G55" t="s">
+        <v>286</v>
+      </c>
+      <c r="X55" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="54">
-      <c r="F54" t="s">
-        <v>285</v>
-      </c>
-      <c r="V54" t="s">
+    <row r="56">
+      <c r="G56" t="s">
+        <v>287</v>
+      </c>
+      <c r="X56" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="55">
-      <c r="F55" t="s">
-        <v>286</v>
-      </c>
-      <c r="V55" t="s">
+    <row r="57">
+      <c r="G57" t="s">
+        <v>296</v>
+      </c>
+      <c r="X57" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="56">
-      <c r="F56" t="s">
-        <v>287</v>
-      </c>
-      <c r="V56" t="s">
+    <row r="58">
+      <c r="G58" t="s">
+        <v>305</v>
+      </c>
+      <c r="X58" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="57">
-      <c r="F57" t="s">
-        <v>296</v>
-      </c>
-      <c r="V57" t="s">
+    <row r="59">
+      <c r="G59" t="s">
+        <v>330</v>
+      </c>
+      <c r="X59" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="58">
-      <c r="F58" t="s">
-        <v>305</v>
-      </c>
-      <c r="V58" t="s">
+    <row r="60">
+      <c r="G60" t="s">
+        <v>302</v>
+      </c>
+      <c r="X60" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="59">
-      <c r="F59" t="s">
-        <v>330</v>
-      </c>
-      <c r="V59" t="s">
+    <row r="61">
+      <c r="G61" t="s">
+        <v>303</v>
+      </c>
+      <c r="X61" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="60">
-      <c r="F60" t="s">
-        <v>302</v>
-      </c>
-      <c r="V60" t="s">
+    <row r="62">
+      <c r="G62" t="s">
+        <v>362</v>
+      </c>
+      <c r="X62" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="61">
-      <c r="F61" t="s">
-        <v>303</v>
-      </c>
-      <c r="V61" t="s">
+    <row r="63">
+      <c r="G63" t="s">
+        <v>363</v>
+      </c>
+      <c r="X63" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="62">
-      <c r="F62" t="s">
-        <v>362</v>
-      </c>
-      <c r="V62" t="s">
+    <row r="64">
+      <c r="G64" t="s">
+        <v>338</v>
+      </c>
+      <c r="X64" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="63">
-      <c r="F63" t="s">
-        <v>363</v>
-      </c>
-      <c r="V63" t="s">
+    <row r="65">
+      <c r="G65" t="s">
+        <v>306</v>
+      </c>
+      <c r="X65" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="64">
-      <c r="F64" t="s">
-        <v>338</v>
-      </c>
-      <c r="V64" t="s">
+    <row r="66">
+      <c r="G66" t="s">
+        <v>262</v>
+      </c>
+      <c r="X66" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="65">
-      <c r="F65" t="s">
-        <v>306</v>
-      </c>
-      <c r="V65" t="s">
+    <row r="67">
+      <c r="G67" t="s">
+        <v>346</v>
+      </c>
+      <c r="X67" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="66">
-      <c r="F66" t="s">
-        <v>262</v>
-      </c>
-      <c r="V66" t="s">
+    <row r="68">
+      <c r="G68" t="s">
+        <v>307</v>
+      </c>
+      <c r="X68" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="67">
-      <c r="F67" t="s">
-        <v>346</v>
-      </c>
-      <c r="V67" t="s">
+    <row r="69">
+      <c r="G69" t="s">
+        <v>401</v>
+      </c>
+      <c r="X69" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="68">
-      <c r="F68" t="s">
-        <v>307</v>
-      </c>
-      <c r="V68" t="s">
+    <row r="70">
+      <c r="G70" t="s">
+        <v>297</v>
+      </c>
+      <c r="X70" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="69">
-      <c r="F69" t="s">
-        <v>401</v>
-      </c>
-      <c r="V69" t="s">
+    <row r="71">
+      <c r="G71" t="s">
+        <v>402</v>
+      </c>
+      <c r="X71" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="70">
-      <c r="F70" t="s">
-        <v>297</v>
-      </c>
-      <c r="V70" t="s">
+    <row r="72">
+      <c r="G72" t="s">
+        <v>255</v>
+      </c>
+      <c r="X72" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="71">
-      <c r="F71" t="s">
-        <v>402</v>
-      </c>
-      <c r="V71" t="s">
+    <row r="73">
+      <c r="G73" t="s">
+        <v>337</v>
+      </c>
+      <c r="X73" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="72">
-      <c r="F72" t="s">
-        <v>255</v>
-      </c>
-      <c r="V72" t="s">
+    <row r="74">
+      <c r="G74" t="s">
+        <v>273</v>
+      </c>
+      <c r="X74" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="73">
-      <c r="F73" t="s">
-        <v>337</v>
-      </c>
-      <c r="V73" t="s">
+    <row r="75">
+      <c r="G75" t="s">
+        <v>279</v>
+      </c>
+      <c r="X75" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="74">
-      <c r="F74" t="s">
-        <v>273</v>
-      </c>
-      <c r="V74" t="s">
+    <row r="76">
+      <c r="G76" t="s">
+        <v>284</v>
+      </c>
+      <c r="X76" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="75">
-      <c r="F75" t="s">
-        <v>279</v>
-      </c>
-      <c r="V75" t="s">
+    <row r="77">
+      <c r="G77" t="s">
+        <v>420</v>
+      </c>
+      <c r="X77" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="76">
-      <c r="F76" t="s">
-        <v>284</v>
-      </c>
-      <c r="V76" t="s">
+    <row r="78">
+      <c r="G78" t="s">
+        <v>325</v>
+      </c>
+      <c r="X78" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="77">
-      <c r="F77" t="s">
-        <v>420</v>
-      </c>
-      <c r="V77" t="s">
+    <row r="79">
+      <c r="G79" t="s">
+        <v>263</v>
+      </c>
+      <c r="X79" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="78">
-      <c r="F78" t="s">
-        <v>325</v>
-      </c>
-      <c r="V78" t="s">
+    <row r="80">
+      <c r="G80" t="s">
+        <v>274</v>
+      </c>
+      <c r="X80" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="G81" t="s">
+        <v>280</v>
+      </c>
+      <c r="X81" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="79">
-      <c r="F79" t="s">
-        <v>263</v>
-      </c>
-      <c r="V79" t="s">
+    <row r="82">
+      <c r="G82" t="s">
+        <v>269</v>
+      </c>
+      <c r="X82" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="80">
-      <c r="F80" t="s">
-        <v>274</v>
-      </c>
-      <c r="V80" t="s">
+    <row r="83">
+      <c r="G83" t="s">
+        <v>264</v>
+      </c>
+      <c r="X83" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="81">
-      <c r="F81" t="s">
-        <v>280</v>
-      </c>
-      <c r="V81" t="s">
+    <row r="84">
+      <c r="G84" t="s">
+        <v>281</v>
+      </c>
+      <c r="X84" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="G85" t="s">
+        <v>265</v>
+      </c>
+      <c r="X85" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="82">
-      <c r="F82" t="s">
-        <v>269</v>
-      </c>
-      <c r="V82" t="s">
+    <row r="86">
+      <c r="G86" t="s">
+        <v>266</v>
+      </c>
+      <c r="X86" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="83">
-      <c r="F83" t="s">
-        <v>264</v>
-      </c>
-      <c r="V83" t="s">
+    <row r="87">
+      <c r="G87" t="s">
+        <v>298</v>
+      </c>
+      <c r="X87" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="84">
-      <c r="F84" t="s">
-        <v>281</v>
-      </c>
-      <c r="V84" t="s">
+    <row r="88">
+      <c r="G88" t="s">
+        <v>304</v>
+      </c>
+      <c r="X88" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="85">
-      <c r="F85" t="s">
-        <v>265</v>
-      </c>
-      <c r="V85" t="s">
+    <row r="89">
+      <c r="G89" t="s">
+        <v>288</v>
+      </c>
+      <c r="X89" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="86">
-      <c r="F86" t="s">
-        <v>266</v>
-      </c>
-      <c r="V86" t="s">
+    <row r="90">
+      <c r="G90" t="s">
+        <v>333</v>
+      </c>
+      <c r="X90" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="87">
-      <c r="F87" t="s">
-        <v>298</v>
-      </c>
-      <c r="V87" t="s">
+    <row r="91">
+      <c r="G91" t="s">
+        <v>270</v>
+      </c>
+      <c r="X91" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="88">
-      <c r="F88" t="s">
-        <v>304</v>
-      </c>
-      <c r="V88" t="s">
+    <row r="92">
+      <c r="G92" t="s">
+        <v>271</v>
+      </c>
+      <c r="X92" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="89">
-      <c r="F89" t="s">
-        <v>288</v>
-      </c>
-      <c r="V89" t="s">
+    <row r="93">
+      <c r="X93" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="90">
-      <c r="F90" t="s">
-        <v>333</v>
-      </c>
-      <c r="V90" t="s">
+    <row r="94">
+      <c r="X94" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="91">
-      <c r="F91" t="s">
-        <v>270</v>
-      </c>
-      <c r="V91" t="s">
+    <row r="95">
+      <c r="X95" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="92">
-      <c r="F92" t="s">
-        <v>271</v>
-      </c>
-      <c r="V92" t="s">
+    <row r="96">
+      <c r="X96" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="93">
-      <c r="V93" t="s">
+    <row r="97">
+      <c r="X97" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="94">
-      <c r="V94" t="s">
+    <row r="98">
+      <c r="X98" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="95">
-      <c r="V95" t="s">
+    <row r="99">
+      <c r="X99" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="96">
-      <c r="V96" t="s">
+    <row r="100">
+      <c r="X100" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="X101" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="97">
-      <c r="V97" t="s">
+    <row r="102">
+      <c r="X102" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="98">
-      <c r="V98" t="s">
+    <row r="103">
+      <c r="X103" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="99">
-      <c r="V99" t="s">
+    <row r="104">
+      <c r="X104" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="100">
-      <c r="V100" t="s">
+    <row r="105">
+      <c r="X105" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="101">
-      <c r="V101" t="s">
+    <row r="106">
+      <c r="X106" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="102">
-      <c r="V102" t="s">
+    <row r="107">
+      <c r="X107" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="103">
-      <c r="V103" t="s">
+    <row r="108">
+      <c r="X108" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="104">
-      <c r="V104" t="s">
+    <row r="109">
+      <c r="X109" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="105">
-      <c r="V105" t="s">
+    <row r="110">
+      <c r="X110" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="106">
-      <c r="V106" t="s">
+    <row r="111">
+      <c r="X111" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="107">
-      <c r="V107" t="s">
+    <row r="112">
+      <c r="X112" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="108">
-      <c r="V108" t="s">
+    <row r="113">
+      <c r="X113" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="109">
-      <c r="V109" t="s">
+    <row r="114">
+      <c r="X114" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="110">
-      <c r="V110" t="s">
+    <row r="115">
+      <c r="X115" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="111">
-      <c r="V111" t="s">
+    <row r="116">
+      <c r="X116" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="112">
-      <c r="V112" t="s">
+    <row r="117">
+      <c r="X117" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="113">
-      <c r="V113" t="s">
+    <row r="118">
+      <c r="X118" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="114">
-      <c r="V114" t="s">
+    <row r="119">
+      <c r="X119" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="115">
-      <c r="V115" t="s">
+    <row r="120">
+      <c r="X120" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="116">
-      <c r="V116" t="s">
+    <row r="121">
+      <c r="X121" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="117">
-      <c r="V117" t="s">
+    <row r="122">
+      <c r="X122" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="118">
-      <c r="V118" t="s">
+    <row r="123">
+      <c r="X123" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="119">
-      <c r="V119" t="s">
+    <row r="124">
+      <c r="X124" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="120">
-      <c r="V120" t="s">
+    <row r="125">
+      <c r="X125" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
### [xml] - [`assertSoap(wsdl,xml)`]: *NEW* command to validate SOAP `xml` against the schema defined in `wsdl` - [`assertSoapFaultCode(expected,xml)`]: *NEW* command to assert the "fault code" in SOAP fault `xml. - [`assertSoapFaultString(expected,xml)`]: *NEW* command to assert the "fault text" in SOAP fault `xml. - [`storeSoapFaultCode(var,xml)`]: *NEW* command to extract and store "fault code" in SOAP fault `xml`. - [`storeSoapFaultString(var,xml)`]: *NEW* command to extract and store "fault text" in SOAP fault `xml`. - [`assertCorrectness(xml,schema)`]: enhance command to support automatic conformance retries over multiple schemas.
### fixed
- enforce no text-wrap on param values of a Nexial output

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -46,7 +46,7 @@
     <definedName name="webcookie">'#system'!$AA$2:$AA$8</definedName>
     <definedName name="ws">'#system'!$AB$2:$AB$17</definedName>
     <definedName name="ws.async">'#system'!$AC$2:$AC$8</definedName>
-    <definedName name="xml">'#system'!$AD$2:$AD$21</definedName>
+    <definedName name="xml">'#system'!$AD$2:$AD$27</definedName>
   </definedNames>
   <calcPr calcId="150000"/>
   <extLst>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7534" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10228" uniqueCount="526">
   <si>
     <t>description</t>
   </si>
@@ -1615,6 +1615,30 @@
   </si>
   <si>
     <t>typeKeys(os,keystrokes)</t>
+  </si>
+  <si>
+    <t>assertSoapConformance(var,wsdl,xml)</t>
+  </si>
+  <si>
+    <t>assertSoapXml(wsdl,xml)</t>
+  </si>
+  <si>
+    <t>assertSoap(wsdl,xml)</t>
+  </si>
+  <si>
+    <t>assertSoapFaultCode(expected,xml)</t>
+  </si>
+  <si>
+    <t>assertSoapFaultString(expected,xml)</t>
+  </si>
+  <si>
+    <t>storeSoapFaultCode(var,xml)</t>
+  </si>
+  <si>
+    <t>storeSoapFaultDetail(var,xml)</t>
+  </si>
+  <si>
+    <t>storeSoapFaultString(var,xml)</t>
   </si>
 </sst>
 </file>
@@ -1622,7 +1646,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="216" x14ac:knownFonts="1">
+  <fonts count="296" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2989,8 +3013,513 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="393">
+  <fills count="528">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5213,8 +5742,773 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="366">
+  <borders count="526">
     <border>
       <left/>
       <right/>
@@ -8725,6 +10019,1636 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -8909,7 +11833,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="229">
+  <cellXfs count="309">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -9555,52 +12479,292 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="362" fontId="199" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="200" fillId="365" borderId="345" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="201" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="345" fillId="365" fontId="200" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="201" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="202" fillId="368" borderId="349" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="349" fillId="368" fontId="202" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="203" fillId="371" borderId="353" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="353" fillId="371" fontId="203" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="204" fillId="374" borderId="353" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="353" fillId="374" fontId="204" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="205" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="205" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="206" fillId="377" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="377" fontId="206" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="207" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="208" fillId="380" borderId="357" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="209" fillId="383" borderId="361" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="210" fillId="386" borderId="365" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="211" fillId="386" borderId="365" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="212" fillId="374" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="213" fillId="389" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="214" fillId="374" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="215" fillId="392" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="207" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="357" fillId="380" fontId="208" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="361" fillId="383" fontId="209" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="365" fillId="386" fontId="210" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="365" fillId="386" fontId="211" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="374" fontId="212" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="389" fontId="213" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="374" fontId="214" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="392" fontId="215" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="373" fillId="395" fontId="216" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="217" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="377" fillId="398" fontId="218" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="381" fillId="401" fontId="219" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="385" fillId="404" fontId="220" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="221" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="407" fontId="222" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="223" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="389" fillId="410" fontId="224" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="393" fillId="401" fontId="225" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="397" fillId="413" fontId="226" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="397" fillId="413" fontId="227" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="404" fontId="228" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="416" fontId="229" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="404" fontId="230" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="419" fontId="231" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="405" fillId="422" fontId="232" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="233" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="409" fillId="425" fontId="234" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="413" fillId="428" fontId="235" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="417" fillId="431" fontId="236" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="237" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="434" fontId="238" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="239" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="421" fillId="437" fontId="240" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="425" fillId="428" fontId="241" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="429" fillId="440" fontId="242" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="429" fillId="440" fontId="243" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="431" fontId="244" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="443" fontId="245" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="431" fontId="246" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="446" fontId="247" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="437" fillId="449" fontId="248" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="249" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="441" fillId="452" fontId="250" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="445" fillId="455" fontId="251" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="449" fillId="458" fontId="252" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="253" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="461" fontId="254" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="255" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="453" fillId="464" fontId="256" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="457" fillId="455" fontId="257" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="461" fillId="467" fontId="258" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="461" fillId="467" fontId="259" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="458" fontId="260" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="470" fontId="261" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="458" fontId="262" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="473" fontId="263" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="469" fillId="476" fontId="264" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="265" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="473" fillId="479" fontId="266" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="477" fillId="482" fontId="267" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="481" fillId="485" fontId="268" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="269" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="488" fontId="270" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="271" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="485" fillId="491" fontId="272" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="489" fillId="482" fontId="273" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="493" fillId="494" fontId="274" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="493" fillId="494" fontId="275" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="485" fontId="276" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="497" fontId="277" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="485" fontId="278" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="500" fontId="279" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="280" fillId="503" borderId="501" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="281" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="282" fillId="506" borderId="505" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="283" fillId="509" borderId="509" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="284" fillId="512" borderId="513" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="285" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="286" fillId="515" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="287" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="288" fillId="518" borderId="517" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="289" fillId="509" borderId="521" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="290" fillId="521" borderId="525" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="291" fillId="521" borderId="525" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="292" fillId="512" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="293" fillId="524" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="294" fillId="512" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="295" fillId="527" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -10458,7 +13622,7 @@
         <v>414</v>
       </c>
       <c r="AD7" t="s">
-        <v>220</v>
+        <v>520</v>
       </c>
     </row>
     <row r="8">
@@ -10514,7 +13678,7 @@
         <v>415</v>
       </c>
       <c r="AD8" t="s">
-        <v>221</v>
+        <v>521</v>
       </c>
     </row>
     <row r="9">
@@ -10561,7 +13725,7 @@
         <v>178</v>
       </c>
       <c r="AD9" t="s">
-        <v>222</v>
+        <v>522</v>
       </c>
     </row>
     <row r="10">
@@ -10602,7 +13766,7 @@
         <v>179</v>
       </c>
       <c r="AD10" t="s">
-        <v>462</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11">
@@ -10640,7 +13804,7 @@
         <v>249</v>
       </c>
       <c r="AD11" t="s">
-        <v>487</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12">
@@ -10678,7 +13842,7 @@
         <v>180</v>
       </c>
       <c r="AD12" t="s">
-        <v>488</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13">
@@ -10713,7 +13877,7 @@
         <v>181</v>
       </c>
       <c r="AD13" t="s">
-        <v>489</v>
+        <v>462</v>
       </c>
     </row>
     <row r="14">
@@ -10748,7 +13912,7 @@
         <v>182</v>
       </c>
       <c r="AD14" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="15">
@@ -10780,7 +13944,7 @@
         <v>183</v>
       </c>
       <c r="AD15" t="s">
-        <v>463</v>
+        <v>488</v>
       </c>
     </row>
     <row r="16">
@@ -10812,7 +13976,7 @@
         <v>184</v>
       </c>
       <c r="AD16" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="17">
@@ -10835,7 +13999,7 @@
         <v>454</v>
       </c>
       <c r="AD17" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="18">
@@ -10855,7 +14019,7 @@
         <v>95</v>
       </c>
       <c r="AD18" t="s">
-        <v>493</v>
+        <v>463</v>
       </c>
     </row>
     <row r="19">
@@ -10875,7 +14039,7 @@
         <v>96</v>
       </c>
       <c r="AD19" t="s">
-        <v>223</v>
+        <v>491</v>
       </c>
     </row>
     <row r="20">
@@ -10895,7 +14059,7 @@
         <v>97</v>
       </c>
       <c r="AD20" t="s">
-        <v>224</v>
+        <v>492</v>
       </c>
     </row>
     <row r="21">
@@ -10915,7 +14079,7 @@
         <v>98</v>
       </c>
       <c r="AD21" t="s">
-        <v>225</v>
+        <v>493</v>
       </c>
     </row>
     <row r="22">
@@ -10934,6 +14098,9 @@
       <c r="Y22" t="s">
         <v>481</v>
       </c>
+      <c r="AD22" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -10951,6 +14118,9 @@
       <c r="Y23" t="s">
         <v>99</v>
       </c>
+      <c r="AD23" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
@@ -10968,6 +14138,9 @@
       <c r="Y24" t="s">
         <v>100</v>
       </c>
+      <c r="AD24" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
@@ -10985,6 +14158,9 @@
       <c r="Y25" t="s">
         <v>101</v>
       </c>
+      <c r="AD25" t="s">
+        <v>525</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
@@ -11002,6 +14178,9 @@
       <c r="Y26" t="s">
         <v>102</v>
       </c>
+      <c r="AD26" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
@@ -11018,6 +14197,9 @@
       </c>
       <c r="Y27" t="s">
         <v>103</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="28">

</xml_diff>

<commit_message>
[xml] - [`assertSoap(wsdl,xml)`]: fix to handle multiple and possibly conflicting namespace(s) within one XSD embedded in a WSDL. Also some code optimization.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -22,7 +22,7 @@
     <definedName name="desktop">'#system'!$G$2:$G$95</definedName>
     <definedName name="excel">'#system'!$H$2:$H$14</definedName>
     <definedName name="external">'#system'!$I$2:$I$5</definedName>
-    <definedName name="image">'#system'!$J$2:$J$6</definedName>
+    <definedName name="image">'#system'!$J$2:$J$7</definedName>
     <definedName name="io">'#system'!$K$2:$K$29</definedName>
     <definedName name="jms">'#system'!$L$2:$L$4</definedName>
     <definedName name="json">'#system'!$M$2:$M$16</definedName>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10228" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10772" uniqueCount="527">
   <si>
     <t>description</t>
   </si>
@@ -1639,6 +1639,9 @@
   </si>
   <si>
     <t>storeSoapFaultString(var,xml)</t>
+  </si>
+  <si>
+    <t>saveDiff(var,baseline,actual)</t>
   </si>
 </sst>
 </file>
@@ -1646,7 +1649,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="296" x14ac:knownFonts="1">
+  <fonts count="312" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3518,8 +3521,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="528">
+  <fills count="555">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6507,8 +6611,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="526">
+  <borders count="558">
     <border>
       <left/>
       <right/>
@@ -10019,6 +10276,332 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -11833,7 +12416,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="309">
+  <cellXfs count="325">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -12719,52 +13302,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="500" fontId="279" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="280" fillId="503" borderId="501" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="281" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="501" fillId="503" fontId="280" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="281" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="282" fillId="506" borderId="505" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="505" fillId="506" fontId="282" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="283" fillId="509" borderId="509" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="509" fillId="509" fontId="283" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="284" fillId="512" borderId="513" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="513" fillId="512" fontId="284" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="285" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="285" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="286" fillId="515" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="515" fontId="286" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="287" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="288" fillId="518" borderId="517" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="289" fillId="509" borderId="521" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="290" fillId="521" borderId="525" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="291" fillId="521" borderId="525" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="292" fillId="512" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="293" fillId="524" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="294" fillId="512" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="295" fillId="527" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="287" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="517" fillId="518" fontId="288" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="521" fillId="509" fontId="289" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="525" fillId="521" fontId="290" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="525" fillId="521" fontId="291" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="512" fontId="292" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="524" fontId="293" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="512" fontId="294" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="527" fontId="295" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="296" fillId="530" borderId="533" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="297" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="298" fillId="533" borderId="537" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="299" fillId="536" borderId="541" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="300" fillId="539" borderId="545" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="301" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="302" fillId="542" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="303" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="304" fillId="545" borderId="549" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="305" fillId="536" borderId="553" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="306" fillId="548" borderId="557" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="307" fillId="548" borderId="557" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="308" fillId="539" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="309" fillId="551" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="310" fillId="539" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="311" fillId="554" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -13582,6 +14213,9 @@
       <c r="H7" t="s">
         <v>434</v>
       </c>
+      <c r="J7" t="s">
+        <v>526</v>
+      </c>
       <c r="K7" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
- minor console output enhancement to highlight (in blue) any execution abort messages and reasons.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10772" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12404" uniqueCount="527">
   <si>
     <t>description</t>
   </si>
@@ -1649,7 +1649,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="312" x14ac:knownFonts="1">
+  <fonts count="360" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3622,8 +3622,311 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="555">
+  <fills count="636">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6764,8 +7067,467 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="558">
+  <borders count="654">
     <border>
       <left/>
       <right/>
@@ -10276,6 +11038,984 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -12416,7 +14156,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="325">
+  <cellXfs count="373">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -13350,52 +15090,196 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="527" fontId="295" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="296" fillId="530" borderId="533" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="297" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="533" fillId="530" fontId="296" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="297" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="298" fillId="533" borderId="537" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="537" fillId="533" fontId="298" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="299" fillId="536" borderId="541" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="541" fillId="536" fontId="299" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="300" fillId="539" borderId="545" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="545" fillId="539" fontId="300" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="301" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="301" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="302" fillId="542" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="542" fontId="302" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="303" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="304" fillId="545" borderId="549" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="305" fillId="536" borderId="553" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="306" fillId="548" borderId="557" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="307" fillId="548" borderId="557" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="308" fillId="539" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="309" fillId="551" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="310" fillId="539" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="311" fillId="554" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="303" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="549" fillId="545" fontId="304" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="553" fillId="536" fontId="305" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="557" fillId="548" fontId="306" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="557" fillId="548" fontId="307" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="539" fontId="308" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="551" fontId="309" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="539" fontId="310" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="554" fontId="311" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="565" fillId="557" fontId="312" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="313" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="569" fillId="560" fontId="314" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="573" fillId="563" fontId="315" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="577" fillId="566" fontId="316" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="317" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="569" fontId="318" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="319" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="581" fillId="572" fontId="320" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="585" fillId="563" fontId="321" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="589" fillId="575" fontId="322" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="589" fillId="575" fontId="323" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="566" fontId="324" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="578" fontId="325" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="566" fontId="326" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="581" fontId="327" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="597" fillId="584" fontId="328" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="329" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="601" fillId="587" fontId="330" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="605" fillId="590" fontId="331" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="609" fillId="593" fontId="332" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="333" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="596" fontId="334" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="335" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="613" fillId="599" fontId="336" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="617" fillId="590" fontId="337" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="621" fillId="602" fontId="338" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="621" fillId="602" fontId="339" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="593" fontId="340" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="605" fontId="341" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="593" fontId="342" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="608" fontId="343" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="344" fillId="611" borderId="629" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="345" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="346" fillId="614" borderId="633" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="347" fillId="617" borderId="637" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="348" fillId="620" borderId="641" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="349" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="350" fillId="623" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="351" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="352" fillId="626" borderId="645" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="353" fillId="617" borderId="649" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="354" fillId="629" borderId="653" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="355" fillId="629" borderId="653" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="356" fillId="620" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="357" fillId="632" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="358" fillId="620" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="359" fillId="635" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[flow control] - [`EndLoopIf()`]: fix code to break repeat-until loop without breaking the enclosing iteration, and vice-versa.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20564" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24372" uniqueCount="527">
   <si>
     <t>description</t>
   </si>
@@ -1649,7 +1649,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="600" x14ac:knownFonts="1">
+  <fonts count="712" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5440,8 +5440,715 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1041">
+  <fills count="1230">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -11336,8 +12043,1079 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1134">
+  <borders count="1358">
     <border>
       <left/>
       <right/>
@@ -14848,6 +16626,2288 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -22856,7 +26916,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="613">
+  <cellXfs count="725">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -24654,52 +28714,388 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1013" fontId="583" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="584" fillId="1016" borderId="1109" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="585" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1109" fillId="1016" fontId="584" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="585" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="586" fillId="1019" borderId="1113" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1113" fillId="1019" fontId="586" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="587" fillId="1022" borderId="1117" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1117" fillId="1022" fontId="587" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="588" fillId="1025" borderId="1121" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1121" fillId="1025" fontId="588" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="589" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="589" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="590" fillId="1028" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1028" fontId="590" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="591" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="592" fillId="1031" borderId="1125" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="593" fillId="1022" borderId="1129" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="594" fillId="1034" borderId="1133" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="595" fillId="1034" borderId="1133" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="596" fillId="1025" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="597" fillId="1037" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="598" fillId="1025" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="599" fillId="1040" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="591" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1125" fillId="1031" fontId="592" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1129" fillId="1022" fontId="593" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1133" fillId="1034" fontId="594" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1133" fillId="1034" fontId="595" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1025" fontId="596" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1037" fontId="597" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1025" fontId="598" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1040" fontId="599" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1141" fillId="1043" fontId="600" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="601" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1145" fillId="1046" fontId="602" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1149" fillId="1049" fontId="603" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1153" fillId="1052" fontId="604" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="605" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1055" fontId="606" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="607" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1157" fillId="1058" fontId="608" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1161" fillId="1049" fontId="609" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1165" fillId="1061" fontId="610" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1165" fillId="1061" fontId="611" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1052" fontId="612" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1064" fontId="613" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1052" fontId="614" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1067" fontId="615" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1173" fillId="1070" fontId="616" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="617" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1177" fillId="1073" fontId="618" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1181" fillId="1076" fontId="619" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1185" fillId="1079" fontId="620" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="621" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1082" fontId="622" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="623" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1189" fillId="1085" fontId="624" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1193" fillId="1076" fontId="625" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1197" fillId="1088" fontId="626" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1197" fillId="1088" fontId="627" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1079" fontId="628" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1091" fontId="629" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1079" fontId="630" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1094" fontId="631" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1205" fillId="1097" fontId="632" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="633" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1209" fillId="1100" fontId="634" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1213" fillId="1103" fontId="635" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1217" fillId="1106" fontId="636" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="637" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1109" fontId="638" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="639" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1221" fillId="1112" fontId="640" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1225" fillId="1103" fontId="641" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1229" fillId="1115" fontId="642" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1229" fillId="1115" fontId="643" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1106" fontId="644" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1118" fontId="645" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1106" fontId="646" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1121" fontId="647" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1237" fillId="1124" fontId="648" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="649" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1241" fillId="1127" fontId="650" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1245" fillId="1130" fontId="651" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1249" fillId="1133" fontId="652" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="653" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1136" fontId="654" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="655" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1253" fillId="1139" fontId="656" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1257" fillId="1130" fontId="657" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1261" fillId="1142" fontId="658" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1261" fillId="1142" fontId="659" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1133" fontId="660" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1145" fontId="661" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1133" fontId="662" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1148" fontId="663" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1269" fillId="1151" fontId="664" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="665" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1273" fillId="1154" fontId="666" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1277" fillId="1157" fontId="667" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1281" fillId="1160" fontId="668" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="669" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1163" fontId="670" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="671" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1285" fillId="1166" fontId="672" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1289" fillId="1157" fontId="673" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1293" fillId="1169" fontId="674" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1293" fillId="1169" fontId="675" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1160" fontId="676" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1172" fontId="677" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1160" fontId="678" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1175" fontId="679" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1301" fillId="1178" fontId="680" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="681" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1305" fillId="1181" fontId="682" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1309" fillId="1184" fontId="683" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1313" fillId="1187" fontId="684" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="685" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1190" fontId="686" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="687" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1317" fillId="1193" fontId="688" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1321" fillId="1184" fontId="689" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1325" fillId="1196" fontId="690" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1325" fillId="1196" fontId="691" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1187" fontId="692" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1199" fontId="693" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1187" fontId="694" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1202" fontId="695" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="696" fillId="1205" borderId="1333" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="697" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="698" fillId="1208" borderId="1337" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="699" fillId="1211" borderId="1341" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="700" fillId="1214" borderId="1345" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="701" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="702" fillId="1217" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="703" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="704" fillId="1220" borderId="1349" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="705" fillId="1211" borderId="1353" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="706" fillId="1223" borderId="1357" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="707" fillId="1223" borderId="1357" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="708" fillId="1214" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="709" fillId="1226" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="710" fillId="1214" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="711" fillId="1229" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[web] - [`clickAll(locator)`]: **NEW** command to click on all web elements matching `locator`. This is useful to support the more modern web applications that use `<DIV>` elements to disguise as dropdown options.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -41,7 +41,7 @@
     <definedName name="ssh">'#system'!$W$2:$W$9</definedName>
     <definedName name="step">'#system'!$X$2:$X$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$30</definedName>
-    <definedName name="web">'#system'!$Y$2:$Y$128</definedName>
+    <definedName name="web">'#system'!$Y$2:$Y$129</definedName>
     <definedName name="webalert">'#system'!$Z$2:$Z$8</definedName>
     <definedName name="webcookie">'#system'!$AA$2:$AA$8</definedName>
     <definedName name="ws">'#system'!$AB$2:$AB$17</definedName>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24372" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26549" uniqueCount="528">
   <si>
     <t>description</t>
   </si>
@@ -1642,6 +1642,9 @@
   </si>
   <si>
     <t>saveDiff(var,baseline,actual)</t>
+  </si>
+  <si>
+    <t>clickAll(locator)</t>
   </si>
 </sst>
 </file>
@@ -1649,7 +1652,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="712" x14ac:knownFonts="1">
+  <fonts count="776" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6147,8 +6150,412 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1230">
+  <fills count="1338">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -13114,8 +13521,620 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1358">
+  <borders count="1486">
     <border>
       <left/>
       <right/>
@@ -16626,6 +17645,1310 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -26916,7 +29239,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="725">
+  <cellXfs count="789">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -29050,52 +31373,244 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1202" fontId="695" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="696" fillId="1205" borderId="1333" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="697" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1333" fillId="1205" fontId="696" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="697" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="698" fillId="1208" borderId="1337" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1337" fillId="1208" fontId="698" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="699" fillId="1211" borderId="1341" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1341" fillId="1211" fontId="699" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="700" fillId="1214" borderId="1345" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1345" fillId="1214" fontId="700" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="701" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="701" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="702" fillId="1217" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1217" fontId="702" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="703" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="704" fillId="1220" borderId="1349" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="705" fillId="1211" borderId="1353" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="706" fillId="1223" borderId="1357" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="707" fillId="1223" borderId="1357" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="708" fillId="1214" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="709" fillId="1226" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="710" fillId="1214" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="711" fillId="1229" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="703" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1349" fillId="1220" fontId="704" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1353" fillId="1211" fontId="705" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1357" fillId="1223" fontId="706" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1357" fillId="1223" fontId="707" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1214" fontId="708" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1226" fontId="709" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1214" fontId="710" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1229" fontId="711" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1365" fillId="1232" fontId="712" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="713" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1369" fillId="1235" fontId="714" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1373" fillId="1238" fontId="715" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1377" fillId="1241" fontId="716" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="717" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1244" fontId="718" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="719" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1381" fillId="1247" fontId="720" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1385" fillId="1238" fontId="721" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1389" fillId="1250" fontId="722" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1389" fillId="1250" fontId="723" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1241" fontId="724" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1253" fontId="725" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1241" fontId="726" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1256" fontId="727" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1397" fillId="1259" fontId="728" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="729" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1401" fillId="1262" fontId="730" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1405" fillId="1265" fontId="731" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1409" fillId="1268" fontId="732" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="733" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1271" fontId="734" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="735" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1413" fillId="1274" fontId="736" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1417" fillId="1265" fontId="737" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1421" fillId="1277" fontId="738" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1421" fillId="1277" fontId="739" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1268" fontId="740" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1280" fontId="741" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1268" fontId="742" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1283" fontId="743" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1429" fillId="1286" fontId="744" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="745" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1433" fillId="1289" fontId="746" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1437" fillId="1292" fontId="747" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1441" fillId="1295" fontId="748" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="749" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1298" fontId="750" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="751" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1445" fillId="1301" fontId="752" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1449" fillId="1292" fontId="753" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1453" fillId="1304" fontId="754" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1453" fillId="1304" fontId="755" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1295" fontId="756" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1307" fontId="757" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1295" fontId="758" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1310" fontId="759" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="760" fillId="1313" borderId="1461" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="761" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="762" fillId="1316" borderId="1465" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="763" fillId="1319" borderId="1469" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="764" fillId="1322" borderId="1473" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="765" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="766" fillId="1325" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="767" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="768" fillId="1328" borderId="1477" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="769" fillId="1319" borderId="1481" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="770" fillId="1331" borderId="1485" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="771" fillId="1331" borderId="1485" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="772" fillId="1322" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="773" fillId="1334" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="774" fillId="1322" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="775" fillId="1337" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -29393,7 +31908,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE128"/>
+  <dimension ref="A1:AE129"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -30762,7 +33277,7 @@
         <v>357</v>
       </c>
       <c r="Y50" t="s">
-        <v>117</v>
+        <v>527</v>
       </c>
     </row>
     <row r="51">
@@ -30770,7 +33285,7 @@
         <v>292</v>
       </c>
       <c r="Y51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52">
@@ -30778,7 +33293,7 @@
         <v>345</v>
       </c>
       <c r="Y52" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53">
@@ -30786,7 +33301,7 @@
         <v>321</v>
       </c>
       <c r="Y53" t="s">
-        <v>482</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54">
@@ -30794,7 +33309,7 @@
         <v>258</v>
       </c>
       <c r="Y54" t="s">
-        <v>451</v>
+        <v>482</v>
       </c>
     </row>
     <row r="55">
@@ -30802,7 +33317,7 @@
         <v>282</v>
       </c>
       <c r="Y55" t="s">
-        <v>120</v>
+        <v>451</v>
       </c>
     </row>
     <row r="56">
@@ -30810,7 +33325,7 @@
         <v>283</v>
       </c>
       <c r="Y56" t="s">
-        <v>336</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57">
@@ -30818,7 +33333,7 @@
         <v>284</v>
       </c>
       <c r="Y57" t="s">
-        <v>452</v>
+        <v>336</v>
       </c>
     </row>
     <row r="58">
@@ -30826,7 +33341,7 @@
         <v>293</v>
       </c>
       <c r="Y58" t="s">
-        <v>121</v>
+        <v>452</v>
       </c>
     </row>
     <row r="59">
@@ -30834,7 +33349,7 @@
         <v>302</v>
       </c>
       <c r="Y59" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60">
@@ -30842,7 +33357,7 @@
         <v>327</v>
       </c>
       <c r="Y60" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="61">
@@ -30850,7 +33365,7 @@
         <v>299</v>
       </c>
       <c r="Y61" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="62">
@@ -30858,7 +33373,7 @@
         <v>300</v>
       </c>
       <c r="Y62" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63">
@@ -30866,7 +33381,7 @@
         <v>358</v>
       </c>
       <c r="Y63" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="64">
@@ -30874,7 +33389,7 @@
         <v>359</v>
       </c>
       <c r="Y64" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="65">
@@ -30882,7 +33397,7 @@
         <v>335</v>
       </c>
       <c r="Y65" t="s">
-        <v>427</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66">
@@ -30890,7 +33405,7 @@
         <v>303</v>
       </c>
       <c r="Y66" t="s">
-        <v>461</v>
+        <v>427</v>
       </c>
     </row>
     <row r="67">
@@ -30898,7 +33413,7 @@
         <v>259</v>
       </c>
       <c r="Y67" t="s">
-        <v>203</v>
+        <v>461</v>
       </c>
     </row>
     <row r="68">
@@ -30906,7 +33421,7 @@
         <v>512</v>
       </c>
       <c r="Y68" t="s">
-        <v>378</v>
+        <v>203</v>
       </c>
     </row>
     <row r="69">
@@ -30914,7 +33429,7 @@
         <v>304</v>
       </c>
       <c r="Y69" t="s">
-        <v>428</v>
+        <v>378</v>
       </c>
     </row>
     <row r="70">
@@ -30922,7 +33437,7 @@
         <v>397</v>
       </c>
       <c r="Y70" t="s">
-        <v>128</v>
+        <v>428</v>
       </c>
     </row>
     <row r="71">
@@ -30930,7 +33445,7 @@
         <v>294</v>
       </c>
       <c r="Y71" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="72">
@@ -30938,7 +33453,7 @@
         <v>398</v>
       </c>
       <c r="Y72" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="73">
@@ -30946,7 +33461,7 @@
         <v>252</v>
       </c>
       <c r="Y73" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74">
@@ -30954,7 +33469,7 @@
         <v>497</v>
       </c>
       <c r="Y74" t="s">
-        <v>186</v>
+        <v>131</v>
       </c>
     </row>
     <row r="75">
@@ -30962,7 +33477,7 @@
         <v>334</v>
       </c>
       <c r="Y75" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="76">
@@ -30970,7 +33485,7 @@
         <v>270</v>
       </c>
       <c r="Y76" t="s">
-        <v>440</v>
+        <v>187</v>
       </c>
     </row>
     <row r="77">
@@ -30978,7 +33493,7 @@
         <v>276</v>
       </c>
       <c r="Y77" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
     </row>
     <row r="78">
@@ -30986,7 +33501,7 @@
         <v>281</v>
       </c>
       <c r="Y78" t="s">
-        <v>132</v>
+        <v>453</v>
       </c>
     </row>
     <row r="79">
@@ -30994,7 +33509,7 @@
         <v>416</v>
       </c>
       <c r="Y79" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="80">
@@ -31002,7 +33517,7 @@
         <v>322</v>
       </c>
       <c r="Y80" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="81">
@@ -31010,7 +33525,7 @@
         <v>260</v>
       </c>
       <c r="Y81" t="s">
-        <v>483</v>
+        <v>134</v>
       </c>
     </row>
     <row r="82">
@@ -31018,7 +33533,7 @@
         <v>271</v>
       </c>
       <c r="Y82" t="s">
-        <v>135</v>
+        <v>483</v>
       </c>
     </row>
     <row r="83">
@@ -31026,7 +33541,7 @@
         <v>277</v>
       </c>
       <c r="Y83" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="84">
@@ -31034,7 +33549,7 @@
         <v>266</v>
       </c>
       <c r="Y84" t="s">
-        <v>188</v>
+        <v>136</v>
       </c>
     </row>
     <row r="85">
@@ -31042,7 +33557,7 @@
         <v>517</v>
       </c>
       <c r="Y85" t="s">
-        <v>484</v>
+        <v>188</v>
       </c>
     </row>
     <row r="86">
@@ -31050,7 +33565,7 @@
         <v>261</v>
       </c>
       <c r="Y86" t="s">
-        <v>189</v>
+        <v>484</v>
       </c>
     </row>
     <row r="87">
@@ -31058,7 +33573,7 @@
         <v>278</v>
       </c>
       <c r="Y87" t="s">
-        <v>441</v>
+        <v>189</v>
       </c>
     </row>
     <row r="88">
@@ -31066,7 +33581,7 @@
         <v>262</v>
       </c>
       <c r="Y88" t="s">
-        <v>190</v>
+        <v>441</v>
       </c>
     </row>
     <row r="89">
@@ -31074,7 +33589,7 @@
         <v>263</v>
       </c>
       <c r="Y89" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="90">
@@ -31082,7 +33597,7 @@
         <v>295</v>
       </c>
       <c r="Y90" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
     </row>
     <row r="91">
@@ -31090,7 +33605,7 @@
         <v>301</v>
       </c>
       <c r="Y91" t="s">
-        <v>137</v>
+        <v>204</v>
       </c>
     </row>
     <row r="92">
@@ -31098,7 +33613,7 @@
         <v>285</v>
       </c>
       <c r="Y92" t="s">
-        <v>192</v>
+        <v>137</v>
       </c>
     </row>
     <row r="93">
@@ -31106,7 +33621,7 @@
         <v>330</v>
       </c>
       <c r="Y93" t="s">
-        <v>429</v>
+        <v>192</v>
       </c>
     </row>
     <row r="94">
@@ -31114,7 +33629,7 @@
         <v>267</v>
       </c>
       <c r="Y94" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="95">
@@ -31122,171 +33637,176 @@
         <v>268</v>
       </c>
       <c r="Y95" t="s">
-        <v>193</v>
+        <v>430</v>
       </c>
     </row>
     <row r="96">
       <c r="Y96" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="97">
       <c r="Y97" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="98">
       <c r="Y98" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="99">
       <c r="Y99" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="100">
       <c r="Y100" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
     </row>
     <row r="101">
       <c r="Y101" t="s">
-        <v>485</v>
+        <v>197</v>
       </c>
     </row>
     <row r="102">
       <c r="Y102" t="s">
-        <v>509</v>
+        <v>485</v>
       </c>
     </row>
     <row r="103">
       <c r="Y103" t="s">
-        <v>138</v>
+        <v>509</v>
       </c>
     </row>
     <row r="104">
       <c r="Y104" t="s">
-        <v>510</v>
+        <v>138</v>
       </c>
     </row>
     <row r="105">
       <c r="Y105" t="s">
-        <v>372</v>
+        <v>510</v>
       </c>
     </row>
     <row r="106">
       <c r="Y106" t="s">
-        <v>139</v>
+        <v>372</v>
       </c>
     </row>
     <row r="107">
       <c r="Y107" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="108">
       <c r="Y108" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="109">
       <c r="Y109" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="110">
       <c r="Y110" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="111">
       <c r="Y111" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="112">
       <c r="Y112" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="113">
       <c r="Y113" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="114">
       <c r="Y114" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="115">
       <c r="Y115" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="116">
       <c r="Y116" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="117">
       <c r="Y117" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="118">
       <c r="Y118" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="119">
       <c r="Y119" t="s">
-        <v>431</v>
+        <v>151</v>
       </c>
     </row>
     <row r="120">
       <c r="Y120" t="s">
-        <v>152</v>
+        <v>431</v>
       </c>
     </row>
     <row r="121">
       <c r="Y121" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="122">
       <c r="Y122" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="123">
       <c r="Y123" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="124">
       <c r="Y124" t="s">
-        <v>39</v>
+        <v>155</v>
       </c>
     </row>
     <row r="125">
       <c r="Y125" t="s">
-        <v>156</v>
+        <v>39</v>
       </c>
     </row>
     <row r="126">
       <c r="Y126" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="127">
       <c r="Y127" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="128">
       <c r="Y128" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="Y129" t="s">
         <v>159</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[json] - [`compact`]: **NEW** command to compact JSON by removing null, empty text and empty nodes.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -25,7 +25,7 @@
     <definedName name="image">'#system'!$J$2:$J$7</definedName>
     <definedName name="io">'#system'!$K$2:$K$29</definedName>
     <definedName name="jms">'#system'!$L$2:$L$4</definedName>
-    <definedName name="json">'#system'!$M$2:$M$16</definedName>
+    <definedName name="json">'#system'!$M$2:$M$17</definedName>
     <definedName name="localdb">'#system'!$N$2:$N$12</definedName>
     <definedName name="macro">'#system'!$O$2:$O$4</definedName>
     <definedName name="mail">'#system'!$P$2:$P$2</definedName>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26549" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27640" uniqueCount="529">
   <si>
     <t>description</t>
   </si>
@@ -1645,6 +1645,9 @@
   </si>
   <si>
     <t>clickAll(locator)</t>
+  </si>
+  <si>
+    <t>compact(var,json,removeEmpty)</t>
   </si>
 </sst>
 </file>
@@ -1652,7 +1655,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="776" x14ac:knownFonts="1">
+  <fonts count="808" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6554,8 +6557,210 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1338">
+  <fills count="1392">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -14133,8 +14338,314 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1486">
+  <borders count="1550">
     <border>
       <left/>
       <right/>
@@ -17645,6 +18156,658 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -29239,7 +30402,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="789">
+  <cellXfs count="821">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -31565,52 +32728,148 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1310" fontId="759" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="760" fillId="1313" borderId="1461" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="761" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1461" fillId="1313" fontId="760" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="761" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="762" fillId="1316" borderId="1465" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1465" fillId="1316" fontId="762" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="763" fillId="1319" borderId="1469" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1469" fillId="1319" fontId="763" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="764" fillId="1322" borderId="1473" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1473" fillId="1322" fontId="764" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="765" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="765" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="766" fillId="1325" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1325" fontId="766" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="767" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="768" fillId="1328" borderId="1477" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="769" fillId="1319" borderId="1481" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="770" fillId="1331" borderId="1485" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="771" fillId="1331" borderId="1485" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="772" fillId="1322" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="773" fillId="1334" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="774" fillId="1322" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="775" fillId="1337" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="767" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1477" fillId="1328" fontId="768" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1481" fillId="1319" fontId="769" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1485" fillId="1331" fontId="770" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1485" fillId="1331" fontId="771" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1322" fontId="772" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1334" fontId="773" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1322" fontId="774" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1337" fontId="775" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1493" fillId="1340" fontId="776" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="777" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1497" fillId="1343" fontId="778" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1501" fillId="1346" fontId="779" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1505" fillId="1349" fontId="780" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="781" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1352" fontId="782" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="783" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1509" fillId="1355" fontId="784" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1513" fillId="1346" fontId="785" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1517" fillId="1358" fontId="786" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1517" fillId="1358" fontId="787" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1349" fontId="788" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1361" fontId="789" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1349" fontId="790" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1364" fontId="791" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="792" fillId="1367" borderId="1525" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="793" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="794" fillId="1370" borderId="1529" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="795" fillId="1373" borderId="1533" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="796" fillId="1376" borderId="1537" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="797" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="798" fillId="1379" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="799" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="800" fillId="1382" borderId="1541" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="801" fillId="1373" borderId="1545" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="802" fillId="1385" borderId="1549" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="803" fillId="1385" borderId="1549" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="804" fillId="1376" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="805" fillId="1388" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="806" fillId="1376" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="807" fillId="1391" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -32673,7 +33932,7 @@
         <v>379</v>
       </c>
       <c r="M12" t="s">
-        <v>423</v>
+        <v>528</v>
       </c>
       <c r="N12" t="s">
         <v>508</v>
@@ -32711,7 +33970,7 @@
         <v>13</v>
       </c>
       <c r="M13" t="s">
-        <v>460</v>
+        <v>423</v>
       </c>
       <c r="Q13" t="s">
         <v>85</v>
@@ -32746,7 +34005,7 @@
         <v>34</v>
       </c>
       <c r="M14" t="s">
-        <v>31</v>
+        <v>460</v>
       </c>
       <c r="Q14" t="s">
         <v>86</v>
@@ -32778,7 +34037,7 @@
         <v>474</v>
       </c>
       <c r="M15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q15" t="s">
         <v>478</v>
@@ -32810,7 +34069,7 @@
         <v>72</v>
       </c>
       <c r="M16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="Q16" t="s">
         <v>479</v>
@@ -32840,6 +34099,9 @@
       </c>
       <c r="K17" t="s">
         <v>73</v>
+      </c>
+      <c r="M17" t="s">
+        <v>35</v>
       </c>
       <c r="Y17" t="s">
         <v>480</v>

</xml_diff>

<commit_message>
[csv] - [`compareExtended(var,profile,expected,actual)`]: enhanced to support numeric conversion of quoted text (e.g. `"1.05"`).]
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28186" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29824" uniqueCount="529">
   <si>
     <t>description</t>
   </si>
@@ -1655,7 +1655,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="824" x14ac:knownFonts="1">
+  <fonts count="872" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6860,8 +6860,311 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1419">
+  <fills count="1500">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -14898,8 +15201,467 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1582">
+  <borders count="1678">
     <border>
       <left/>
       <right/>
@@ -18410,6 +19172,984 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -30982,7 +32722,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="837">
+  <cellXfs count="885">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -33452,52 +35192,196 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1391" fontId="807" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="808" fillId="1394" borderId="1557" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="809" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1557" fillId="1394" fontId="808" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="809" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="810" fillId="1397" borderId="1561" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1561" fillId="1397" fontId="810" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="811" fillId="1400" borderId="1565" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1565" fillId="1400" fontId="811" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="812" fillId="1403" borderId="1569" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1569" fillId="1403" fontId="812" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="813" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="813" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="814" fillId="1406" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1406" fontId="814" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="815" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="816" fillId="1409" borderId="1573" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="817" fillId="1400" borderId="1577" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="818" fillId="1412" borderId="1581" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="819" fillId="1412" borderId="1581" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="820" fillId="1403" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="821" fillId="1415" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="822" fillId="1403" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="823" fillId="1418" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="815" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1573" fillId="1409" fontId="816" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1577" fillId="1400" fontId="817" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1581" fillId="1412" fontId="818" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1581" fillId="1412" fontId="819" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1403" fontId="820" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1415" fontId="821" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1403" fontId="822" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1418" fontId="823" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1589" fillId="1421" fontId="824" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="825" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1593" fillId="1424" fontId="826" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1597" fillId="1427" fontId="827" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1601" fillId="1430" fontId="828" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="829" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1433" fontId="830" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="831" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1605" fillId="1436" fontId="832" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1609" fillId="1427" fontId="833" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1613" fillId="1439" fontId="834" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1613" fillId="1439" fontId="835" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1430" fontId="836" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1442" fontId="837" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1430" fontId="838" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1445" fontId="839" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1621" fillId="1448" fontId="840" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="841" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1625" fillId="1451" fontId="842" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1629" fillId="1454" fontId="843" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1633" fillId="1457" fontId="844" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="845" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1460" fontId="846" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="847" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1637" fillId="1463" fontId="848" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1641" fillId="1454" fontId="849" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1645" fillId="1466" fontId="850" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1645" fillId="1466" fontId="851" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1457" fontId="852" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1469" fontId="853" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1457" fontId="854" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1472" fontId="855" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="856" fillId="1475" borderId="1653" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="857" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="858" fillId="1478" borderId="1657" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="859" fillId="1481" borderId="1661" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="860" fillId="1484" borderId="1665" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="861" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="862" fillId="1487" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="863" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="864" fillId="1490" borderId="1669" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="865" fillId="1481" borderId="1673" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="866" fillId="1493" borderId="1677" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="867" fillId="1493" borderId="1677" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="868" fillId="1484" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="869" fillId="1496" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="870" fillId="1484" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="871" fillId="1499" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[io] - [`writeFile(file,content,append)`]: support `content` as a HTTP resource, in addition to file and direct content. - [`writeFileAsIs(file,content,append)`]: support `content` as a HTTP resource, in addition to file and direct content. - [`compare(expected,actual,failFast)`]: supports comparison report render as HTML.   - default CSS for the HTML comparison report available at https://nexiality.github.io/documentation/assets/report/io-compare-report.css - [`compare(expected,actual,failFast)`]: support `expected` and `actual` as a HTTP resource, in addition to file and direct content.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -40,13 +40,14 @@
     <definedName name="sound">'#system'!$V$2:$V$5</definedName>
     <definedName name="ssh">'#system'!$W$2:$W$9</definedName>
     <definedName name="step">'#system'!$X$2:$X$4</definedName>
-    <definedName name="target">'#system'!$A$2:$A$30</definedName>
-    <definedName name="web">'#system'!$Y$2:$Y$129</definedName>
-    <definedName name="webalert">'#system'!$Z$2:$Z$8</definedName>
-    <definedName name="webcookie">'#system'!$AA$2:$AA$8</definedName>
-    <definedName name="ws">'#system'!$AB$2:$AB$17</definedName>
-    <definedName name="ws.async">'#system'!$AC$2:$AC$8</definedName>
-    <definedName name="xml">'#system'!$AD$2:$AD$27</definedName>
+    <definedName name="target">'#system'!$A$2:$A$31</definedName>
+    <definedName name="web">'#system'!$Z$2:$Z$129</definedName>
+    <definedName name="webalert">'#system'!$AA$2:$AA$8</definedName>
+    <definedName name="webcookie">'#system'!$AB$2:$AB$8</definedName>
+    <definedName name="ws">'#system'!$AC$2:$AC$17</definedName>
+    <definedName name="ws.async">'#system'!$AD$2:$AD$8</definedName>
+    <definedName name="xml">'#system'!$AE$2:$AE$27</definedName>
+    <definedName name="text">'#system'!$Y$2:$Y$2</definedName>
   </definedNames>
   <calcPr calcId="150000"/>
   <extLst>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30370" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32017" uniqueCount="531">
   <si>
     <t>description</t>
   </si>
@@ -1648,6 +1649,12 @@
   </si>
   <si>
     <t>compact(var,json,removeEmpty)</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>spellCheck(var,profile,text)</t>
   </si>
 </sst>
 </file>
@@ -1655,7 +1662,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="888" x14ac:knownFonts="1">
+  <fonts count="936" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7264,8 +7271,311 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1527">
+  <fills count="1608">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -15914,8 +16224,467 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1710">
+  <borders count="1806">
     <border>
       <left/>
       <right/>
@@ -19426,6 +20195,984 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -33302,7 +35049,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="901">
+  <cellXfs count="949">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -35964,52 +37711,196 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1499" fontId="871" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="872" fillId="1502" borderId="1685" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="873" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1685" fillId="1502" fontId="872" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="873" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="874" fillId="1505" borderId="1689" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1689" fillId="1505" fontId="874" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="875" fillId="1508" borderId="1693" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1693" fillId="1508" fontId="875" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="876" fillId="1511" borderId="1697" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1697" fillId="1511" fontId="876" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="877" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="877" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="878" fillId="1514" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1514" fontId="878" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="879" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="880" fillId="1517" borderId="1701" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="881" fillId="1508" borderId="1705" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="882" fillId="1520" borderId="1709" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="883" fillId="1520" borderId="1709" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="884" fillId="1511" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="885" fillId="1523" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="886" fillId="1511" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="887" fillId="1526" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="879" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1701" fillId="1517" fontId="880" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1705" fillId="1508" fontId="881" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1709" fillId="1520" fontId="882" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1709" fillId="1520" fontId="883" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1511" fontId="884" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1523" fontId="885" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1511" fontId="886" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1526" fontId="887" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1717" fillId="1529" fontId="888" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="889" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1721" fillId="1532" fontId="890" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1725" fillId="1535" fontId="891" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1729" fillId="1538" fontId="892" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="893" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1541" fontId="894" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="895" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1733" fillId="1544" fontId="896" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1737" fillId="1535" fontId="897" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1741" fillId="1547" fontId="898" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1741" fillId="1547" fontId="899" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1538" fontId="900" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1550" fontId="901" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1538" fontId="902" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1553" fontId="903" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1749" fillId="1556" fontId="904" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="905" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1753" fillId="1559" fontId="906" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1757" fillId="1562" fontId="907" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1761" fillId="1565" fontId="908" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="909" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1568" fontId="910" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="911" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1765" fillId="1571" fontId="912" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1769" fillId="1562" fontId="913" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1773" fillId="1574" fontId="914" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1773" fillId="1574" fontId="915" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1565" fontId="916" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1577" fontId="917" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1565" fontId="918" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1580" fontId="919" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="920" fillId="1583" borderId="1781" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="921" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="922" fillId="1586" borderId="1785" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="923" fillId="1589" borderId="1789" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="924" fillId="1592" borderId="1793" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="925" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="926" fillId="1595" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="927" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="928" fillId="1598" borderId="1797" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="929" fillId="1589" borderId="1801" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="930" fillId="1601" borderId="1805" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="931" fillId="1601" borderId="1805" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="932" fillId="1592" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="933" fillId="1604" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="934" fillId="1592" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="935" fillId="1607" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -36307,7 +38198,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE129"/>
+  <dimension ref="A1:AF129"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -36390,21 +38281,24 @@
         <v>384</v>
       </c>
       <c r="Y1" t="s">
+        <v>529</v>
+      </c>
+      <c r="Z1" t="s">
         <v>45</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>46</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>47</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>48</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>401</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>215</v>
       </c>
     </row>
@@ -36482,21 +38376,24 @@
         <v>394</v>
       </c>
       <c r="Y2" t="s">
+        <v>530</v>
+      </c>
+      <c r="Z2" t="s">
         <v>87</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>160</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>165</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>172</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>419</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>486</v>
       </c>
     </row>
@@ -36567,22 +38464,22 @@
       <c r="X3" t="s">
         <v>395</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>88</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>161</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>166</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>353</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>173</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>216</v>
       </c>
     </row>
@@ -36650,22 +38547,22 @@
       <c r="X4" t="s">
         <v>396</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>343</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>162</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>167</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>173</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>411</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>217</v>
       </c>
     </row>
@@ -36724,22 +38621,22 @@
       <c r="W5" t="s">
         <v>348</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>344</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>163</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>168</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>174</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>412</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>218</v>
       </c>
     </row>
@@ -36792,22 +38689,22 @@
       <c r="W6" t="s">
         <v>350</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>89</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>432</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>169</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>175</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>413</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>219</v>
       </c>
     </row>
@@ -36854,22 +38751,22 @@
       <c r="W7" t="s">
         <v>349</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>90</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>433</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>170</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>176</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>414</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>520</v>
       </c>
     </row>
@@ -36910,22 +38807,22 @@
       <c r="W8" t="s">
         <v>351</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>91</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>164</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>171</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AC8" t="s">
         <v>177</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AD8" t="s">
         <v>415</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AE8" t="s">
         <v>521</v>
       </c>
     </row>
@@ -36966,13 +38863,13 @@
       <c r="W9" t="s">
         <v>352</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="Z9" t="s">
         <v>198</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AC9" t="s">
         <v>178</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AE9" t="s">
         <v>522</v>
       </c>
     </row>
@@ -37007,13 +38904,13 @@
       <c r="T10" t="s">
         <v>393</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="Z10" t="s">
         <v>247</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AC10" t="s">
         <v>179</v>
       </c>
-      <c r="AD10" t="s">
+      <c r="AE10" t="s">
         <v>220</v>
       </c>
     </row>
@@ -37045,13 +38942,13 @@
       <c r="R11" t="s">
         <v>236</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="Z11" t="s">
         <v>248</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AC11" t="s">
         <v>249</v>
       </c>
-      <c r="AD11" t="s">
+      <c r="AE11" t="s">
         <v>221</v>
       </c>
     </row>
@@ -37083,13 +38980,13 @@
       <c r="R12" t="s">
         <v>237</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="Z12" t="s">
         <v>92</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AC12" t="s">
         <v>180</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AE12" t="s">
         <v>222</v>
       </c>
     </row>
@@ -37118,13 +39015,13 @@
       <c r="R13" t="s">
         <v>242</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="Z13" t="s">
         <v>316</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AC13" t="s">
         <v>181</v>
       </c>
-      <c r="AD13" t="s">
+      <c r="AE13" t="s">
         <v>462</v>
       </c>
     </row>
@@ -37153,13 +39050,13 @@
       <c r="R14" t="s">
         <v>238</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="Z14" t="s">
         <v>93</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="AC14" t="s">
         <v>182</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AE14" t="s">
         <v>487</v>
       </c>
     </row>
@@ -37185,13 +39082,13 @@
       <c r="R15" t="s">
         <v>239</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="Z15" t="s">
         <v>94</v>
       </c>
-      <c r="AB15" t="s">
+      <c r="AC15" t="s">
         <v>183</v>
       </c>
-      <c r="AD15" t="s">
+      <c r="AE15" t="s">
         <v>488</v>
       </c>
     </row>
@@ -37217,13 +39114,13 @@
       <c r="R16" t="s">
         <v>240</v>
       </c>
-      <c r="Y16" t="s">
+      <c r="Z16" t="s">
         <v>66</v>
       </c>
-      <c r="AB16" t="s">
+      <c r="AC16" t="s">
         <v>184</v>
       </c>
-      <c r="AD16" t="s">
+      <c r="AE16" t="s">
         <v>489</v>
       </c>
     </row>
@@ -37243,13 +39140,13 @@
       <c r="M17" t="s">
         <v>35</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="Z17" t="s">
         <v>480</v>
       </c>
-      <c r="AB17" t="s">
+      <c r="AC17" t="s">
         <v>454</v>
       </c>
-      <c r="AD17" t="s">
+      <c r="AE17" t="s">
         <v>490</v>
       </c>
     </row>
@@ -37266,10 +39163,10 @@
       <c r="K18" t="s">
         <v>450</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="Z18" t="s">
         <v>95</v>
       </c>
-      <c r="AD18" t="s">
+      <c r="AE18" t="s">
         <v>463</v>
       </c>
     </row>
@@ -37286,10 +39183,10 @@
       <c r="K19" t="s">
         <v>74</v>
       </c>
-      <c r="Y19" t="s">
+      <c r="Z19" t="s">
         <v>96</v>
       </c>
-      <c r="AD19" t="s">
+      <c r="AE19" t="s">
         <v>491</v>
       </c>
     </row>
@@ -37306,10 +39203,10 @@
       <c r="K20" t="s">
         <v>75</v>
       </c>
-      <c r="Y20" t="s">
+      <c r="Z20" t="s">
         <v>97</v>
       </c>
-      <c r="AD20" t="s">
+      <c r="AE20" t="s">
         <v>492</v>
       </c>
     </row>
@@ -37326,10 +39223,10 @@
       <c r="K21" t="s">
         <v>369</v>
       </c>
-      <c r="Y21" t="s">
+      <c r="Z21" t="s">
         <v>98</v>
       </c>
-      <c r="AD21" t="s">
+      <c r="AE21" t="s">
         <v>493</v>
       </c>
     </row>
@@ -37346,10 +39243,10 @@
       <c r="K22" t="s">
         <v>458</v>
       </c>
-      <c r="Y22" t="s">
+      <c r="Z22" t="s">
         <v>481</v>
       </c>
-      <c r="AD22" t="s">
+      <c r="AE22" t="s">
         <v>223</v>
       </c>
     </row>
@@ -37366,10 +39263,10 @@
       <c r="K23" t="s">
         <v>36</v>
       </c>
-      <c r="Y23" t="s">
+      <c r="Z23" t="s">
         <v>99</v>
       </c>
-      <c r="AD23" t="s">
+      <c r="AE23" t="s">
         <v>523</v>
       </c>
     </row>
@@ -37386,16 +39283,16 @@
       <c r="K24" t="s">
         <v>381</v>
       </c>
-      <c r="Y24" t="s">
+      <c r="Z24" t="s">
         <v>100</v>
       </c>
-      <c r="AD24" t="s">
+      <c r="AE24" t="s">
         <v>524</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>529</v>
       </c>
       <c r="E25" t="s">
         <v>213</v>
@@ -37406,16 +39303,16 @@
       <c r="K25" t="s">
         <v>511</v>
       </c>
-      <c r="Y25" t="s">
+      <c r="Z25" t="s">
         <v>101</v>
       </c>
-      <c r="AD25" t="s">
+      <c r="AE25" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E26" t="s">
         <v>214</v>
@@ -37426,16 +39323,16 @@
       <c r="K26" t="s">
         <v>76</v>
       </c>
-      <c r="Y26" t="s">
+      <c r="Z26" t="s">
         <v>102</v>
       </c>
-      <c r="AD26" t="s">
+      <c r="AE26" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E27" t="s">
         <v>456</v>
@@ -37446,16 +39343,16 @@
       <c r="K27" t="s">
         <v>421</v>
       </c>
-      <c r="Y27" t="s">
+      <c r="Z27" t="s">
         <v>103</v>
       </c>
-      <c r="AD27" t="s">
+      <c r="AE27" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E28" t="s">
         <v>457</v>
@@ -37466,13 +39363,13 @@
       <c r="K28" t="s">
         <v>37</v>
       </c>
-      <c r="Y28" t="s">
+      <c r="Z28" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>401</v>
+        <v>48</v>
       </c>
       <c r="E29" t="s">
         <v>403</v>
@@ -37483,13 +39380,13 @@
       <c r="K29" t="s">
         <v>38</v>
       </c>
-      <c r="Y29" t="s">
+      <c r="Z29" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>215</v>
+        <v>401</v>
       </c>
       <c r="E30" t="s">
         <v>55</v>
@@ -37497,18 +39394,21 @@
       <c r="G30" t="s">
         <v>205</v>
       </c>
-      <c r="Y30" t="s">
+      <c r="Z30" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="31">
+      <c r="A31" t="s">
+        <v>215</v>
+      </c>
       <c r="E31" t="s">
         <v>56</v>
       </c>
       <c r="G31" t="s">
         <v>265</v>
       </c>
-      <c r="Y31" t="s">
+      <c r="Z31" t="s">
         <v>106</v>
       </c>
     </row>
@@ -37519,7 +39419,7 @@
       <c r="G32" t="s">
         <v>275</v>
       </c>
-      <c r="Y32" t="s">
+      <c r="Z32" t="s">
         <v>107</v>
       </c>
     </row>
@@ -37530,7 +39430,7 @@
       <c r="G33" t="s">
         <v>496</v>
       </c>
-      <c r="Y33" t="s">
+      <c r="Z33" t="s">
         <v>108</v>
       </c>
     </row>
@@ -37541,7 +39441,7 @@
       <c r="G34" t="s">
         <v>250</v>
       </c>
-      <c r="Y34" t="s">
+      <c r="Z34" t="s">
         <v>109</v>
       </c>
     </row>
@@ -37552,7 +39452,7 @@
       <c r="G35" t="s">
         <v>320</v>
       </c>
-      <c r="Y35" t="s">
+      <c r="Z35" t="s">
         <v>199</v>
       </c>
     </row>
@@ -37563,7 +39463,7 @@
       <c r="G36" t="s">
         <v>297</v>
       </c>
-      <c r="Y36" t="s">
+      <c r="Z36" t="s">
         <v>110</v>
       </c>
     </row>
@@ -37574,7 +39474,7 @@
       <c r="G37" t="s">
         <v>251</v>
       </c>
-      <c r="Y37" t="s">
+      <c r="Z37" t="s">
         <v>328</v>
       </c>
     </row>
@@ -37582,7 +39482,7 @@
       <c r="G38" t="s">
         <v>298</v>
       </c>
-      <c r="Y38" t="s">
+      <c r="Z38" t="s">
         <v>425</v>
       </c>
     </row>
@@ -37590,7 +39490,7 @@
       <c r="G39" t="s">
         <v>257</v>
       </c>
-      <c r="Y39" t="s">
+      <c r="Z39" t="s">
         <v>515</v>
       </c>
     </row>
@@ -37598,7 +39498,7 @@
       <c r="G40" t="s">
         <v>69</v>
       </c>
-      <c r="Y40" t="s">
+      <c r="Z40" t="s">
         <v>382</v>
       </c>
     </row>
@@ -37606,7 +39506,7 @@
       <c r="G41" t="s">
         <v>201</v>
       </c>
-      <c r="Y41" t="s">
+      <c r="Z41" t="s">
         <v>111</v>
       </c>
     </row>
@@ -37614,7 +39514,7 @@
       <c r="G42" t="s">
         <v>279</v>
       </c>
-      <c r="Y42" t="s">
+      <c r="Z42" t="s">
         <v>112</v>
       </c>
     </row>
@@ -37622,7 +39522,7 @@
       <c r="G43" t="s">
         <v>290</v>
       </c>
-      <c r="Y43" t="s">
+      <c r="Z43" t="s">
         <v>113</v>
       </c>
     </row>
@@ -37630,7 +39530,7 @@
       <c r="G44" t="s">
         <v>291</v>
       </c>
-      <c r="Y44" t="s">
+      <c r="Z44" t="s">
         <v>114</v>
       </c>
     </row>
@@ -37638,7 +39538,7 @@
       <c r="G45" t="s">
         <v>333</v>
       </c>
-      <c r="Y45" t="s">
+      <c r="Z45" t="s">
         <v>115</v>
       </c>
     </row>
@@ -37646,7 +39546,7 @@
       <c r="G46" t="s">
         <v>332</v>
       </c>
-      <c r="Y46" t="s">
+      <c r="Z46" t="s">
         <v>116</v>
       </c>
     </row>
@@ -37654,7 +39554,7 @@
       <c r="G47" t="s">
         <v>200</v>
       </c>
-      <c r="Y47" t="s">
+      <c r="Z47" t="s">
         <v>426</v>
       </c>
     </row>
@@ -37662,7 +39562,7 @@
       <c r="G48" t="s">
         <v>310</v>
       </c>
-      <c r="Y48" t="s">
+      <c r="Z48" t="s">
         <v>202</v>
       </c>
     </row>
@@ -37670,7 +39570,7 @@
       <c r="G49" t="s">
         <v>329</v>
       </c>
-      <c r="Y49" t="s">
+      <c r="Z49" t="s">
         <v>68</v>
       </c>
     </row>
@@ -37678,7 +39578,7 @@
       <c r="G50" t="s">
         <v>357</v>
       </c>
-      <c r="Y50" t="s">
+      <c r="Z50" t="s">
         <v>527</v>
       </c>
     </row>
@@ -37686,7 +39586,7 @@
       <c r="G51" t="s">
         <v>292</v>
       </c>
-      <c r="Y51" t="s">
+      <c r="Z51" t="s">
         <v>117</v>
       </c>
     </row>
@@ -37694,7 +39594,7 @@
       <c r="G52" t="s">
         <v>345</v>
       </c>
-      <c r="Y52" t="s">
+      <c r="Z52" t="s">
         <v>118</v>
       </c>
     </row>
@@ -37702,7 +39602,7 @@
       <c r="G53" t="s">
         <v>321</v>
       </c>
-      <c r="Y53" t="s">
+      <c r="Z53" t="s">
         <v>119</v>
       </c>
     </row>
@@ -37710,7 +39610,7 @@
       <c r="G54" t="s">
         <v>258</v>
       </c>
-      <c r="Y54" t="s">
+      <c r="Z54" t="s">
         <v>482</v>
       </c>
     </row>
@@ -37718,7 +39618,7 @@
       <c r="G55" t="s">
         <v>282</v>
       </c>
-      <c r="Y55" t="s">
+      <c r="Z55" t="s">
         <v>451</v>
       </c>
     </row>
@@ -37726,7 +39626,7 @@
       <c r="G56" t="s">
         <v>283</v>
       </c>
-      <c r="Y56" t="s">
+      <c r="Z56" t="s">
         <v>120</v>
       </c>
     </row>
@@ -37734,7 +39634,7 @@
       <c r="G57" t="s">
         <v>284</v>
       </c>
-      <c r="Y57" t="s">
+      <c r="Z57" t="s">
         <v>336</v>
       </c>
     </row>
@@ -37742,7 +39642,7 @@
       <c r="G58" t="s">
         <v>293</v>
       </c>
-      <c r="Y58" t="s">
+      <c r="Z58" t="s">
         <v>452</v>
       </c>
     </row>
@@ -37750,7 +39650,7 @@
       <c r="G59" t="s">
         <v>302</v>
       </c>
-      <c r="Y59" t="s">
+      <c r="Z59" t="s">
         <v>121</v>
       </c>
     </row>
@@ -37758,7 +39658,7 @@
       <c r="G60" t="s">
         <v>327</v>
       </c>
-      <c r="Y60" t="s">
+      <c r="Z60" t="s">
         <v>122</v>
       </c>
     </row>
@@ -37766,7 +39666,7 @@
       <c r="G61" t="s">
         <v>299</v>
       </c>
-      <c r="Y61" t="s">
+      <c r="Z61" t="s">
         <v>123</v>
       </c>
     </row>
@@ -37774,7 +39674,7 @@
       <c r="G62" t="s">
         <v>300</v>
       </c>
-      <c r="Y62" t="s">
+      <c r="Z62" t="s">
         <v>124</v>
       </c>
     </row>
@@ -37782,7 +39682,7 @@
       <c r="G63" t="s">
         <v>358</v>
       </c>
-      <c r="Y63" t="s">
+      <c r="Z63" t="s">
         <v>125</v>
       </c>
     </row>
@@ -37790,7 +39690,7 @@
       <c r="G64" t="s">
         <v>359</v>
       </c>
-      <c r="Y64" t="s">
+      <c r="Z64" t="s">
         <v>126</v>
       </c>
     </row>
@@ -37798,7 +39698,7 @@
       <c r="G65" t="s">
         <v>335</v>
       </c>
-      <c r="Y65" t="s">
+      <c r="Z65" t="s">
         <v>127</v>
       </c>
     </row>
@@ -37806,7 +39706,7 @@
       <c r="G66" t="s">
         <v>303</v>
       </c>
-      <c r="Y66" t="s">
+      <c r="Z66" t="s">
         <v>427</v>
       </c>
     </row>
@@ -37814,7 +39714,7 @@
       <c r="G67" t="s">
         <v>259</v>
       </c>
-      <c r="Y67" t="s">
+      <c r="Z67" t="s">
         <v>461</v>
       </c>
     </row>
@@ -37822,7 +39722,7 @@
       <c r="G68" t="s">
         <v>512</v>
       </c>
-      <c r="Y68" t="s">
+      <c r="Z68" t="s">
         <v>203</v>
       </c>
     </row>
@@ -37830,7 +39730,7 @@
       <c r="G69" t="s">
         <v>304</v>
       </c>
-      <c r="Y69" t="s">
+      <c r="Z69" t="s">
         <v>378</v>
       </c>
     </row>
@@ -37838,7 +39738,7 @@
       <c r="G70" t="s">
         <v>397</v>
       </c>
-      <c r="Y70" t="s">
+      <c r="Z70" t="s">
         <v>428</v>
       </c>
     </row>
@@ -37846,7 +39746,7 @@
       <c r="G71" t="s">
         <v>294</v>
       </c>
-      <c r="Y71" t="s">
+      <c r="Z71" t="s">
         <v>128</v>
       </c>
     </row>
@@ -37854,7 +39754,7 @@
       <c r="G72" t="s">
         <v>398</v>
       </c>
-      <c r="Y72" t="s">
+      <c r="Z72" t="s">
         <v>129</v>
       </c>
     </row>
@@ -37862,7 +39762,7 @@
       <c r="G73" t="s">
         <v>252</v>
       </c>
-      <c r="Y73" t="s">
+      <c r="Z73" t="s">
         <v>130</v>
       </c>
     </row>
@@ -37870,7 +39770,7 @@
       <c r="G74" t="s">
         <v>497</v>
       </c>
-      <c r="Y74" t="s">
+      <c r="Z74" t="s">
         <v>131</v>
       </c>
     </row>
@@ -37878,7 +39778,7 @@
       <c r="G75" t="s">
         <v>334</v>
       </c>
-      <c r="Y75" t="s">
+      <c r="Z75" t="s">
         <v>186</v>
       </c>
     </row>
@@ -37886,7 +39786,7 @@
       <c r="G76" t="s">
         <v>270</v>
       </c>
-      <c r="Y76" t="s">
+      <c r="Z76" t="s">
         <v>187</v>
       </c>
     </row>
@@ -37894,7 +39794,7 @@
       <c r="G77" t="s">
         <v>276</v>
       </c>
-      <c r="Y77" t="s">
+      <c r="Z77" t="s">
         <v>440</v>
       </c>
     </row>
@@ -37902,7 +39802,7 @@
       <c r="G78" t="s">
         <v>281</v>
       </c>
-      <c r="Y78" t="s">
+      <c r="Z78" t="s">
         <v>453</v>
       </c>
     </row>
@@ -37910,7 +39810,7 @@
       <c r="G79" t="s">
         <v>416</v>
       </c>
-      <c r="Y79" t="s">
+      <c r="Z79" t="s">
         <v>132</v>
       </c>
     </row>
@@ -37918,7 +39818,7 @@
       <c r="G80" t="s">
         <v>322</v>
       </c>
-      <c r="Y80" t="s">
+      <c r="Z80" t="s">
         <v>133</v>
       </c>
     </row>
@@ -37926,7 +39826,7 @@
       <c r="G81" t="s">
         <v>260</v>
       </c>
-      <c r="Y81" t="s">
+      <c r="Z81" t="s">
         <v>134</v>
       </c>
     </row>
@@ -37934,7 +39834,7 @@
       <c r="G82" t="s">
         <v>271</v>
       </c>
-      <c r="Y82" t="s">
+      <c r="Z82" t="s">
         <v>483</v>
       </c>
     </row>
@@ -37942,7 +39842,7 @@
       <c r="G83" t="s">
         <v>277</v>
       </c>
-      <c r="Y83" t="s">
+      <c r="Z83" t="s">
         <v>135</v>
       </c>
     </row>
@@ -37950,7 +39850,7 @@
       <c r="G84" t="s">
         <v>266</v>
       </c>
-      <c r="Y84" t="s">
+      <c r="Z84" t="s">
         <v>136</v>
       </c>
     </row>
@@ -37958,7 +39858,7 @@
       <c r="G85" t="s">
         <v>517</v>
       </c>
-      <c r="Y85" t="s">
+      <c r="Z85" t="s">
         <v>188</v>
       </c>
     </row>
@@ -37966,7 +39866,7 @@
       <c r="G86" t="s">
         <v>261</v>
       </c>
-      <c r="Y86" t="s">
+      <c r="Z86" t="s">
         <v>484</v>
       </c>
     </row>
@@ -37974,7 +39874,7 @@
       <c r="G87" t="s">
         <v>278</v>
       </c>
-      <c r="Y87" t="s">
+      <c r="Z87" t="s">
         <v>189</v>
       </c>
     </row>
@@ -37982,7 +39882,7 @@
       <c r="G88" t="s">
         <v>262</v>
       </c>
-      <c r="Y88" t="s">
+      <c r="Z88" t="s">
         <v>441</v>
       </c>
     </row>
@@ -37990,7 +39890,7 @@
       <c r="G89" t="s">
         <v>263</v>
       </c>
-      <c r="Y89" t="s">
+      <c r="Z89" t="s">
         <v>190</v>
       </c>
     </row>
@@ -37998,7 +39898,7 @@
       <c r="G90" t="s">
         <v>295</v>
       </c>
-      <c r="Y90" t="s">
+      <c r="Z90" t="s">
         <v>191</v>
       </c>
     </row>
@@ -38006,7 +39906,7 @@
       <c r="G91" t="s">
         <v>301</v>
       </c>
-      <c r="Y91" t="s">
+      <c r="Z91" t="s">
         <v>204</v>
       </c>
     </row>
@@ -38014,7 +39914,7 @@
       <c r="G92" t="s">
         <v>285</v>
       </c>
-      <c r="Y92" t="s">
+      <c r="Z92" t="s">
         <v>137</v>
       </c>
     </row>
@@ -38022,7 +39922,7 @@
       <c r="G93" t="s">
         <v>330</v>
       </c>
-      <c r="Y93" t="s">
+      <c r="Z93" t="s">
         <v>192</v>
       </c>
     </row>
@@ -38030,7 +39930,7 @@
       <c r="G94" t="s">
         <v>267</v>
       </c>
-      <c r="Y94" t="s">
+      <c r="Z94" t="s">
         <v>429</v>
       </c>
     </row>
@@ -38038,177 +39938,177 @@
       <c r="G95" t="s">
         <v>268</v>
       </c>
-      <c r="Y95" t="s">
+      <c r="Z95" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="96">
-      <c r="Y96" t="s">
+      <c r="Z96" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="97">
-      <c r="Y97" t="s">
+      <c r="Z97" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="98">
-      <c r="Y98" t="s">
+      <c r="Z98" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="99">
-      <c r="Y99" t="s">
+      <c r="Z99" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="100">
-      <c r="Y100" t="s">
+      <c r="Z100" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="101">
-      <c r="Y101" t="s">
+      <c r="Z101" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="102">
-      <c r="Y102" t="s">
+      <c r="Z102" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="103">
-      <c r="Y103" t="s">
+      <c r="Z103" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="104">
-      <c r="Y104" t="s">
+      <c r="Z104" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="105">
-      <c r="Y105" t="s">
+      <c r="Z105" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="106">
-      <c r="Y106" t="s">
+      <c r="Z106" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="107">
-      <c r="Y107" t="s">
+      <c r="Z107" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="108">
-      <c r="Y108" t="s">
+      <c r="Z108" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="109">
-      <c r="Y109" t="s">
+      <c r="Z109" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="110">
-      <c r="Y110" t="s">
+      <c r="Z110" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="111">
-      <c r="Y111" t="s">
+      <c r="Z111" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="112">
-      <c r="Y112" t="s">
+      <c r="Z112" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="113">
-      <c r="Y113" t="s">
+      <c r="Z113" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="114">
-      <c r="Y114" t="s">
+      <c r="Z114" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="115">
-      <c r="Y115" t="s">
+      <c r="Z115" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="116">
-      <c r="Y116" t="s">
+      <c r="Z116" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="117">
-      <c r="Y117" t="s">
+      <c r="Z117" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="118">
-      <c r="Y118" t="s">
+      <c r="Z118" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="119">
-      <c r="Y119" t="s">
+      <c r="Z119" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="120">
-      <c r="Y120" t="s">
+      <c r="Z120" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="121">
-      <c r="Y121" t="s">
+      <c r="Z121" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="122">
-      <c r="Y122" t="s">
+      <c r="Z122" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="123">
-      <c r="Y123" t="s">
+      <c r="Z123" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="124">
-      <c r="Y124" t="s">
+      <c r="Z124" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="125">
-      <c r="Y125" t="s">
+      <c r="Z125" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="126">
-      <c r="Y126" t="s">
+      <c r="Z126" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="127">
-      <c r="Y127" t="s">
+      <c r="Z127" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="128">
-      <c r="Y128" t="s">
+      <c r="Z128" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="129">
-      <c r="Y129" t="s">
+      <c r="Z129" t="s">
         <v>159</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[desktop] - [`mouseWheel(amount,modifiers,x,y)`](../commands/desktop/mouseWheel(amount,modifiers,x,y)): **NEW** command to   simulate mouse wheel movement. `amount` as negative value means to scroll _backwards_. - [`clickScreen(button,modifiers,x,y)`](../commands/desktop/clickScreen(button,modifiers,x,y)): **NEW** command to   simulate mouse click based on current screen (not AUT).
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42467" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43017" uniqueCount="532">
   <si>
     <t>description</t>
   </si>
@@ -1665,7 +1665,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1240" x14ac:knownFonts="1">
+  <fonts count="1256" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -9496,8 +9496,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="2121">
+  <fills count="2148">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -21512,8 +21613,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2414">
+  <borders count="2446">
     <border>
       <left/>
       <right/>
@@ -25024,6 +25278,332 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -46072,7 +46652,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1253">
+  <cellXfs count="1269">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -49790,52 +50370,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="2093" fontId="1223" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1224" fillId="2096" borderId="2389" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1225" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2389" fillId="2096" fontId="1224" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1225" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1226" fillId="2099" borderId="2393" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2393" fillId="2099" fontId="1226" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1227" fillId="2102" borderId="2397" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2397" fillId="2102" fontId="1227" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1228" fillId="2105" borderId="2401" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2401" fillId="2105" fontId="1228" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1229" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1229" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1230" fillId="2108" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2108" fontId="1230" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1231" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1232" fillId="2111" borderId="2405" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1233" fillId="2102" borderId="2409" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1234" fillId="2114" borderId="2413" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1235" fillId="2114" borderId="2413" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1236" fillId="2105" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1237" fillId="2117" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1238" fillId="2105" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1239" fillId="2120" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1231" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2405" fillId="2111" fontId="1232" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2409" fillId="2102" fontId="1233" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2413" fillId="2114" fontId="1234" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2413" fillId="2114" fontId="1235" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2105" fontId="1236" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2117" fontId="1237" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2105" fontId="1238" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2120" fontId="1239" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1240" fillId="2123" borderId="2421" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1241" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1242" fillId="2126" borderId="2425" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1243" fillId="2129" borderId="2429" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1244" fillId="2132" borderId="2433" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1245" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1246" fillId="2135" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1247" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1248" fillId="2138" borderId="2437" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1249" fillId="2129" borderId="2441" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1250" fillId="2141" borderId="2445" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1251" fillId="2141" borderId="2445" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1252" fillId="2132" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1253" fillId="2144" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1254" fillId="2132" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1255" fillId="2147" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[desktop] - [`mouseWheel(amount,modifiers,x,y)`](../commands/desktop/mouseWheel(amount,modifiers,x,y)): support simple "position"   words for `x` and `y`. - [`mouseWheel(amount,modifiers,x,y)`](../commands/desktop/mouseWheel(amount,modifiers,x,y)): restrict to Windows for now.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47433" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48537" uniqueCount="534">
   <si>
     <t>description</t>
   </si>
@@ -1671,7 +1671,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1384" x14ac:knownFonts="1">
+  <fonts count="1416" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -10411,8 +10411,210 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="2364">
+  <fills count="2418">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -23804,8 +24006,314 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2702">
+  <borders count="2766">
     <border>
       <left/>
       <right/>
@@ -27316,6 +27824,658 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -51298,7 +52458,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1397">
+  <cellXfs count="1429">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -55448,52 +56608,148 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="2336" fontId="1367" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1368" fillId="2339" borderId="2677" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1369" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2677" fillId="2339" fontId="1368" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1369" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1370" fillId="2342" borderId="2681" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2681" fillId="2342" fontId="1370" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1371" fillId="2345" borderId="2685" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2685" fillId="2345" fontId="1371" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1372" fillId="2348" borderId="2689" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2689" fillId="2348" fontId="1372" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1373" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1373" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1374" fillId="2351" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2351" fontId="1374" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1375" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1376" fillId="2354" borderId="2693" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1377" fillId="2345" borderId="2697" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1378" fillId="2357" borderId="2701" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1379" fillId="2357" borderId="2701" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1380" fillId="2348" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1381" fillId="2360" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1382" fillId="2348" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1383" fillId="2363" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1375" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2693" fillId="2354" fontId="1376" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2697" fillId="2345" fontId="1377" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2701" fillId="2357" fontId="1378" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2701" fillId="2357" fontId="1379" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2348" fontId="1380" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2360" fontId="1381" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2348" fontId="1382" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2363" fontId="1383" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2709" fillId="2366" fontId="1384" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1385" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2713" fillId="2369" fontId="1386" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2717" fillId="2372" fontId="1387" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2721" fillId="2375" fontId="1388" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1389" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2378" fontId="1390" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1391" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2725" fillId="2381" fontId="1392" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2729" fillId="2372" fontId="1393" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2733" fillId="2384" fontId="1394" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2733" fillId="2384" fontId="1395" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2375" fontId="1396" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2387" fontId="1397" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2375" fontId="1398" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2390" fontId="1399" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1400" fillId="2393" borderId="2741" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1401" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1402" fillId="2396" borderId="2745" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1403" fillId="2399" borderId="2749" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1404" fillId="2402" borderId="2753" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1405" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1406" fillId="2405" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1407" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1408" fillId="2408" borderId="2757" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1409" fillId="2399" borderId="2761" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1410" fillId="2411" borderId="2765" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1411" fillId="2411" borderId="2765" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1412" fillId="2402" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1413" fillId="2414" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1414" fillId="2402" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1415" fillId="2417" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[desktop] - [`typeKeys(os,keystrokes)`](../commands/desktop/typeKeys(os,keystrokes)): support the use of `*` for `os`.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48537" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50193" uniqueCount="534">
   <si>
     <t>description</t>
   </si>
@@ -1671,7 +1671,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1416" x14ac:knownFonts="1">
+  <fonts count="1464" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -10613,8 +10613,311 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="2418">
+  <fills count="2499">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -24312,8 +24615,467 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2766">
+  <borders count="2862">
     <border>
       <left/>
       <right/>
@@ -27824,6 +28586,984 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -52458,7 +54198,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1429">
+  <cellXfs count="1477">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -56704,52 +58444,196 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="2390" fontId="1399" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1400" fillId="2393" borderId="2741" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1401" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2741" fillId="2393" fontId="1400" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1401" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1402" fillId="2396" borderId="2745" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2745" fillId="2396" fontId="1402" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1403" fillId="2399" borderId="2749" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2749" fillId="2399" fontId="1403" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1404" fillId="2402" borderId="2753" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2753" fillId="2402" fontId="1404" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1405" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1405" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1406" fillId="2405" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2405" fontId="1406" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1407" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1408" fillId="2408" borderId="2757" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1409" fillId="2399" borderId="2761" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1410" fillId="2411" borderId="2765" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1411" fillId="2411" borderId="2765" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1412" fillId="2402" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1413" fillId="2414" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1414" fillId="2402" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1415" fillId="2417" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1407" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2757" fillId="2408" fontId="1408" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2761" fillId="2399" fontId="1409" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2765" fillId="2411" fontId="1410" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2765" fillId="2411" fontId="1411" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2402" fontId="1412" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2414" fontId="1413" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2402" fontId="1414" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2417" fontId="1415" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2773" fillId="2420" fontId="1416" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1417" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2777" fillId="2423" fontId="1418" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2781" fillId="2426" fontId="1419" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2785" fillId="2429" fontId="1420" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1421" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2432" fontId="1422" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1423" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2789" fillId="2435" fontId="1424" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2793" fillId="2426" fontId="1425" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2797" fillId="2438" fontId="1426" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2797" fillId="2438" fontId="1427" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2429" fontId="1428" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2441" fontId="1429" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2429" fontId="1430" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2444" fontId="1431" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2805" fillId="2447" fontId="1432" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1433" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2809" fillId="2450" fontId="1434" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2813" fillId="2453" fontId="1435" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2817" fillId="2456" fontId="1436" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1437" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2459" fontId="1438" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1439" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2821" fillId="2462" fontId="1440" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2825" fillId="2453" fontId="1441" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2829" fillId="2465" fontId="1442" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2829" fillId="2465" fontId="1443" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2456" fontId="1444" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2468" fontId="1445" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2456" fontId="1446" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2471" fontId="1447" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1448" fillId="2474" borderId="2837" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1449" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1450" fillId="2477" borderId="2841" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1451" fillId="2480" borderId="2845" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1452" fillId="2483" borderId="2849" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1453" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1454" fillId="2486" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1455" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1456" fillId="2489" borderId="2853" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1457" fillId="2480" borderId="2857" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1458" fillId="2492" borderId="2861" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1459" fillId="2492" borderId="2861" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1460" fillId="2483" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1461" fillId="2495" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1462" fillId="2483" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1463" fillId="2498" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[fix] - Fixed exception found when capturing screenshot within a   [base &raquo; `repeatUntil(steps,maxWaitMs)`](../commands/base/repeatUntil(steps,maxWaitMs)) loop.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58473" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60129" uniqueCount="534">
   <si>
     <t>description</t>
   </si>
@@ -1671,7 +1671,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1704" x14ac:knownFonts="1">
+  <fonts count="1752" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -12431,8 +12431,311 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="2904">
+  <fills count="2985">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -28884,8 +29187,467 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3342">
+  <borders count="3438">
     <border>
       <left/>
       <right/>
@@ -32396,6 +33158,984 @@
       </top>
       <bottom style="thin">
         <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
       </bottom>
     </border>
     <border>
@@ -62898,7 +64638,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1717">
+  <cellXfs count="1765">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -68008,52 +69748,196 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="2876" fontId="1687" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1688" fillId="2879" borderId="3317" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1689" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3317" fillId="2879" fontId="1688" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1689" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1690" fillId="2882" borderId="3321" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3321" fillId="2882" fontId="1690" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1691" fillId="2885" borderId="3325" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3325" fillId="2885" fontId="1691" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1692" fillId="2888" borderId="3329" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3329" fillId="2888" fontId="1692" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1693" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1693" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1694" fillId="2891" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2891" fontId="1694" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1695" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1696" fillId="2894" borderId="3333" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1697" fillId="2885" borderId="3337" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1698" fillId="2897" borderId="3341" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1699" fillId="2897" borderId="3341" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1700" fillId="2888" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1701" fillId="2900" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1702" fillId="2888" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1703" fillId="2903" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1695" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3333" fillId="2894" fontId="1696" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3337" fillId="2885" fontId="1697" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3341" fillId="2897" fontId="1698" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3341" fillId="2897" fontId="1699" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2888" fontId="1700" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2900" fontId="1701" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2888" fontId="1702" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2903" fontId="1703" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3349" fillId="2906" fontId="1704" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1705" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3353" fillId="2909" fontId="1706" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3357" fillId="2912" fontId="1707" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3361" fillId="2915" fontId="1708" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1709" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2918" fontId="1710" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1711" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3365" fillId="2921" fontId="1712" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3369" fillId="2912" fontId="1713" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3373" fillId="2924" fontId="1714" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3373" fillId="2924" fontId="1715" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2915" fontId="1716" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2927" fontId="1717" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2915" fontId="1718" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2930" fontId="1719" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3381" fillId="2933" fontId="1720" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1721" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3385" fillId="2936" fontId="1722" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3389" fillId="2939" fontId="1723" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3393" fillId="2942" fontId="1724" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1725" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2945" fontId="1726" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1727" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3397" fillId="2948" fontId="1728" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3401" fillId="2939" fontId="1729" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3405" fillId="2951" fontId="1730" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3405" fillId="2951" fontId="1731" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2942" fontId="1732" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2954" fontId="1733" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2942" fontId="1734" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2957" fontId="1735" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1736" fillId="2960" borderId="3413" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1737" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1738" fillId="2963" borderId="3417" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1739" fillId="2966" borderId="3421" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1740" fillId="2969" borderId="3425" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1741" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1742" fillId="2972" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1743" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1744" fillId="2975" borderId="3429" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1745" fillId="2966" borderId="3433" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1746" fillId="2978" borderId="3437" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1747" fillId="2978" borderId="3437" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1748" fillId="2969" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1749" fillId="2981" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1750" fillId="2969" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1751" fillId="2984" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[base] - [`nexial.assert.lenient`]: join multiple lines into one before text assertion. Default is `true`. - [`nexial.assert.asNumber`]: assert text numerically so that `1` is the same as `1.0`. Default is `true`. - [`nexial.assert.useTrim`]: trim text before assertion. Default is `false`. - [`nexial.assert.caseInsensitive`]: assert text case-insensitively. Default is `false`.
[web]
- [`saveTableAsCsv(locator,nextPageLocator,file)`] and [`saveDivsAsCsv(headers,rows,cells,nextPage,file)`]:
  - code fix to properly handle data cell that contains a mix of cell text and form element.

- updated Installation Guide on documentation site

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2775" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3328" uniqueCount="532">
   <si>
     <t>description</t>
   </si>
@@ -1665,7 +1665,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="72" x14ac:knownFonts="1">
+  <fonts count="88" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2123,8 +2123,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="111">
+  <fills count="138">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2749,8 +2850,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="130">
+  <borders count="162">
     <border>
       <left/>
       <right/>
@@ -4077,13 +4331,339 @@
         <color rgb="C3C3C3"/>
       </bottom>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="101">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -4297,52 +4877,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="83" fontId="55" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="86" borderId="105" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="105" fillId="86" fontId="56" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="57" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="89" borderId="109" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="109" fillId="89" fontId="58" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="92" borderId="113" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="113" fillId="92" fontId="59" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="95" borderId="117" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="117" fillId="95" fontId="60" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="61" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="98" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="98" fontId="62" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="63" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="64" fillId="101" borderId="121" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="121" fillId="101" fontId="64" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="92" borderId="125" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="125" fillId="92" fontId="65" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="66" fillId="104" borderId="129" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="129" fillId="104" fontId="66" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="104" borderId="129" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="129" fillId="104" fontId="67" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="95" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="95" fontId="68" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="69" fillId="107" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="107" fontId="69" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="70" fillId="95" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="95" fontId="70" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="71" fillId="110" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="110" fontId="71" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="113" borderId="137" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="116" borderId="141" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="119" borderId="145" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="122" borderId="149" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="125" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="128" borderId="153" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="119" borderId="157" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="82" fillId="131" borderId="161" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="131" borderId="161" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="84" fillId="122" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="134" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="86" fillId="122" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="87" fillId="137" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[improvements] - minor updates to [`nexial-project`] batch files to reduce output - minor improvement to trim directory name before validating its existence or usefulness.
[aws.vision commands]
- [`saveText(profile,image,var)`]: support 'system' profile to simplify scripting for users using team-wide or company-wide [setup]

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22800" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24480" uniqueCount="541">
   <si>
     <t>description</t>
   </si>
@@ -1693,7 +1693,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="648" x14ac:knownFonts="1">
+  <fonts count="696" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5787,8 +5787,311 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1083">
+  <fills count="1164">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -11921,8 +12224,467 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1282">
+  <borders count="1378">
     <border>
       <left/>
       <right/>
@@ -11944,6 +12706,984 @@
         <color theme="2" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
     </border>
     <border>
       <top style="thin"/>
@@ -24991,7 +26731,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="661">
+  <cellXfs count="709">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -26933,52 +28673,196 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1055" fontId="631" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="632" fillId="1058" borderId="1257" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="633" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1257" fillId="1058" fontId="632" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="633" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="634" fillId="1061" borderId="1261" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1261" fillId="1061" fontId="634" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="635" fillId="1064" borderId="1265" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1265" fillId="1064" fontId="635" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="636" fillId="1067" borderId="1269" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1269" fillId="1067" fontId="636" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="637" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="637" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="638" fillId="1070" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1070" fontId="638" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="639" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="640" fillId="1073" borderId="1273" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="641" fillId="1064" borderId="1277" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="642" fillId="1076" borderId="1281" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="643" fillId="1076" borderId="1281" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="644" fillId="1067" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="645" fillId="1079" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="646" fillId="1067" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="647" fillId="1082" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="639" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1273" fillId="1073" fontId="640" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1277" fillId="1064" fontId="641" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1281" fillId="1076" fontId="642" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1281" fillId="1076" fontId="643" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1067" fontId="644" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1079" fontId="645" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1067" fontId="646" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1082" fontId="647" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1289" fillId="1085" fontId="648" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="649" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1293" fillId="1088" fontId="650" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1297" fillId="1091" fontId="651" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1301" fillId="1094" fontId="652" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="653" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1097" fontId="654" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="655" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1305" fillId="1100" fontId="656" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1309" fillId="1091" fontId="657" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1313" fillId="1103" fontId="658" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1313" fillId="1103" fontId="659" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1094" fontId="660" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1106" fontId="661" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1094" fontId="662" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1109" fontId="663" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1321" fillId="1112" fontId="664" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="665" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1325" fillId="1115" fontId="666" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1329" fillId="1118" fontId="667" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1333" fillId="1121" fontId="668" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="669" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1124" fontId="670" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="671" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1337" fillId="1127" fontId="672" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1341" fillId="1118" fontId="673" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1345" fillId="1130" fontId="674" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1345" fillId="1130" fontId="675" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1121" fontId="676" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1133" fontId="677" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1121" fontId="678" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1136" fontId="679" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="680" fillId="1139" borderId="1353" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="681" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="682" fillId="1142" borderId="1357" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="683" fillId="1145" borderId="1361" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="684" fillId="1148" borderId="1365" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="685" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="686" fillId="1151" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="687" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="688" fillId="1154" borderId="1369" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="689" fillId="1145" borderId="1373" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="690" fillId="1157" borderId="1377" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="691" fillId="1157" borderId="1377" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="692" fillId="1148" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="693" fillId="1160" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="694" fillId="1148" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="695" fillId="1163" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[expression] - [TEXT expression]: code fix to handle escaped delimiter (meaning same character as [`nexial.textDelim`])
[web]
- [`saveDivsAsCsv(headers,rows,cells,nextPage,file)`]: enable the use of `(null)`, `(empty)` or `(blank)` for `headers` and `nextPage` to omit the use of these parameters.
- [`saveTableAsCsv(locator,nextPageLocator,file)`]: enable the use of `(null)`, `(empty)` or `(blank)` for `nextPage` to omit the use of this parameter.
- [`saveInfiniteDivsAsCsv(config,file)`]: enable the use of `(null)`, `(empty)` or `(blank)` for `header-cell` to omit the use of this `config`.
- [`saveInfiniteTableAsCsv(config,file)`]: enable the use of `(null)`, `(empty)` or `(blank)` for `header-cell` to omit the use of this `config`.
- [web &raquo; `closeAll`](../commands/web/closeAll()): adjust to correct shut down sequence of target electron app.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26160" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27280" uniqueCount="544">
   <si>
     <t>description</t>
   </si>
@@ -1702,7 +1702,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="744" x14ac:knownFonts="1">
+  <fonts count="776" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6402,8 +6402,210 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1245">
+  <fills count="1299">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -13454,8 +13656,314 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1474">
+  <borders count="1538">
     <border>
       <left/>
       <right/>
@@ -13477,6 +13985,658 @@
         <color theme="2" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
     </border>
     <border>
       <top style="thin"/>
@@ -28480,7 +29640,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="757">
+  <cellXfs count="789">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -30710,52 +31870,148 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1217" fontId="727" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="728" fillId="1220" borderId="1449" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="729" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1449" fillId="1220" fontId="728" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="729" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="730" fillId="1223" borderId="1453" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1453" fillId="1223" fontId="730" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="731" fillId="1226" borderId="1457" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1457" fillId="1226" fontId="731" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="732" fillId="1229" borderId="1461" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1461" fillId="1229" fontId="732" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="733" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="733" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="734" fillId="1232" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1232" fontId="734" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="735" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="736" fillId="1235" borderId="1465" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="737" fillId="1226" borderId="1469" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="738" fillId="1238" borderId="1473" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="739" fillId="1238" borderId="1473" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="740" fillId="1229" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="741" fillId="1241" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="742" fillId="1229" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="743" fillId="1244" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="735" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1465" fillId="1235" fontId="736" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1469" fillId="1226" fontId="737" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1473" fillId="1238" fontId="738" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1473" fillId="1238" fontId="739" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1229" fontId="740" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1241" fontId="741" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1229" fontId="742" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1244" fontId="743" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1481" fillId="1247" fontId="744" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="745" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1485" fillId="1250" fontId="746" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1489" fillId="1253" fontId="747" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1493" fillId="1256" fontId="748" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="749" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1259" fontId="750" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="751" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1497" fillId="1262" fontId="752" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1501" fillId="1253" fontId="753" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1505" fillId="1265" fontId="754" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1505" fillId="1265" fontId="755" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1256" fontId="756" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1268" fontId="757" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1256" fontId="758" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1271" fontId="759" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="760" fillId="1274" borderId="1513" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="761" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="762" fillId="1277" borderId="1517" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="763" fillId="1280" borderId="1521" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="764" fillId="1283" borderId="1525" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="765" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="766" fillId="1286" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="767" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="768" fillId="1289" borderId="1529" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="769" fillId="1280" borderId="1533" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="770" fillId="1292" borderId="1537" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="771" fillId="1292" borderId="1537" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="772" fillId="1283" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="773" fillId="1295" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="774" fillId="1283" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="775" fillId="1298" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[system variables] - [`nexial.resolveTextAsURL`]: **NEW** System variable to detect if a text parameter is a valid URL and if so, to download the content of that URL (GET) automatically. This supersede the now-deprecated System variable [`nexial.expression.resolveURL`] and applies beyond [TEXT expression] to areas such as [`ws`], [`csv`], [`io`], [`json`], [`web` >> `executeScript(var,script)`] and [`xml`] commands. The default for this System variable is `false`.
[web]
- [`nexial.web.highlight`]: fixed error when target element doesn't have any `style` attribute

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30080" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32320" uniqueCount="544">
   <si>
     <t>description</t>
   </si>
@@ -1702,7 +1702,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="856" x14ac:knownFonts="1">
+  <fonts count="920" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7109,8 +7109,412 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1434">
+  <fills count="1542">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -15232,8 +15636,620 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1698">
+  <borders count="1826">
     <border>
       <left/>
       <right/>
@@ -15255,6 +16271,1310 @@
         <color theme="2" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
     </border>
     <border>
       <top style="thin"/>
@@ -32540,7 +34860,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="869">
+  <cellXfs count="933">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -35106,52 +37426,244 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1406" fontId="839" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="840" fillId="1409" borderId="1673" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="841" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1673" fillId="1409" fontId="840" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="841" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="842" fillId="1412" borderId="1677" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1677" fillId="1412" fontId="842" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="843" fillId="1415" borderId="1681" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1681" fillId="1415" fontId="843" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="844" fillId="1418" borderId="1685" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1685" fillId="1418" fontId="844" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="845" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="845" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="846" fillId="1421" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1421" fontId="846" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="847" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="848" fillId="1424" borderId="1689" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="849" fillId="1415" borderId="1693" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="850" fillId="1427" borderId="1697" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="851" fillId="1427" borderId="1697" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="852" fillId="1418" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="853" fillId="1430" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="854" fillId="1418" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="855" fillId="1433" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="847" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1689" fillId="1424" fontId="848" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1693" fillId="1415" fontId="849" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1697" fillId="1427" fontId="850" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1697" fillId="1427" fontId="851" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1418" fontId="852" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1430" fontId="853" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1418" fontId="854" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1433" fontId="855" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1705" fillId="1436" fontId="856" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="857" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1709" fillId="1439" fontId="858" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1713" fillId="1442" fontId="859" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1717" fillId="1445" fontId="860" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="861" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1448" fontId="862" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="863" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1721" fillId="1451" fontId="864" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1725" fillId="1442" fontId="865" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1729" fillId="1454" fontId="866" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1729" fillId="1454" fontId="867" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1445" fontId="868" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1457" fontId="869" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1445" fontId="870" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1460" fontId="871" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1737" fillId="1463" fontId="872" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="873" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1741" fillId="1466" fontId="874" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1745" fillId="1469" fontId="875" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1749" fillId="1472" fontId="876" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="877" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1475" fontId="878" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="879" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1753" fillId="1478" fontId="880" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1757" fillId="1469" fontId="881" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1761" fillId="1481" fontId="882" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1761" fillId="1481" fontId="883" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1472" fontId="884" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1484" fontId="885" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1472" fontId="886" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1487" fontId="887" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1769" fillId="1490" fontId="888" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="889" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1773" fillId="1493" fontId="890" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1777" fillId="1496" fontId="891" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1781" fillId="1499" fontId="892" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="893" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1502" fontId="894" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="895" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1785" fillId="1505" fontId="896" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1789" fillId="1496" fontId="897" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1793" fillId="1508" fontId="898" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1793" fillId="1508" fontId="899" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1499" fontId="900" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1511" fontId="901" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1499" fontId="902" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1514" fontId="903" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="904" fillId="1517" borderId="1801" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="905" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="906" fillId="1520" borderId="1805" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="907" fillId="1523" borderId="1809" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="908" fillId="1526" borderId="1813" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="909" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="910" fillId="1529" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="911" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="912" fillId="1532" borderId="1817" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="913" fillId="1523" borderId="1821" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="914" fillId="1535" borderId="1825" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="915" fillId="1535" borderId="1825" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="916" fillId="1526" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="917" fillId="1538" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="918" fillId="1526" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="919" fillId="1541" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[expression] - [CSV &raquo; `replaceColumnRegex(searchFor,replaceWith,columnNameOrIndices`]:   - the parameter `columnNameOrIndices` now can be expressed as `*` to indicate **ALL** columns.   - fixed error when working on a file with columns wrapped in double quotes. - [CSV &raquo; `saveRowData(rowIndex)`]: save a row of CSV data as data variable by using the corresponding CSV header name as data variable name.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32320" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33440" uniqueCount="544">
   <si>
     <t>description</t>
   </si>
@@ -1702,7 +1702,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="920" x14ac:knownFonts="1">
+  <fonts count="952" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7513,8 +7513,210 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1542">
+  <fills count="1596">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -16248,8 +16450,314 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1826">
+  <borders count="1890">
     <border>
       <left/>
       <right/>
@@ -16271,6 +16779,658 @@
         <color theme="2" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
     </border>
     <border>
       <top style="thin"/>
@@ -34860,7 +36020,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="933">
+  <cellXfs count="965">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -37618,52 +38778,148 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1514" fontId="903" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="904" fillId="1517" borderId="1801" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="905" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1801" fillId="1517" fontId="904" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="905" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="906" fillId="1520" borderId="1805" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1805" fillId="1520" fontId="906" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="907" fillId="1523" borderId="1809" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1809" fillId="1523" fontId="907" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="908" fillId="1526" borderId="1813" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1813" fillId="1526" fontId="908" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="909" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="909" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="910" fillId="1529" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1529" fontId="910" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="911" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="912" fillId="1532" borderId="1817" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="913" fillId="1523" borderId="1821" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="914" fillId="1535" borderId="1825" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="915" fillId="1535" borderId="1825" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="916" fillId="1526" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="917" fillId="1538" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="918" fillId="1526" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="919" fillId="1541" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="911" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1817" fillId="1532" fontId="912" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1821" fillId="1523" fontId="913" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1825" fillId="1535" fontId="914" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1825" fillId="1535" fontId="915" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1526" fontId="916" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1538" fontId="917" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1526" fontId="918" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1541" fontId="919" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1833" fillId="1544" fontId="920" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="921" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1837" fillId="1547" fontId="922" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1841" fillId="1550" fontId="923" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1845" fillId="1553" fontId="924" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="925" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1556" fontId="926" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="927" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1849" fillId="1559" fontId="928" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1853" fillId="1550" fontId="929" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1857" fillId="1562" fontId="930" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1857" fillId="1562" fontId="931" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1553" fontId="932" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1565" fontId="933" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1553" fontId="934" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1568" fontId="935" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="936" fillId="1571" borderId="1865" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="937" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="938" fillId="1574" borderId="1869" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="939" fillId="1577" borderId="1873" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="940" fillId="1580" borderId="1877" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="941" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="942" fillId="1583" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="943" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="944" fillId="1586" borderId="1881" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="945" fillId="1577" borderId="1885" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="946" fillId="1589" borderId="1889" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="947" fillId="1589" borderId="1889" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="948" fillId="1580" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="949" fillId="1592" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="950" fillId="1580" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="951" fillId="1595" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
minor fixes for Nexial Interactive
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -15,7 +15,7 @@
     <definedName name="aws.s3">'#system'!$B$2:$B$9</definedName>
     <definedName name="aws.ses">'#system'!$C$2:$C$3</definedName>
     <definedName name="aws.sqs">'#system'!$D$2:$D$6</definedName>
-    <definedName name="base">'#system'!$F$2:$F$39</definedName>
+    <definedName name="base">'#system'!$F$2:$F$40</definedName>
     <definedName name="csv">'#system'!$G$2:$G$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33440" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35684" uniqueCount="545">
   <si>
     <t>description</t>
   </si>
@@ -1695,6 +1695,9 @@
   </si>
   <si>
     <t>assertTextNotContain(locator,text)</t>
+  </si>
+  <si>
+    <t>clear(variables)</t>
   </si>
 </sst>
 </file>
@@ -1702,7 +1705,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="952" x14ac:knownFonts="1">
+  <fonts count="1016" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7715,8 +7718,412 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1596">
+  <fills count="1704">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -16756,8 +17163,620 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1890">
+  <borders count="2018">
     <border>
       <left/>
       <right/>
@@ -16779,6 +17798,1310 @@
         <color theme="2" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
     </border>
     <border>
       <top style="thin"/>
@@ -36020,7 +38343,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="965">
+  <cellXfs count="1029">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -38874,52 +41197,244 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1568" fontId="935" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="936" fillId="1571" borderId="1865" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="937" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1865" fillId="1571" fontId="936" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="937" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="938" fillId="1574" borderId="1869" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1869" fillId="1574" fontId="938" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="939" fillId="1577" borderId="1873" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1873" fillId="1577" fontId="939" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="940" fillId="1580" borderId="1877" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1877" fillId="1580" fontId="940" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="941" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="941" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="942" fillId="1583" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1583" fontId="942" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="943" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="944" fillId="1586" borderId="1881" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="945" fillId="1577" borderId="1885" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="946" fillId="1589" borderId="1889" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="947" fillId="1589" borderId="1889" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="948" fillId="1580" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="949" fillId="1592" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="950" fillId="1580" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="951" fillId="1595" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="943" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1881" fillId="1586" fontId="944" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1885" fillId="1577" fontId="945" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1889" fillId="1589" fontId="946" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1889" fillId="1589" fontId="947" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1580" fontId="948" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1592" fontId="949" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1580" fontId="950" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1595" fontId="951" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1897" fillId="1598" fontId="952" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="953" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1901" fillId="1601" fontId="954" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1905" fillId="1604" fontId="955" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1909" fillId="1607" fontId="956" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="957" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1610" fontId="958" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="959" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1913" fillId="1613" fontId="960" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1917" fillId="1604" fontId="961" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1921" fillId="1616" fontId="962" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1921" fillId="1616" fontId="963" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1607" fontId="964" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1619" fontId="965" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1607" fontId="966" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1622" fontId="967" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1929" fillId="1625" fontId="968" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="969" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1933" fillId="1628" fontId="970" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1937" fillId="1631" fontId="971" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1941" fillId="1634" fontId="972" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="973" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1637" fontId="974" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="975" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1945" fillId="1640" fontId="976" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1949" fillId="1631" fontId="977" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1953" fillId="1643" fontId="978" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1953" fillId="1643" fontId="979" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1634" fontId="980" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1646" fontId="981" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1634" fontId="982" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1649" fontId="983" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1961" fillId="1652" fontId="984" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="985" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1965" fillId="1655" fontId="986" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1969" fillId="1658" fontId="987" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1973" fillId="1661" fontId="988" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="989" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1664" fontId="990" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="991" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1977" fillId="1667" fontId="992" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1981" fillId="1658" fontId="993" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1985" fillId="1670" fontId="994" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1985" fillId="1670" fontId="995" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1661" fontId="996" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1673" fontId="997" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1661" fontId="998" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1676" fontId="999" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1000" fillId="1679" borderId="1993" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1001" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1002" fillId="1682" borderId="1997" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1003" fillId="1685" borderId="2001" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1004" fillId="1688" borderId="2005" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1005" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1006" fillId="1691" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1007" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1008" fillId="1694" borderId="2009" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1009" fillId="1685" borderId="2013" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1010" fillId="1697" borderId="2017" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1011" fillId="1697" borderId="2017" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1012" fillId="1688" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1013" fillId="1700" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1014" fillId="1688" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1015" fillId="1703" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -40174,7 +42689,7 @@
         <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>402</v>
+        <v>544</v>
       </c>
       <c r="H18" t="s">
         <v>80</v>
@@ -40197,7 +42712,7 @@
         <v>227</v>
       </c>
       <c r="F19" t="s">
-        <v>51</v>
+        <v>402</v>
       </c>
       <c r="H19" t="s">
         <v>81</v>
@@ -40217,7 +42732,7 @@
         <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H20" t="s">
         <v>286</v>
@@ -40237,7 +42752,7 @@
         <v>383</v>
       </c>
       <c r="F21" t="s">
-        <v>525</v>
+        <v>52</v>
       </c>
       <c r="H21" t="s">
         <v>287</v>
@@ -40257,7 +42772,7 @@
         <v>399</v>
       </c>
       <c r="F22" t="s">
-        <v>53</v>
+        <v>525</v>
       </c>
       <c r="H22" t="s">
         <v>288</v>
@@ -40277,7 +42792,7 @@
         <v>400</v>
       </c>
       <c r="F23" t="s">
-        <v>311</v>
+        <v>53</v>
       </c>
       <c r="H23" t="s">
         <v>289</v>
@@ -40297,7 +42812,7 @@
         <v>346</v>
       </c>
       <c r="F24" t="s">
-        <v>54</v>
+        <v>311</v>
       </c>
       <c r="H24" t="s">
         <v>280</v>
@@ -40317,7 +42832,7 @@
         <v>384</v>
       </c>
       <c r="F25" t="s">
-        <v>436</v>
+        <v>54</v>
       </c>
       <c r="H25" t="s">
         <v>269</v>
@@ -40337,7 +42852,7 @@
         <v>45</v>
       </c>
       <c r="F26" t="s">
-        <v>213</v>
+        <v>436</v>
       </c>
       <c r="H26" t="s">
         <v>67</v>
@@ -40357,7 +42872,7 @@
         <v>46</v>
       </c>
       <c r="F27" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H27" t="s">
         <v>272</v>
@@ -40377,7 +42892,7 @@
         <v>47</v>
       </c>
       <c r="F28" t="s">
-        <v>456</v>
+        <v>214</v>
       </c>
       <c r="H28" t="s">
         <v>256</v>
@@ -40394,7 +42909,7 @@
         <v>48</v>
       </c>
       <c r="F29" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H29" t="s">
         <v>273</v>
@@ -40411,7 +42926,7 @@
         <v>401</v>
       </c>
       <c r="F30" t="s">
-        <v>403</v>
+        <v>457</v>
       </c>
       <c r="H30" t="s">
         <v>274</v>
@@ -40425,7 +42940,7 @@
         <v>215</v>
       </c>
       <c r="F31" t="s">
-        <v>55</v>
+        <v>403</v>
       </c>
       <c r="H31" t="s">
         <v>205</v>
@@ -40436,7 +42951,7 @@
     </row>
     <row r="32">
       <c r="F32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H32" t="s">
         <v>265</v>
@@ -40447,7 +42962,7 @@
     </row>
     <row r="33">
       <c r="F33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H33" t="s">
         <v>275</v>
@@ -40458,7 +42973,7 @@
     </row>
     <row r="34">
       <c r="F34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H34" t="s">
         <v>496</v>
@@ -40469,7 +42984,7 @@
     </row>
     <row r="35">
       <c r="F35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H35" t="s">
         <v>250</v>
@@ -40480,7 +42995,7 @@
     </row>
     <row r="36">
       <c r="F36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H36" t="s">
         <v>320</v>
@@ -40491,7 +43006,7 @@
     </row>
     <row r="37">
       <c r="F37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H37" t="s">
         <v>297</v>
@@ -40502,7 +43017,7 @@
     </row>
     <row r="38">
       <c r="F38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H38" t="s">
         <v>251</v>
@@ -40512,6 +43027,9 @@
       </c>
     </row>
     <row r="39">
+      <c r="F39" t="s">
+        <v>62</v>
+      </c>
       <c r="H39" t="s">
         <v>298</v>
       </c>

</xml_diff>

<commit_message>
[fixes] - fixed code to support the creation and changes to System variables that are related to email notification during   execution. Previous code only read in these System variables the start of an execution. The impacted System variables   are namely `nexial.mailHeader`, `nexial.mailFooter`, `nexial.mailSubject`, `nexial.mailTo`, `nexial.enableEmail`.
[expression]
- [CSV &raquo; `removeRows(conditions)`]: now supports the removal of one or more rows based on row index. Note that row index is 0-based and for CSV that is parsed with `header=true`, row 0 is the row *AFTER* the header.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35684" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37367" uniqueCount="545">
   <si>
     <t>description</t>
   </si>
@@ -1705,7 +1705,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1016" x14ac:knownFonts="1">
+  <fonts count="1064" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -8122,8 +8122,311 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1704">
+  <fills count="1785">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -17775,8 +18078,467 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2018">
+  <borders count="2114">
     <border>
       <left/>
       <right/>
@@ -17798,6 +18560,984 @@
         <color theme="2" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
     </border>
     <border>
       <top style="thin"/>
@@ -38343,7 +40083,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1029">
+  <cellXfs count="1077">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -41389,52 +43129,196 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="1676" fontId="999" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1000" fillId="1679" borderId="1993" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1001" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1993" fillId="1679" fontId="1000" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1001" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1002" fillId="1682" borderId="1997" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="1997" fillId="1682" fontId="1002" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1003" fillId="1685" borderId="2001" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2001" fillId="1685" fontId="1003" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1004" fillId="1688" borderId="2005" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2005" fillId="1688" fontId="1004" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1005" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1005" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1006" fillId="1691" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1691" fontId="1006" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1007" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1008" fillId="1694" borderId="2009" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1009" fillId="1685" borderId="2013" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1010" fillId="1697" borderId="2017" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1011" fillId="1697" borderId="2017" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1012" fillId="1688" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1013" fillId="1700" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1014" fillId="1688" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1015" fillId="1703" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1007" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2009" fillId="1694" fontId="1008" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2013" fillId="1685" fontId="1009" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2017" fillId="1697" fontId="1010" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2017" fillId="1697" fontId="1011" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1688" fontId="1012" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1700" fontId="1013" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1688" fontId="1014" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1703" fontId="1015" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2025" fillId="1706" fontId="1016" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1017" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2029" fillId="1709" fontId="1018" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2033" fillId="1712" fontId="1019" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2037" fillId="1715" fontId="1020" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1021" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1718" fontId="1022" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1023" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2041" fillId="1721" fontId="1024" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2045" fillId="1712" fontId="1025" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2049" fillId="1724" fontId="1026" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2049" fillId="1724" fontId="1027" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1715" fontId="1028" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1727" fontId="1029" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1715" fontId="1030" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1730" fontId="1031" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2057" fillId="1733" fontId="1032" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1033" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2061" fillId="1736" fontId="1034" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2065" fillId="1739" fontId="1035" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2069" fillId="1742" fontId="1036" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1037" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1745" fontId="1038" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1039" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2073" fillId="1748" fontId="1040" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2077" fillId="1739" fontId="1041" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2081" fillId="1751" fontId="1042" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2081" fillId="1751" fontId="1043" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1742" fontId="1044" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1754" fontId="1045" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1742" fontId="1046" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="1757" fontId="1047" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1048" fillId="1760" borderId="2089" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1049" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1050" fillId="1763" borderId="2093" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1051" fillId="1766" borderId="2097" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1052" fillId="1769" borderId="2101" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1053" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1054" fillId="1772" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1055" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1056" fillId="1775" borderId="2105" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1057" fillId="1766" borderId="2109" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1058" fillId="1778" borderId="2113" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1059" fillId="1778" borderId="2113" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1060" fillId="1769" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1061" fillId="1781" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1062" fillId="1769" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1063" fillId="1784" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[expression] - [CSV expression]: fix issue dealing with content that contains delimiter or double quotes. - [CSV >> `parse(config)`]: **NEW** config - `keepQuote` - to keep or remove quote after parsing. This only apply to column values where the quote is not needed (such as those without delimiter).
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44099" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44660" uniqueCount="546">
   <si>
     <t>description</t>
   </si>
@@ -1708,7 +1708,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1256" x14ac:knownFonts="1">
+  <fonts count="1272" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -9640,8 +9640,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="2109">
+  <fills count="2136">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -21588,8 +21689,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2498">
+  <borders count="2530">
     <border>
       <left/>
       <right/>
@@ -21611,6 +21865,332 @@
         <color theme="2" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
     </border>
     <border>
       <top style="thin"/>
@@ -47046,7 +47626,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1269">
+  <cellXfs count="1285">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -50812,52 +51392,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="2081" fontId="1239" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1240" fillId="2084" borderId="2473" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1241" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2473" fillId="2084" fontId="1240" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1241" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1242" fillId="2087" borderId="2477" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2477" fillId="2087" fontId="1242" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1243" fillId="2090" borderId="2481" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2481" fillId="2090" fontId="1243" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1244" fillId="2093" borderId="2485" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2485" fillId="2093" fontId="1244" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1245" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1245" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1246" fillId="2096" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2096" fontId="1246" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1247" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1248" fillId="2099" borderId="2489" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1249" fillId="2090" borderId="2493" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1250" fillId="2102" borderId="2497" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1251" fillId="2102" borderId="2497" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1252" fillId="2093" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1253" fillId="2105" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1254" fillId="2093" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1255" fillId="2108" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1247" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2489" fillId="2099" fontId="1248" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2493" fillId="2090" fontId="1249" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2497" fillId="2102" fontId="1250" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2497" fillId="2102" fontId="1251" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2093" fontId="1252" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2105" fontId="1253" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2093" fontId="1254" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2108" fontId="1255" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1256" fillId="2111" borderId="2505" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1257" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1258" fillId="2114" borderId="2509" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1259" fillId="2117" borderId="2513" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1260" fillId="2120" borderId="2517" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1261" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1262" fillId="2123" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1263" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1264" fillId="2126" borderId="2521" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1265" fillId="2117" borderId="2525" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1266" fillId="2129" borderId="2529" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1267" fillId="2129" borderId="2529" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1268" fillId="2120" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1269" fillId="2132" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1270" fillId="2120" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1271" fillId="2135" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[io] - [`assertPath(path)`]: This command asserts that path exists and is readable by the run-user of the execution.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48026" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48587" uniqueCount="548">
   <si>
     <t>description</t>
   </si>
@@ -1714,7 +1714,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1368" x14ac:knownFonts="1">
+  <fonts count="1384" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -10353,8 +10353,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="2298">
+  <fills count="2325">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -23372,8 +23473,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2722">
+  <borders count="2754">
     <border>
       <left/>
       <right/>
@@ -23395,6 +23649,332 @@
         <color theme="2" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
     </border>
     <border>
       <top style="thin"/>
@@ -51112,7 +51692,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1381">
+  <cellXfs count="1397">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -55214,52 +55794,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="2270" fontId="1351" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1352" fillId="2273" borderId="2697" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1353" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2697" fillId="2273" fontId="1352" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1353" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1354" fillId="2276" borderId="2701" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2701" fillId="2276" fontId="1354" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1355" fillId="2279" borderId="2705" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2705" fillId="2279" fontId="1355" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1356" fillId="2282" borderId="2709" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2709" fillId="2282" fontId="1356" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1357" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1357" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1358" fillId="2285" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2285" fontId="1358" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1359" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1360" fillId="2288" borderId="2713" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1361" fillId="2279" borderId="2717" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1362" fillId="2291" borderId="2721" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1363" fillId="2291" borderId="2721" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1364" fillId="2282" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1365" fillId="2294" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1366" fillId="2282" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1367" fillId="2297" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1359" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2713" fillId="2288" fontId="1360" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2717" fillId="2279" fontId="1361" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2721" fillId="2291" fontId="1362" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2721" fillId="2291" fontId="1363" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2282" fontId="1364" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2294" fontId="1365" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2282" fontId="1366" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2297" fontId="1367" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1368" fillId="2300" borderId="2729" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1369" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1370" fillId="2303" borderId="2733" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1371" fillId="2306" borderId="2737" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1372" fillId="2309" borderId="2741" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1373" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1374" fillId="2312" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1375" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1376" fillId="2315" borderId="2745" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1377" fillId="2306" borderId="2749" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1378" fillId="2318" borderId="2753" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1379" fillId="2318" borderId="2753" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1380" fillId="2309" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1381" fillId="2321" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1382" fillId="2309" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1383" fillId="2324" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
- update docs for Browser Performance Metrics - minor code fix
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -23,7 +23,7 @@
     <definedName name="excel">'#system'!$I$2:$I$14</definedName>
     <definedName name="external">'#system'!$J$2:$J$5</definedName>
     <definedName name="image">'#system'!$K$2:$K$7</definedName>
-    <definedName name="io">'#system'!$L$2:$L$29</definedName>
+    <definedName name="io">'#system'!$L$2:$L$30</definedName>
     <definedName name="jms">'#system'!$M$2:$M$4</definedName>
     <definedName name="json">'#system'!$N$2:$N$18</definedName>
     <definedName name="localdb">'#system'!$O$2:$O$12</definedName>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48587" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49149" uniqueCount="549">
   <si>
     <t>description</t>
   </si>
@@ -1708,13 +1708,16 @@
   <si>
     <t>assertAttributeContain(locator,attrName,contains)</t>
   </si>
+  <si>
+    <t>assertPath(path)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1384" x14ac:knownFonts="1">
+  <fonts count="1400" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -10454,8 +10457,109 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="2325">
+  <fills count="2352">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -23626,8 +23730,161 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2754">
+  <borders count="2786">
     <border>
       <left/>
       <right/>
@@ -23649,6 +23906,332 @@
         <color theme="2" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
     </border>
     <border>
       <top style="thin"/>
@@ -51692,7 +52275,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1397">
+  <cellXfs count="1413">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -55842,52 +56425,100 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="2297" fontId="1367" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1368" fillId="2300" borderId="2729" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1369" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2729" fillId="2300" fontId="1368" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1369" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1370" fillId="2303" borderId="2733" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2733" fillId="2303" fontId="1370" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1371" fillId="2306" borderId="2737" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2737" fillId="2306" fontId="1371" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1372" fillId="2309" borderId="2741" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2741" fillId="2309" fontId="1372" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1373" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1373" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1374" fillId="2312" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2312" fontId="1374" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1375" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1376" fillId="2315" borderId="2745" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1377" fillId="2306" borderId="2749" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1378" fillId="2318" borderId="2753" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1379" fillId="2318" borderId="2753" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1380" fillId="2309" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1381" fillId="2321" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1382" fillId="2309" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1383" fillId="2324" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1375" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2745" fillId="2315" fontId="1376" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2749" fillId="2306" fontId="1377" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2753" fillId="2318" fontId="1378" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2753" fillId="2318" fontId="1379" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2309" fontId="1380" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2321" fontId="1381" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2309" fontId="1382" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2324" fontId="1383" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1384" fillId="2327" borderId="2761" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1385" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1386" fillId="2330" borderId="2765" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1387" fillId="2333" borderId="2769" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1388" fillId="2336" borderId="2773" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1389" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1390" fillId="2339" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1391" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1392" fillId="2342" borderId="2777" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1393" fillId="2333" borderId="2781" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1394" fillId="2345" borderId="2785" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1395" fillId="2345" borderId="2785" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1396" fillId="2336" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1397" fillId="2348" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1398" fillId="2336" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1399" fillId="2351" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -56499,7 +57130,7 @@
         <v>340</v>
       </c>
       <c r="L4" t="s">
-        <v>226</v>
+        <v>548</v>
       </c>
       <c r="M4" t="s">
         <v>325</v>
@@ -56582,7 +57213,7 @@
         <v>341</v>
       </c>
       <c r="L5" t="s">
-        <v>449</v>
+        <v>226</v>
       </c>
       <c r="N5" t="s">
         <v>78</v>
@@ -56653,7 +57284,7 @@
         <v>338</v>
       </c>
       <c r="L6" t="s">
-        <v>63</v>
+        <v>449</v>
       </c>
       <c r="N6" t="s">
         <v>21</v>
@@ -56715,7 +57346,7 @@
         <v>522</v>
       </c>
       <c r="L7" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="N7" t="s">
         <v>305</v>
@@ -56774,7 +57405,7 @@
         <v>318</v>
       </c>
       <c r="L8" t="s">
-        <v>472</v>
+        <v>12</v>
       </c>
       <c r="N8" t="s">
         <v>26</v>
@@ -56830,7 +57461,7 @@
         <v>319</v>
       </c>
       <c r="L9" t="s">
-        <v>71</v>
+        <v>472</v>
       </c>
       <c r="N9" t="s">
         <v>27</v>
@@ -56874,7 +57505,7 @@
         <v>439</v>
       </c>
       <c r="L10" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="N10" t="s">
         <v>28</v>
@@ -56915,7 +57546,7 @@
         <v>312</v>
       </c>
       <c r="L11" t="s">
-        <v>473</v>
+        <v>30</v>
       </c>
       <c r="N11" t="s">
         <v>459</v>
@@ -56953,7 +57584,7 @@
         <v>313</v>
       </c>
       <c r="L12" t="s">
-        <v>379</v>
+        <v>473</v>
       </c>
       <c r="N12" t="s">
         <v>524</v>
@@ -56991,7 +57622,7 @@
         <v>314</v>
       </c>
       <c r="L13" t="s">
-        <v>13</v>
+        <v>379</v>
       </c>
       <c r="N13" t="s">
         <v>423</v>
@@ -57026,7 +57657,7 @@
         <v>315</v>
       </c>
       <c r="L14" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="N14" t="s">
         <v>460</v>
@@ -57058,7 +57689,7 @@
         <v>254</v>
       </c>
       <c r="L15" t="s">
-        <v>474</v>
+        <v>34</v>
       </c>
       <c r="N15" t="s">
         <v>31</v>
@@ -57090,7 +57721,7 @@
         <v>255</v>
       </c>
       <c r="L16" t="s">
-        <v>72</v>
+        <v>474</v>
       </c>
       <c r="N16" t="s">
         <v>528</v>
@@ -57122,7 +57753,7 @@
         <v>307</v>
       </c>
       <c r="L17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N17" t="s">
         <v>32</v>
@@ -57148,7 +57779,7 @@
         <v>80</v>
       </c>
       <c r="L18" t="s">
-        <v>450</v>
+        <v>73</v>
       </c>
       <c r="N18" t="s">
         <v>35</v>
@@ -57171,7 +57802,7 @@
         <v>81</v>
       </c>
       <c r="L19" t="s">
-        <v>74</v>
+        <v>450</v>
       </c>
       <c r="Z19" t="s">
         <v>96</v>
@@ -57191,7 +57822,7 @@
         <v>286</v>
       </c>
       <c r="L20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Z20" t="s">
         <v>97</v>
@@ -57211,7 +57842,7 @@
         <v>287</v>
       </c>
       <c r="L21" t="s">
-        <v>545</v>
+        <v>75</v>
       </c>
       <c r="Z21" t="s">
         <v>98</v>
@@ -57231,7 +57862,7 @@
         <v>288</v>
       </c>
       <c r="L22" t="s">
-        <v>458</v>
+        <v>545</v>
       </c>
       <c r="Z22" t="s">
         <v>481</v>
@@ -57251,7 +57882,7 @@
         <v>289</v>
       </c>
       <c r="L23" t="s">
-        <v>36</v>
+        <v>458</v>
       </c>
       <c r="Z23" t="s">
         <v>99</v>
@@ -57271,7 +57902,7 @@
         <v>280</v>
       </c>
       <c r="L24" t="s">
-        <v>381</v>
+        <v>36</v>
       </c>
       <c r="Z24" t="s">
         <v>529</v>
@@ -57291,7 +57922,7 @@
         <v>269</v>
       </c>
       <c r="L25" t="s">
-        <v>511</v>
+        <v>381</v>
       </c>
       <c r="Z25" t="s">
         <v>100</v>
@@ -57311,7 +57942,7 @@
         <v>67</v>
       </c>
       <c r="L26" t="s">
-        <v>76</v>
+        <v>511</v>
       </c>
       <c r="Z26" t="s">
         <v>101</v>
@@ -57331,7 +57962,7 @@
         <v>272</v>
       </c>
       <c r="L27" t="s">
-        <v>421</v>
+        <v>76</v>
       </c>
       <c r="Z27" t="s">
         <v>102</v>
@@ -57351,7 +57982,7 @@
         <v>256</v>
       </c>
       <c r="L28" t="s">
-        <v>37</v>
+        <v>421</v>
       </c>
       <c r="Z28" t="s">
         <v>103</v>
@@ -57368,7 +57999,7 @@
         <v>273</v>
       </c>
       <c r="L29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Z29" t="s">
         <v>317</v>
@@ -57383,6 +58014,9 @@
       </c>
       <c r="H30" t="s">
         <v>274</v>
+      </c>
+      <c r="L30" t="s">
+        <v>38</v>
       </c>
       <c r="Z30" t="s">
         <v>104</v>

</xml_diff>

<commit_message>
[expression] - [JSON &raquo; `compact(removeEmpty)`]: fix code to remove null values.
[json]
- [`compact(var,json,removeEmpty)`]: fix code to remove null values.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49149" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51959" uniqueCount="549">
   <si>
     <t>description</t>
   </si>
@@ -1717,7 +1717,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1400" x14ac:knownFonts="1">
+  <fonts count="1480" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -10558,8 +10558,513 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="2352">
+  <fills count="2487">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -23883,8 +24388,773 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2786">
+  <borders count="2946">
     <border>
       <left/>
       <right/>
@@ -23906,6 +25176,1636 @@
         <color theme="2" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
     </border>
     <border>
       <top style="thin"/>
@@ -52275,7 +55175,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1413">
+  <cellXfs count="1493">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -56473,52 +59373,292 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="2324" fontId="1383" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1384" fillId="2327" borderId="2761" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1385" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2761" fillId="2327" fontId="1384" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1385" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1386" fillId="2330" borderId="2765" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2765" fillId="2330" fontId="1386" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1387" fillId="2333" borderId="2769" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2769" fillId="2333" fontId="1387" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1388" fillId="2336" borderId="2773" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2773" fillId="2336" fontId="1388" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1389" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1389" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1390" fillId="2339" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2339" fontId="1390" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1391" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1392" fillId="2342" borderId="2777" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1393" fillId="2333" borderId="2781" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1394" fillId="2345" borderId="2785" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1395" fillId="2345" borderId="2785" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1396" fillId="2336" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1397" fillId="2348" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1398" fillId="2336" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1399" fillId="2351" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1391" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2777" fillId="2342" fontId="1392" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2781" fillId="2333" fontId="1393" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2785" fillId="2345" fontId="1394" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2785" fillId="2345" fontId="1395" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2336" fontId="1396" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2348" fontId="1397" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2336" fontId="1398" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2351" fontId="1399" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2793" fillId="2354" fontId="1400" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1401" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2797" fillId="2357" fontId="1402" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2801" fillId="2360" fontId="1403" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2805" fillId="2363" fontId="1404" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1405" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2366" fontId="1406" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1407" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2809" fillId="2369" fontId="1408" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2813" fillId="2360" fontId="1409" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2817" fillId="2372" fontId="1410" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2817" fillId="2372" fontId="1411" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2363" fontId="1412" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2375" fontId="1413" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2363" fontId="1414" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2378" fontId="1415" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2825" fillId="2381" fontId="1416" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1417" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2829" fillId="2384" fontId="1418" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2833" fillId="2387" fontId="1419" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2837" fillId="2390" fontId="1420" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1421" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2393" fontId="1422" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1423" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2841" fillId="2396" fontId="1424" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2845" fillId="2387" fontId="1425" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2849" fillId="2399" fontId="1426" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2849" fillId="2399" fontId="1427" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2390" fontId="1428" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2402" fontId="1429" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2390" fontId="1430" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2405" fontId="1431" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2857" fillId="2408" fontId="1432" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1433" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2861" fillId="2411" fontId="1434" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2865" fillId="2414" fontId="1435" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2869" fillId="2417" fontId="1436" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1437" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2420" fontId="1438" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1439" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2873" fillId="2423" fontId="1440" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2877" fillId="2414" fontId="1441" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2881" fillId="2426" fontId="1442" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2881" fillId="2426" fontId="1443" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2417" fontId="1444" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2429" fontId="1445" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2417" fontId="1446" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2432" fontId="1447" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2889" fillId="2435" fontId="1448" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1449" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2893" fillId="2438" fontId="1450" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2897" fillId="2441" fontId="1451" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2901" fillId="2444" fontId="1452" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1453" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2447" fontId="1454" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1455" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2905" fillId="2450" fontId="1456" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2909" fillId="2441" fontId="1457" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2913" fillId="2453" fontId="1458" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2913" fillId="2453" fontId="1459" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2444" fontId="1460" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2456" fontId="1461" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2444" fontId="1462" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2459" fontId="1463" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1464" fillId="2462" borderId="2921" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1465" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1466" fillId="2465" borderId="2925" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1467" fillId="2468" borderId="2929" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1468" fillId="2471" borderId="2933" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1469" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1470" fillId="2474" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1471" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1472" fillId="2477" borderId="2937" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1473" fillId="2468" borderId="2941" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1474" fillId="2480" borderId="2945" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1475" fillId="2480" borderId="2945" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1476" fillId="2471" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1477" fillId="2483" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1478" fillId="2471" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1479" fillId="2486" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[expression] - [JSON >> `pack`]: code fix to enforce JSON beautification after "packing".
[built-in function]
- [`$(execution|plan|name)`]: **NEW** function to reveal the plan file name currently in execution.
- [`$(execution|plan|fullpath)`]: **NEW** function to reveal the fully qualified path for the plan currently in execution.
- [`$(execution|plan|index)`]: **NEW** function to reveal the plan step (i.e. row number) of the plan currently in execution.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52521" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54769" uniqueCount="549">
   <si>
     <t>description</t>
   </si>
@@ -1717,7 +1717,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1496" x14ac:knownFonts="1">
+  <fonts count="1560" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -11164,8 +11164,412 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="2514">
+  <fills count="2622">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -25407,8 +25811,620 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2978">
+  <borders count="3106">
     <border>
       <left/>
       <right/>
@@ -25430,6 +26446,1310 @@
         <color theme="2" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
     </border>
     <border>
       <top style="thin"/>
@@ -55755,7 +58075,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1509">
+  <cellXfs count="1573">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -60241,52 +62561,244 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="2486" fontId="1479" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1480" fillId="2489" borderId="2953" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1481" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2953" fillId="2489" fontId="1480" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1481" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1482" fillId="2492" borderId="2957" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2957" fillId="2492" fontId="1482" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1483" fillId="2495" borderId="2961" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2961" fillId="2495" fontId="1483" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1484" fillId="2498" borderId="2965" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2965" fillId="2498" fontId="1484" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1485" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1485" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1486" fillId="2501" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2501" fontId="1486" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1487" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1488" fillId="2504" borderId="2969" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1489" fillId="2495" borderId="2973" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1490" fillId="2507" borderId="2977" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1491" fillId="2507" borderId="2977" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1492" fillId="2498" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1493" fillId="2510" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1494" fillId="2498" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1495" fillId="2513" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1487" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2969" fillId="2504" fontId="1488" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2973" fillId="2495" fontId="1489" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2977" fillId="2507" fontId="1490" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2977" fillId="2507" fontId="1491" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2498" fontId="1492" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2510" fontId="1493" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2498" fontId="1494" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2513" fontId="1495" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2985" fillId="2516" fontId="1496" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1497" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2989" fillId="2519" fontId="1498" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2993" fillId="2522" fontId="1499" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="2997" fillId="2525" fontId="1500" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1501" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2528" fontId="1502" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1503" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3001" fillId="2531" fontId="1504" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3005" fillId="2522" fontId="1505" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3009" fillId="2534" fontId="1506" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3009" fillId="2534" fontId="1507" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2525" fontId="1508" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2537" fontId="1509" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2525" fontId="1510" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2540" fontId="1511" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3017" fillId="2543" fontId="1512" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1513" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3021" fillId="2546" fontId="1514" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3025" fillId="2549" fontId="1515" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3029" fillId="2552" fontId="1516" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1517" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2555" fontId="1518" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1519" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3033" fillId="2558" fontId="1520" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3037" fillId="2549" fontId="1521" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3041" fillId="2561" fontId="1522" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3041" fillId="2561" fontId="1523" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2552" fontId="1524" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2564" fontId="1525" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2552" fontId="1526" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2567" fontId="1527" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3049" fillId="2570" fontId="1528" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1529" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3053" fillId="2573" fontId="1530" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3057" fillId="2576" fontId="1531" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3061" fillId="2579" fontId="1532" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1533" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2582" fontId="1534" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1535" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3065" fillId="2585" fontId="1536" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3069" fillId="2576" fontId="1537" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3073" fillId="2588" fontId="1538" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3073" fillId="2588" fontId="1539" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2579" fontId="1540" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2591" fontId="1541" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2579" fontId="1542" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2594" fontId="1543" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1544" fillId="2597" borderId="3081" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1545" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1546" fillId="2600" borderId="3085" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1547" fillId="2603" borderId="3089" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1548" fillId="2606" borderId="3093" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1549" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1550" fillId="2609" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1551" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1552" fillId="2612" borderId="3097" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1553" fillId="2603" borderId="3101" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1554" fillId="2615" borderId="3105" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1555" fillId="2615" borderId="3105" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1556" fillId="2606" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1557" fillId="2618" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1558" fillId="2606" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1559" fillId="2621" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[base] - [`repeatUntil(steps,maxWaitMs)`]: add console output when exception is thrown.
[web]
- [`nexial.browser.userData`]: **NEW** System variable to specify browser profile directory.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -42,7 +42,7 @@
     <definedName name="step">'#system'!$Y$2:$Y$4</definedName>
     <definedName name="target">'#system'!$A$2:$A$31</definedName>
     <definedName name="text">'#system'!$Y$2:$Y$2</definedName>
-    <definedName name="web">'#system'!$Z$2:$Z$135</definedName>
+    <definedName name="web">'#system'!$Z$2:$Z$137</definedName>
     <definedName name="webalert">'#system'!$AA$2:$AA$8</definedName>
     <definedName name="webcookie">'#system'!$AB$2:$AB$8</definedName>
     <definedName name="ws">'#system'!$AC$2:$AC$17</definedName>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54769" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56457" uniqueCount="551">
   <si>
     <t>description</t>
   </si>
@@ -1711,13 +1711,19 @@
   <si>
     <t>assertPath(path)</t>
   </si>
+  <si>
+    <t>saveSelectedText(var,locator)</t>
+  </si>
+  <si>
+    <t>saveSelectedValue(var,locator)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1560" x14ac:knownFonts="1">
+  <fonts count="1608" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -11568,8 +11574,311 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="2622">
+  <fills count="2703">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -26423,8 +26732,467 @@
         <bgColor rgb="E6E6E6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF"/>
+        <bgColor rgb="FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3106">
+  <borders count="3202">
     <border>
       <left/>
       <right/>
@@ -26446,6 +27214,984 @@
         <color theme="2" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C8B4B4"/>
+      </left>
+      <right style="thin">
+        <color rgb="C8B4B4"/>
+      </right>
+      <top style="thin">
+        <color rgb="C8B4B4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C8B4B4"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="BEC8CD"/>
+      </left>
+      <right style="thin">
+        <color rgb="BEC8CD"/>
+      </right>
+      <top style="thin">
+        <color rgb="BEC8CD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="BEC8CD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDC3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDC3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDC3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDC3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDC3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDC3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDC3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDC3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DCDCDC"/>
+      </left>
+      <right style="thin">
+        <color rgb="DCDCDC"/>
+      </right>
+      <top style="thin">
+        <color rgb="DCDCDC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DCDCDC"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="CDCDCD"/>
+      </left>
+      <right style="thin">
+        <color rgb="CDCDCD"/>
+      </right>
+      <top style="thin">
+        <color rgb="CDCDCD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="CDCDCD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="C3C3C3"/>
+      </left>
+      <right style="thin">
+        <color rgb="C3C3C3"/>
+      </right>
+      <top style="thin">
+        <color rgb="C3C3C3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="C3C3C3"/>
+      </bottom>
     </border>
     <border>
       <top style="thin"/>
@@ -58075,7 +59821,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1573">
+  <cellXfs count="1621">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -62753,52 +64499,196 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="2594" fontId="1543" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1544" fillId="2597" borderId="3081" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1545" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3081" fillId="2597" fontId="1544" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1545" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1546" fillId="2600" borderId="3085" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3085" fillId="2600" fontId="1546" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1547" fillId="2603" borderId="3089" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3089" fillId="2603" fontId="1547" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1548" fillId="2606" borderId="3093" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3093" fillId="2606" fontId="1548" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1549" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1549" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1550" fillId="2609" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2609" fontId="1550" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1551" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1552" fillId="2612" borderId="3097" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1553" fillId="2603" borderId="3101" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1554" fillId="2615" borderId="3105" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1555" fillId="2615" borderId="3105" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1556" fillId="2606" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1557" fillId="2618" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1558" fillId="2606" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1559" fillId="2621" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1551" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3097" fillId="2612" fontId="1552" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3101" fillId="2603" fontId="1553" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3105" fillId="2615" fontId="1554" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3105" fillId="2615" fontId="1555" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2606" fontId="1556" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2618" fontId="1557" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2606" fontId="1558" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2621" fontId="1559" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3113" fillId="2624" fontId="1560" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1561" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3117" fillId="2627" fontId="1562" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3121" fillId="2630" fontId="1563" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3125" fillId="2633" fontId="1564" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1565" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2636" fontId="1566" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1567" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3129" fillId="2639" fontId="1568" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3133" fillId="2630" fontId="1569" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3137" fillId="2642" fontId="1570" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3137" fillId="2642" fontId="1571" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2633" fontId="1572" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2645" fontId="1573" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2633" fontId="1574" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2648" fontId="1575" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3145" fillId="2651" fontId="1576" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1577" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3149" fillId="2654" fontId="1578" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3153" fillId="2657" fontId="1579" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3157" fillId="2660" fontId="1580" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1581" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2663" fontId="1582" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="1583" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3161" fillId="2666" fontId="1584" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3165" fillId="2657" fontId="1585" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3169" fillId="2669" fontId="1586" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="3169" fillId="2669" fontId="1587" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2660" fontId="1588" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2672" fontId="1589" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2660" fontId="1590" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="2675" fontId="1591" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1592" fillId="2678" borderId="3177" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1593" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1594" fillId="2681" borderId="3181" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1595" fillId="2684" borderId="3185" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1596" fillId="2687" borderId="3189" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1597" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1598" fillId="2690" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1599" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1600" fillId="2693" borderId="3193" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1601" fillId="2684" borderId="3197" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1602" fillId="2696" borderId="3201" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1603" fillId="2696" borderId="3201" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1604" fillId="2687" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1605" fillId="2699" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1606" fillId="2687" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1607" fillId="2702" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -63096,7 +64986,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF135"/>
+  <dimension ref="A1:AF137"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -64878,186 +66768,196 @@
     </row>
     <row r="99">
       <c r="Z99" t="s">
-        <v>430</v>
+        <v>549</v>
       </c>
     </row>
     <row r="100">
       <c r="Z100" t="s">
-        <v>193</v>
+        <v>550</v>
       </c>
     </row>
     <row r="101">
       <c r="Z101" t="s">
-        <v>194</v>
+        <v>430</v>
       </c>
     </row>
     <row r="102">
       <c r="Z102" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="103">
       <c r="Z103" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="104">
       <c r="Z104" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
     </row>
     <row r="105">
       <c r="Z105" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="106">
       <c r="Z106" t="s">
-        <v>485</v>
+        <v>211</v>
       </c>
     </row>
     <row r="107">
       <c r="Z107" t="s">
-        <v>540</v>
+        <v>197</v>
       </c>
     </row>
     <row r="108">
       <c r="Z108" t="s">
-        <v>509</v>
+        <v>485</v>
       </c>
     </row>
     <row r="109">
       <c r="Z109" t="s">
-        <v>138</v>
+        <v>540</v>
       </c>
     </row>
     <row r="110">
       <c r="Z110" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="111">
       <c r="Z111" t="s">
-        <v>372</v>
+        <v>138</v>
       </c>
     </row>
     <row r="112">
       <c r="Z112" t="s">
-        <v>139</v>
+        <v>510</v>
       </c>
     </row>
     <row r="113">
       <c r="Z113" t="s">
-        <v>140</v>
+        <v>372</v>
       </c>
     </row>
     <row r="114">
       <c r="Z114" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="115">
       <c r="Z115" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="116">
       <c r="Z116" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="117">
       <c r="Z117" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="118">
       <c r="Z118" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="119">
       <c r="Z119" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="120">
       <c r="Z120" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="121">
       <c r="Z121" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="122">
       <c r="Z122" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="123">
       <c r="Z123" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="124">
       <c r="Z124" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="125">
       <c r="Z125" t="s">
-        <v>431</v>
+        <v>150</v>
       </c>
     </row>
     <row r="126">
       <c r="Z126" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="127">
       <c r="Z127" t="s">
-        <v>531</v>
+        <v>431</v>
       </c>
     </row>
     <row r="128">
       <c r="Z128" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="129">
       <c r="Z129" t="s">
-        <v>154</v>
+        <v>531</v>
       </c>
     </row>
     <row r="130">
       <c r="Z130" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="131">
       <c r="Z131" t="s">
-        <v>39</v>
+        <v>154</v>
       </c>
     </row>
     <row r="132">
       <c r="Z132" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="133">
       <c r="Z133" t="s">
-        <v>157</v>
+        <v>39</v>
       </c>
     </row>
     <row r="134">
       <c r="Z134" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="135">
       <c r="Z135" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="Z136" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="Z137" t="s">
         <v>159</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[improvements] - [`nexial-script-update`]: automatically trim scenario names and activity with leading/trailing whitespaces to avoid execution-time errors.
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4212" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5412" uniqueCount="577">
   <si>
     <t>description</t>
   </si>
@@ -1811,7 +1811,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="110" x14ac:knownFonts="1">
+  <fonts count="144" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2507,8 +2507,222 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="147">
+  <fills count="195">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2519,6 +2733,278 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -3367,7 +3853,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="157">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -3692,55 +4178,157 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="119" fontId="92" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="93" fillId="125" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="125" fontId="93" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="94" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="95" fillId="128" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="128" fontId="95" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="96" fillId="131" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="131" fontId="96" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="97" fillId="134" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="134" fontId="97" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="98" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="99" fillId="137" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="137" fontId="99" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="100" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="101" fillId="140" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="140" fontId="101" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="102" fillId="143" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="143" fontId="102" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="103" fillId="131" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="131" fontId="103" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="104" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="105" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="106" fillId="134" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="134" fontId="106" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="107" fillId="146" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="146" fontId="107" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="108" fillId="134" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="134" fontId="108" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="109" fillId="143" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="143" fontId="109" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="149" fontId="110" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="111" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="152" fontId="112" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="155" fontId="113" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="158" fontId="114" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="115" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="161" fontId="116" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="117" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="164" fontId="118" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="167" fontId="119" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="155" fontId="120" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="121" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="122" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="158" fontId="123" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="170" fontId="124" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="158" fontId="125" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="167" fontId="126" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="127" fillId="173" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="129" fillId="176" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="130" fillId="179" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="131" fillId="182" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="133" fillId="185" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="134" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="135" fillId="188" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="136" fillId="191" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="137" fillId="179" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="138" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="139" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="140" fillId="182" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="141" fillId="194" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="142" fillId="182" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="143" fillId="191" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
update docs minor code update for better message
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5412" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6012" uniqueCount="577">
   <si>
     <t>description</t>
   </si>
@@ -1811,7 +1811,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="144" x14ac:knownFonts="1">
+  <fonts count="161" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2721,8 +2721,115 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="195">
+  <fills count="219">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2733,6 +2840,142 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -3853,7 +4096,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="174">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -4280,55 +4523,106 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="167" fontId="126" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="127" fillId="173" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="173" fontId="127" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="128" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="129" fillId="176" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="176" fontId="129" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="130" fillId="179" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="179" fontId="130" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="131" fillId="182" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="182" fontId="131" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="132" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="132" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="133" fillId="185" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="185" fontId="133" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="134" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="134" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="135" fillId="188" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="188" fontId="135" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="136" fillId="191" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="191" fontId="136" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="137" fillId="179" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="179" fontId="137" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="138" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="138" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="139" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="139" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="140" fillId="182" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="182" fontId="140" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="141" fillId="194" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="194" fontId="141" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="142" fillId="182" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="182" fontId="142" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="143" fillId="191" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="191" fontId="143" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="144" fillId="197" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="145" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="146" fillId="200" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="147" fillId="203" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="148" fillId="206" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="149" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="150" fillId="209" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="151" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="152" fillId="212" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="153" fillId="215" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="154" fillId="203" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="155" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="156" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="157" fillId="206" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="158" fillId="218" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="159" fillId="206" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="160" fillId="215" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[pdf] - [`savePageCount(pdf,var)`]: *NEW* command to extract the page count for a given `pdf` file. - [`split(pdf,saveTo)`]: *NEW* command to split a given `pdf` file into single page PDF files.
[image]
- support OCR for PDF files

Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -29,12 +29,12 @@
     <definedName name="json">'#system'!$N$2:$N$18</definedName>
     <definedName name="localdb">'#system'!$O$2:$O$13</definedName>
     <definedName name="macro">'#system'!$P$2:$P$4</definedName>
-    <definedName name="mail">'#system'!$Q$2:$Q$4</definedName>
+    <definedName name="mail">'#system'!$Q$2:$Q$5</definedName>
     <definedName name="math">'#system'!$K$2:$K$13</definedName>
     <definedName name="mq">'#system'!$J$2:$J$3</definedName>
     <definedName name="nextgen">'#system'!$K$2:$K$28</definedName>
     <definedName name="number">'#system'!$R$2:$R$16</definedName>
-    <definedName name="pdf">'#system'!$S$2:$S$18</definedName>
+    <definedName name="pdf">'#system'!$S$2:$S$20</definedName>
     <definedName name="rdbms">'#system'!$T$2:$T$9</definedName>
     <definedName name="redis">'#system'!$U$2:$U$10</definedName>
     <definedName name="sms">'#system'!$V$2:$V$2</definedName>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7218" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9032" uniqueCount="586">
   <si>
     <t>description</t>
   </si>
@@ -1816,6 +1816,21 @@
   </si>
   <si>
     <t>send(profile,var)</t>
+  </si>
+  <si>
+    <t>clearComposed(var)</t>
+  </si>
+  <si>
+    <t>compose(var,config,value)</t>
+  </si>
+  <si>
+    <t>sendComposed(profile,var)</t>
+  </si>
+  <si>
+    <t>split(pdf,saveTo)</t>
+  </si>
+  <si>
+    <t>savePageCount(pdf,var)</t>
   </si>
 </sst>
 </file>
@@ -1823,7 +1838,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="195" x14ac:knownFonts="1">
+  <fonts count="246" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3054,8 +3069,329 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="267">
+  <fills count="339">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3066,6 +3402,414 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -4594,7 +5338,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="208">
+  <cellXfs count="259">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -5174,55 +5918,208 @@
     <xf applyFill="true" applyFont="true" borderId="0" fillId="239" fontId="177" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="178" fillId="245" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="245" fontId="178" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="179" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="179" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="180" fillId="248" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="248" fontId="180" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="181" fillId="251" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="251" fontId="181" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="182" fillId="254" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="254" fontId="182" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="183" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="183" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="184" fillId="257" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="257" fontId="184" numFmtId="0" xfId="0">
       <alignment indent="1" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="185" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="185" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="186" fillId="260" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="260" fontId="186" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="187" fillId="263" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="263" fontId="187" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="188" fillId="251" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="251" fontId="188" numFmtId="0" xfId="0">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="189" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="189" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="190" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf applyFont="true" borderId="0" fillId="0" fontId="190" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="191" fillId="254" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="254" fontId="191" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="192" fillId="266" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="266" fontId="192" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="193" fillId="254" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="254" fontId="193" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="194" fillId="263" borderId="0" xfId="0" applyFill="true" applyFont="true">
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="263" fontId="194" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="269" fontId="195" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="196" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="272" fontId="197" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="275" fontId="198" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="278" fontId="199" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="200" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="281" fontId="201" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="202" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="284" fontId="203" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="287" fontId="204" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="275" fontId="205" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="206" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="207" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="278" fontId="208" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="290" fontId="209" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="278" fontId="210" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="287" fontId="211" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="293" fontId="212" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="213" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="296" fontId="214" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="299" fontId="215" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="302" fontId="216" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="217" numFmtId="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="305" fontId="218" numFmtId="0" xfId="0">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="219" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="308" fontId="220" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="311" fontId="221" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="299" fontId="222" numFmtId="0" xfId="0">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="223" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFont="true" borderId="0" fillId="0" fontId="224" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="302" fontId="225" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="314" fontId="226" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="302" fontId="227" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyFill="true" applyFont="true" borderId="0" fillId="311" fontId="228" numFmtId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="229" fillId="317" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="230" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="231" fillId="320" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="232" fillId="323" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="233" fillId="326" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="234" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="235" fillId="329" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="236" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="237" fillId="332" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="238" fillId="335" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="239" fillId="323" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="240" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="241" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="242" fillId="326" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="243" fillId="338" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="244" fillId="326" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="245" fillId="335" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -5677,7 +6574,7 @@
         <v>467</v>
       </c>
       <c r="Q2" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="R2" t="s">
         <v>412</v>
@@ -5772,7 +6669,7 @@
         <v>468</v>
       </c>
       <c r="Q3" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="R3" t="s">
         <v>413</v>
@@ -5861,7 +6758,7 @@
         <v>469</v>
       </c>
       <c r="Q4" t="s">
-        <v>580</v>
+        <v>399</v>
       </c>
       <c r="R4" t="s">
         <v>19</v>
@@ -5943,6 +6840,9 @@
       <c r="O5" t="s">
         <v>493</v>
       </c>
+      <c r="Q5" t="s">
+        <v>583</v>
+      </c>
       <c r="R5" t="s">
         <v>22</v>
       </c>
@@ -6540,7 +7440,7 @@
         <v>35</v>
       </c>
       <c r="S18" t="s">
-        <v>239</v>
+        <v>585</v>
       </c>
       <c r="AA18" t="s">
         <v>66</v>
@@ -6562,6 +7462,9 @@
       <c r="L19" t="s">
         <v>73</v>
       </c>
+      <c r="S19" t="s">
+        <v>239</v>
+      </c>
       <c r="AA19" t="s">
         <v>472</v>
       </c>
@@ -6581,6 +7484,9 @@
       </c>
       <c r="L20" t="s">
         <v>442</v>
+      </c>
+      <c r="S20" t="s">
+        <v>584</v>
       </c>
       <c r="AA20" t="s">
         <v>95</v>

</xml_diff>

<commit_message>
code fix for `macro.produces()` to allow for empty value
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11485" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12102" uniqueCount="599">
   <si>
     <t>description</t>
   </si>
@@ -1878,7 +1878,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="314" x14ac:knownFonts="1">
+  <fonts count="331" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3858,8 +3858,115 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="435">
+  <fills count="459">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3870,6 +3977,142 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -6350,7 +6593,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="327">
+  <cellXfs count="344">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -7336,6 +7579,57 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="313" fillId="431" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="314" fillId="437" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="315" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="316" fillId="440" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="317" fillId="443" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="318" fillId="446" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="319" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="320" fillId="449" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="321" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="322" fillId="452" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="323" fillId="455" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="324" fillId="443" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="325" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="326" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="327" fillId="446" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="328" fillId="458" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="329" fillId="446" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="330" fillId="455" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[fixes] - code fix to improve support on saving array to data variable
[web]
- [`saveTextArray(var,locator)`]: honor the use of `nexial.textDelim`.

Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12102" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13336" uniqueCount="599">
   <si>
     <t>description</t>
   </si>
@@ -1878,7 +1878,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="331" x14ac:knownFonts="1">
+  <fonts count="365" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3965,8 +3965,222 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="459">
+  <fills count="507">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3977,6 +4191,278 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -6593,7 +7079,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="344">
+  <cellXfs count="378">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -7630,6 +8116,108 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="330" fillId="455" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="331" fillId="461" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="332" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="333" fillId="464" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="334" fillId="467" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="335" fillId="470" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="336" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="337" fillId="473" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="338" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="339" fillId="476" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="340" fillId="479" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="341" fillId="467" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="342" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="343" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="344" fillId="470" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="345" fillId="482" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="346" fillId="470" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="347" fillId="479" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="348" fillId="485" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="349" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="350" fillId="488" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="351" fillId="491" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="352" fillId="494" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="353" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="354" fillId="497" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="355" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="356" fillId="500" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="357" fillId="503" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="358" fillId="491" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="359" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="360" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="361" fillId="494" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="362" fillId="506" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="363" fillId="494" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="364" fillId="503" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[expression] - [`[TEXT(...) => repeat(count)]`]: *NEW* repeat current text by number of `times. - [`[LIST(...) => index(item)]`]: support `CONTAIN:` and `REGEX:` prefixes for improved expressiveness.
[tn.5250]
- [`typeOnMatchedColumns(matches,keystrokes)`]: *NEW* command to allow the matching of table row based on multiple columns (each filter separated by new line).
- code fix to support table structure that is prefix with text content.

Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13336" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13953" uniqueCount="599">
   <si>
     <t>description</t>
   </si>
@@ -1878,7 +1878,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="365" x14ac:knownFonts="1">
+  <fonts count="382" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4179,8 +4179,115 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="507">
+  <fills count="531">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4191,6 +4298,142 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -7079,7 +7322,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="378">
+  <cellXfs count="395">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -8218,6 +8461,57 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="364" fillId="503" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="365" fillId="509" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="366" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="367" fillId="512" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="368" fillId="515" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="369" fillId="518" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="370" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="371" fillId="521" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="372" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="373" fillId="524" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="374" fillId="527" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="375" fillId="515" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="376" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="377" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="378" fillId="518" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="379" fillId="530" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="380" fillId="518" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="381" fillId="527" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[tn.5250] - IOOBE when filtering table data
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13953" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14570" uniqueCount="599">
   <si>
     <t>description</t>
   </si>
@@ -1878,7 +1878,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="382" x14ac:knownFonts="1">
+  <fonts count="399" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4286,8 +4286,115 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="531">
+  <fills count="555">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4298,6 +4405,142 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -7322,7 +7565,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="395">
+  <cellXfs count="412">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -8512,6 +8755,57 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="381" fillId="527" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="382" fillId="533" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="383" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="384" fillId="536" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="385" fillId="539" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="386" fillId="542" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="387" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="388" fillId="545" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="389" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="390" fillId="548" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="391" fillId="551" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="392" fillId="539" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="393" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="394" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="395" fillId="542" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="396" fillId="554" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="397" fillId="542" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="398" fillId="551" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[system variables] - [`nexial.io.matchRecursive`]: *NEW* System variable to determine if Nexial should scan recursively the target directory when invoking [io &raquo; `saveMatches(var,path,fileFilter,textFilter)`].
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15187" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16421" uniqueCount="599">
   <si>
     <t>description</t>
   </si>
@@ -1878,7 +1878,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="416" x14ac:knownFonts="1">
+  <fonts count="450" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4500,8 +4500,222 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="579">
+  <fills count="627">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4512,6 +4726,278 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -7808,7 +8294,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="429">
+  <cellXfs count="463">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -9100,6 +9586,108 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="415" fillId="575" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="416" fillId="581" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="417" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="418" fillId="584" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="419" fillId="587" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="420" fillId="590" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="421" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="422" fillId="593" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="423" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="424" fillId="596" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="425" fillId="599" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="426" fillId="587" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="427" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="428" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="429" fillId="590" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="430" fillId="602" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="431" fillId="590" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="432" fillId="599" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="433" fillId="605" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="434" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="435" fillId="608" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="436" fillId="611" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="437" fillId="614" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="438" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="439" fillId="617" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="440" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="441" fillId="620" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="442" fillId="623" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="443" fillId="611" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="444" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="445" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="446" fillId="614" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="447" fillId="626" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="448" fillId="614" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="449" fillId="623" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[function] - [`$(format|phone|text)`]: improvement to accept phone number with non-numeric characters such as `-`, `.`, `(` and `)`.
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16421" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17038" uniqueCount="599">
   <si>
     <t>description</t>
   </si>
@@ -1878,7 +1878,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="450" x14ac:knownFonts="1">
+  <fonts count="467" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4714,8 +4714,115 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="627">
+  <fills count="651">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4726,6 +4833,142 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -8294,7 +8537,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="463">
+  <cellXfs count="480">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -9688,6 +9931,57 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="449" fillId="623" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="450" fillId="629" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="451" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="452" fillId="632" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="453" fillId="635" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="454" fillId="638" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="455" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="456" fillId="641" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="457" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="458" fillId="644" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="459" fillId="647" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="460" fillId="635" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="461" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="462" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="463" fillId="638" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="464" fillId="650" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="465" fillId="638" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="466" fillId="647" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
Revert "[function] - [`$(format|phone|text)`]: improvement to accept phone number with non-numeric characters such as `-`, `.`, `(` and `)`."
This reverts commit 5e4e3ab2

Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17038" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16421" uniqueCount="599">
   <si>
     <t>description</t>
   </si>
@@ -1878,7 +1878,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="467" x14ac:knownFonts="1">
+  <fonts count="450" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -4714,115 +4714,8 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="3E511F"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="287389"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="287389"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="6E6E3C"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="9C0006"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="11.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="5A5A32"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="11.0"/>
-      <color rgb="12284A"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="808080"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="0000FF"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="9C0006"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="006100"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="9C0006"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="808080"/>
-      <u val="none"/>
-    </font>
   </fonts>
-  <fills count="651">
+  <fills count="627">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4833,142 +4726,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="E6EFD7"/>
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="E6EFD7"/>
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="DCE1E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="DCE1E6"/>
-        <bgColor rgb="DCE1E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="DCE1E6"/>
-        <bgColor rgb="DCE1E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="F0F0E1"/>
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="F0F0E1"/>
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFC7CE"/>
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC7CE"/>
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="ECECE8"/>
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="ECECE8"/>
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FAFAFA"/>
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FAFAFA"/>
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="E6E6E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="E6E6E6"/>
-        <bgColor rgb="E6E6E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="E6E6E6"/>
-        <bgColor rgb="E6E6E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="C6EFCE"/>
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="C6EFCE"/>
-        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -8537,7 +8294,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="480">
+  <cellXfs count="463">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -9931,57 +9688,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="449" fillId="623" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="450" fillId="629" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="451" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="452" fillId="632" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment indent="1" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="453" fillId="635" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment indent="1" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="454" fillId="638" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="455" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="456" fillId="641" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment indent="1" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="457" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="458" fillId="644" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="459" fillId="647" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="460" fillId="635" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="461" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="462" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="463" fillId="638" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="464" fillId="650" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="465" fillId="638" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="466" fillId="647" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[ssh] - added additional logging for better RCA
[web]
- [`assertCssPresent(locator,property,value)`]: supports the conversion of HEX color to RGBA form.

Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18889" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20740" uniqueCount="599">
   <si>
     <t>description</t>
   </si>
@@ -1878,7 +1878,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="518" x14ac:knownFonts="1">
+  <fonts count="569" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5142,8 +5142,329 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="723">
+  <fills count="795">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5154,6 +5475,414 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -9266,7 +9995,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="531">
+  <cellXfs count="582">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -10864,6 +11593,159 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="517" fillId="719" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="518" fillId="725" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="519" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="520" fillId="728" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="521" fillId="731" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="522" fillId="734" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="523" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="524" fillId="737" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="525" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="526" fillId="740" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="527" fillId="743" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="528" fillId="731" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="529" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="530" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="531" fillId="734" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="532" fillId="746" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="533" fillId="734" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="534" fillId="743" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="535" fillId="749" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="536" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="537" fillId="752" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="538" fillId="755" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="539" fillId="758" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="540" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="541" fillId="761" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="542" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="543" fillId="764" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="544" fillId="767" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="545" fillId="755" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="546" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="547" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="548" fillId="758" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="549" fillId="770" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="550" fillId="758" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="551" fillId="767" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="552" fillId="773" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="553" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="554" fillId="776" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="555" fillId="779" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="556" fillId="782" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="557" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="558" fillId="785" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="559" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="560" fillId="788" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="561" fillId="791" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="562" fillId="779" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="563" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="564" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="565" fillId="782" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="566" fillId="794" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="567" fillId="782" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="568" fillId="791" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[base] - [`assertMatch(text,regex)`]: now supports PolyMatcher
[macro]
- [`expects(var,default)`]: fixed logic to use default when specified `var` has no value.

[tn.5250]
- [`waitUntilTextPresent(text,maxWaitMs)`]: *NEW* command to wait until specified text is found on current TN5250 screen.
- [`waitUntilTitlePresent(title,maxWaitMs)`]: *NEW* command to wait until specified text is found on current TN5250 screen title.
- [`waitUntilMessagePresent(message,maxWaitMs)`]: *NEW* command to wait until specified text is found on current TN5250 status message.
- [`inspectScreen()`]: add pre-fetch wait time (1.5second) prior to render TN5250 screen data.

Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20740" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21974" uniqueCount="599">
   <si>
     <t>description</t>
   </si>
@@ -1878,7 +1878,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="569" x14ac:knownFonts="1">
+  <fonts count="603" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5463,8 +5463,222 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="795">
+  <fills count="843">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5475,6 +5689,278 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -9995,7 +10481,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="582">
+  <cellXfs count="616">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -11746,6 +12232,108 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="568" fillId="791" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="569" fillId="797" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="570" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="571" fillId="800" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="572" fillId="803" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="573" fillId="806" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="574" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="575" fillId="809" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="576" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="577" fillId="812" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="578" fillId="815" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="579" fillId="803" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="580" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="581" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="582" fillId="806" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="583" fillId="818" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="584" fillId="806" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="585" fillId="815" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="586" fillId="821" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="587" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="588" fillId="824" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="589" fillId="827" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="590" fillId="830" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="591" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="592" fillId="833" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="593" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="594" fillId="836" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="595" fillId="839" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="596" fillId="827" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="597" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="598" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="599" fillId="830" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="600" fillId="842" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="601" fillId="830" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="602" fillId="839" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[expression] - [LIST &raquo; `removeMatch(match)`]: *NEW* operation to remove from a LIT the items that match the specified `match` criteria.
`RegexUtils.natch`: support matching on empty string (with `^$`)

Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -20,8 +20,8 @@
     <definedName name="csv">'#system'!$G$2:$G$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$H$2:$H$98</definedName>
-    <definedName name="excel">'#system'!$I$2:$I$16</definedName>
+    <definedName name="desktop">'#system'!$H$2:$H$100</definedName>
+    <definedName name="excel">'#system'!$I$2:$I$17</definedName>
     <definedName name="external">'#system'!$J$2:$J$7</definedName>
     <definedName name="image">'#system'!$K$2:$K$8</definedName>
     <definedName name="io">'#system'!$L$2:$L$32</definedName>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21974" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22594" uniqueCount="602">
   <si>
     <t>description</t>
   </si>
@@ -1871,6 +1871,15 @@
   </si>
   <si>
     <t>assertNotReadOnly(file)</t>
+  </si>
+  <si>
+    <t>doubleClick(name)</t>
+  </si>
+  <si>
+    <t>doubleClickByLocator(locator)</t>
+  </si>
+  <si>
+    <t>renameSheet(file,worksheet,newName)</t>
   </si>
 </sst>
 </file>
@@ -1878,7 +1887,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="603" x14ac:knownFonts="1">
+  <fonts count="620" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5677,8 +5686,115 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="843">
+  <fills count="867">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5689,6 +5805,142 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -10481,7 +10733,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="616">
+  <cellXfs count="633">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -12334,6 +12586,57 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="602" fillId="839" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="603" fillId="845" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="604" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="605" fillId="848" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="606" fillId="851" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="607" fillId="854" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="608" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="609" fillId="857" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="610" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="611" fillId="860" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="612" fillId="863" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="613" fillId="851" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="614" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="615" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="616" fillId="854" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="617" fillId="866" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="618" fillId="854" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="619" fillId="863" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -13265,7 +13568,7 @@
         <v>351</v>
       </c>
       <c r="I8" t="s">
-        <v>316</v>
+        <v>601</v>
       </c>
       <c r="K8" t="s">
         <v>513</v>
@@ -13330,7 +13633,7 @@
         <v>352</v>
       </c>
       <c r="I9" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L9" t="s">
         <v>12</v>
@@ -13383,7 +13686,7 @@
         <v>294</v>
       </c>
       <c r="I10" t="s">
-        <v>547</v>
+        <v>317</v>
       </c>
       <c r="L10" t="s">
         <v>464</v>
@@ -13427,7 +13730,7 @@
         <v>340</v>
       </c>
       <c r="I11" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="L11" t="s">
         <v>71</v>
@@ -13465,7 +13768,7 @@
         <v>262</v>
       </c>
       <c r="I12" t="s">
-        <v>432</v>
+        <v>548</v>
       </c>
       <c r="L12" t="s">
         <v>30</v>
@@ -13503,7 +13806,7 @@
         <v>251</v>
       </c>
       <c r="I13" t="s">
-        <v>310</v>
+        <v>432</v>
       </c>
       <c r="L13" t="s">
         <v>465</v>
@@ -13541,7 +13844,7 @@
         <v>304</v>
       </c>
       <c r="I14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L14" t="s">
         <v>374</v>
@@ -13576,7 +13879,7 @@
         <v>252</v>
       </c>
       <c r="I15" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L15" t="s">
         <v>13</v>
@@ -13611,7 +13914,7 @@
         <v>253</v>
       </c>
       <c r="I16" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L16" t="s">
         <v>34</v>
@@ -13645,6 +13948,9 @@
       <c r="H17" t="s">
         <v>305</v>
       </c>
+      <c r="I17" t="s">
+        <v>313</v>
+      </c>
       <c r="L17" t="s">
         <v>466</v>
       </c>
@@ -14146,7 +14452,7 @@
     </row>
     <row r="51">
       <c r="H51" t="s">
-        <v>327</v>
+        <v>599</v>
       </c>
       <c r="AA51" t="s">
         <v>555</v>
@@ -14154,7 +14460,7 @@
     </row>
     <row r="52">
       <c r="H52" t="s">
-        <v>353</v>
+        <v>600</v>
       </c>
       <c r="AA52" t="s">
         <v>201</v>
@@ -14162,7 +14468,7 @@
     </row>
     <row r="53">
       <c r="H53" t="s">
-        <v>290</v>
+        <v>327</v>
       </c>
       <c r="AA53" t="s">
         <v>68</v>
@@ -14170,7 +14476,7 @@
     </row>
     <row r="54">
       <c r="H54" t="s">
-        <v>341</v>
+        <v>353</v>
       </c>
       <c r="AA54" t="s">
         <v>514</v>
@@ -14178,7 +14484,7 @@
     </row>
     <row r="55">
       <c r="H55" t="s">
-        <v>319</v>
+        <v>290</v>
       </c>
       <c r="AA55" t="s">
         <v>117</v>
@@ -14186,7 +14492,7 @@
     </row>
     <row r="56">
       <c r="H56" t="s">
-        <v>256</v>
+        <v>341</v>
       </c>
       <c r="AA56" t="s">
         <v>118</v>
@@ -14194,7 +14500,7 @@
     </row>
     <row r="57">
       <c r="H57" t="s">
-        <v>280</v>
+        <v>319</v>
       </c>
       <c r="AA57" t="s">
         <v>119</v>
@@ -14202,7 +14508,7 @@
     </row>
     <row r="58">
       <c r="H58" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
       <c r="AA58" t="s">
         <v>474</v>
@@ -14210,7 +14516,7 @@
     </row>
     <row r="59">
       <c r="H59" t="s">
-        <v>518</v>
+        <v>280</v>
       </c>
       <c r="AA59" t="s">
         <v>443</v>
@@ -14218,7 +14524,7 @@
     </row>
     <row r="60">
       <c r="H60" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AA60" t="s">
         <v>120</v>
@@ -14226,7 +14532,7 @@
     </row>
     <row r="61">
       <c r="H61" t="s">
-        <v>291</v>
+        <v>518</v>
       </c>
       <c r="AA61" t="s">
         <v>334</v>
@@ -14234,7 +14540,7 @@
     </row>
     <row r="62">
       <c r="H62" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="AA62" t="s">
         <v>444</v>
@@ -14242,7 +14548,7 @@
     </row>
     <row r="63">
       <c r="H63" t="s">
-        <v>325</v>
+        <v>291</v>
       </c>
       <c r="AA63" t="s">
         <v>121</v>
@@ -14250,7 +14556,7 @@
     </row>
     <row r="64">
       <c r="H64" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="AA64" t="s">
         <v>122</v>
@@ -14258,7 +14564,7 @@
     </row>
     <row r="65">
       <c r="H65" t="s">
-        <v>298</v>
+        <v>325</v>
       </c>
       <c r="AA65" t="s">
         <v>123</v>
@@ -14266,7 +14572,7 @@
     </row>
     <row r="66">
       <c r="H66" t="s">
-        <v>354</v>
+        <v>297</v>
       </c>
       <c r="AA66" t="s">
         <v>124</v>
@@ -14274,7 +14580,7 @@
     </row>
     <row r="67">
       <c r="H67" t="s">
-        <v>355</v>
+        <v>298</v>
       </c>
       <c r="AA67" t="s">
         <v>125</v>
@@ -14282,7 +14588,7 @@
     </row>
     <row r="68">
       <c r="H68" t="s">
-        <v>333</v>
+        <v>354</v>
       </c>
       <c r="AA68" t="s">
         <v>126</v>
@@ -14290,7 +14596,7 @@
     </row>
     <row r="69">
       <c r="H69" t="s">
-        <v>301</v>
+        <v>355</v>
       </c>
       <c r="AA69" t="s">
         <v>127</v>
@@ -14298,7 +14604,7 @@
     </row>
     <row r="70">
       <c r="H70" t="s">
-        <v>257</v>
+        <v>333</v>
       </c>
       <c r="AA70" t="s">
         <v>421</v>
@@ -14306,7 +14612,7 @@
     </row>
     <row r="71">
       <c r="H71" t="s">
-        <v>504</v>
+        <v>301</v>
       </c>
       <c r="AA71" t="s">
         <v>453</v>
@@ -14314,7 +14620,7 @@
     </row>
     <row r="72">
       <c r="H72" t="s">
-        <v>302</v>
+        <v>257</v>
       </c>
       <c r="AA72" t="s">
         <v>202</v>
@@ -14322,7 +14628,7 @@
     </row>
     <row r="73">
       <c r="H73" t="s">
-        <v>392</v>
+        <v>504</v>
       </c>
       <c r="AA73" t="s">
         <v>373</v>
@@ -14330,7 +14636,7 @@
     </row>
     <row r="74">
       <c r="H74" t="s">
-        <v>292</v>
+        <v>302</v>
       </c>
       <c r="AA74" t="s">
         <v>422</v>
@@ -14338,7 +14644,7 @@
     </row>
     <row r="75">
       <c r="H75" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AA75" t="s">
         <v>128</v>
@@ -14346,7 +14652,7 @@
     </row>
     <row r="76">
       <c r="H76" t="s">
-        <v>250</v>
+        <v>292</v>
       </c>
       <c r="AA76" t="s">
         <v>129</v>
@@ -14354,7 +14660,7 @@
     </row>
     <row r="77">
       <c r="H77" t="s">
-        <v>489</v>
+        <v>393</v>
       </c>
       <c r="AA77" t="s">
         <v>130</v>
@@ -14362,7 +14668,7 @@
     </row>
     <row r="78">
       <c r="H78" t="s">
-        <v>332</v>
+        <v>250</v>
       </c>
       <c r="AA78" t="s">
         <v>131</v>
@@ -14370,7 +14676,7 @@
     </row>
     <row r="79">
       <c r="H79" t="s">
-        <v>268</v>
+        <v>489</v>
       </c>
       <c r="AA79" t="s">
         <v>570</v>
@@ -14378,7 +14684,7 @@
     </row>
     <row r="80">
       <c r="H80" t="s">
-        <v>274</v>
+        <v>332</v>
       </c>
       <c r="AA80" t="s">
         <v>185</v>
@@ -14386,7 +14692,7 @@
     </row>
     <row r="81">
       <c r="H81" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="AA81" t="s">
         <v>186</v>
@@ -14394,7 +14700,7 @@
     </row>
     <row r="82">
       <c r="H82" t="s">
-        <v>411</v>
+        <v>274</v>
       </c>
       <c r="AA82" t="s">
         <v>433</v>
@@ -14402,7 +14708,7 @@
     </row>
     <row r="83">
       <c r="H83" t="s">
-        <v>320</v>
+        <v>279</v>
       </c>
       <c r="AA83" t="s">
         <v>445</v>
@@ -14410,7 +14716,7 @@
     </row>
     <row r="84">
       <c r="H84" t="s">
-        <v>258</v>
+        <v>411</v>
       </c>
       <c r="AA84" t="s">
         <v>132</v>
@@ -14418,7 +14724,7 @@
     </row>
     <row r="85">
       <c r="H85" t="s">
-        <v>269</v>
+        <v>320</v>
       </c>
       <c r="AA85" t="s">
         <v>133</v>
@@ -14426,7 +14732,7 @@
     </row>
     <row r="86">
       <c r="H86" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="AA86" t="s">
         <v>134</v>
@@ -14434,7 +14740,7 @@
     </row>
     <row r="87">
       <c r="H87" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="AA87" t="s">
         <v>475</v>
@@ -14442,7 +14748,7 @@
     </row>
     <row r="88">
       <c r="H88" t="s">
-        <v>506</v>
+        <v>275</v>
       </c>
       <c r="AA88" t="s">
         <v>135</v>
@@ -14450,7 +14756,7 @@
     </row>
     <row r="89">
       <c r="H89" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="AA89" t="s">
         <v>136</v>
@@ -14458,7 +14764,7 @@
     </row>
     <row r="90">
       <c r="H90" t="s">
-        <v>276</v>
+        <v>506</v>
       </c>
       <c r="AA90" t="s">
         <v>187</v>
@@ -14466,7 +14772,7 @@
     </row>
     <row r="91">
       <c r="H91" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AA91" t="s">
         <v>476</v>
@@ -14474,7 +14780,7 @@
     </row>
     <row r="92">
       <c r="H92" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
       <c r="AA92" t="s">
         <v>537</v>
@@ -14482,7 +14788,7 @@
     </row>
     <row r="93">
       <c r="H93" t="s">
-        <v>293</v>
+        <v>260</v>
       </c>
       <c r="AA93" t="s">
         <v>188</v>
@@ -14490,7 +14796,7 @@
     </row>
     <row r="94">
       <c r="H94" t="s">
-        <v>299</v>
+        <v>261</v>
       </c>
       <c r="AA94" t="s">
         <v>434</v>
@@ -14498,7 +14804,7 @@
     </row>
     <row r="95">
       <c r="H95" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="AA95" t="s">
         <v>189</v>
@@ -14506,7 +14812,7 @@
     </row>
     <row r="96">
       <c r="H96" t="s">
-        <v>328</v>
+        <v>299</v>
       </c>
       <c r="AA96" t="s">
         <v>190</v>
@@ -14514,7 +14820,7 @@
     </row>
     <row r="97">
       <c r="H97" t="s">
-        <v>265</v>
+        <v>283</v>
       </c>
       <c r="AA97" t="s">
         <v>524</v>
@@ -14522,18 +14828,24 @@
     </row>
     <row r="98">
       <c r="H98" t="s">
-        <v>266</v>
+        <v>328</v>
       </c>
       <c r="AA98" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="99">
+      <c r="H99" t="s">
+        <v>265</v>
+      </c>
       <c r="AA99" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="100">
+      <c r="H100" t="s">
+        <v>266</v>
+      </c>
       <c r="AA100" t="s">
         <v>137</v>
       </c>

</xml_diff>

<commit_message>
[nexial interactive] - `DESKTOP(xpath) => context(label,label,...)` to trigger context on a desktop element. - `DESKTOP(name) => context(label,label,...)` to trigger context on a desktop element.
[desktop commands]
- [`clickMenuByLocator(locator,menu)`]: *NEW* command to trigger application menu via a `locator`.
- [`contextMenuByLocator(locator,menu)`]: *NEW* command to trigger context menu (i.e. right-click) on a desktop element via `locator`.
- [`contextMenu(name,menu)`]: *NEW* command to trigger context menu (i.e. right-click) on a desktop element via `locator`.
- improved keyboard automation by utilizing Winium's internal "shortcut" script.

- upgrade to Sprint Boot 2.4.2
- upgrade to Kotlin 1.4.21

Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -20,7 +20,7 @@
     <definedName name="csv">'#system'!$G$2:$G$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$H$2:$H$100</definedName>
+    <definedName name="desktop">'#system'!$H$2:$H$105</definedName>
     <definedName name="excel">'#system'!$I$2:$I$17</definedName>
     <definedName name="external">'#system'!$J$2:$J$7</definedName>
     <definedName name="image">'#system'!$K$2:$K$8</definedName>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22594" uniqueCount="602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24459" uniqueCount="607">
   <si>
     <t>description</t>
   </si>
@@ -1880,6 +1880,21 @@
   </si>
   <si>
     <t>renameSheet(file,worksheet,newName)</t>
+  </si>
+  <si>
+    <t>clickMenu(elem,menu)</t>
+  </si>
+  <si>
+    <t>clickMenuByLocator(locator,menu)</t>
+  </si>
+  <si>
+    <t>contextMenu(elem,menu)</t>
+  </si>
+  <si>
+    <t>contextMenu(name,menu)</t>
+  </si>
+  <si>
+    <t>contextMenuByLocator(locator,menu)</t>
   </si>
 </sst>
 </file>
@@ -1887,7 +1902,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="620" x14ac:knownFonts="1">
+  <fonts count="671" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5793,8 +5808,329 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="867">
+  <fills count="939">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5805,6 +6141,414 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -10733,7 +11477,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="633">
+  <cellXfs count="684">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -12637,6 +13381,159 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="619" fillId="863" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="620" fillId="869" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="621" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="622" fillId="872" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="623" fillId="875" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="624" fillId="878" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="625" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="626" fillId="881" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="627" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="628" fillId="884" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="629" fillId="887" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="630" fillId="875" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="631" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="632" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="633" fillId="878" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="634" fillId="890" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="635" fillId="878" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="636" fillId="887" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="637" fillId="893" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="638" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="639" fillId="896" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="640" fillId="899" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="641" fillId="902" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="642" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="643" fillId="905" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="644" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="645" fillId="908" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="646" fillId="911" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="647" fillId="899" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="648" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="649" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="650" fillId="902" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="651" fillId="914" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="652" fillId="902" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="653" fillId="911" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="654" fillId="917" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="655" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="656" fillId="920" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="657" fillId="923" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="658" fillId="926" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="659" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="660" fillId="929" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="661" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="662" fillId="932" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="663" fillId="935" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="664" fillId="923" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="665" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="666" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="667" fillId="926" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="668" fillId="938" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="669" fillId="926" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="670" fillId="935" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -14355,7 +15252,7 @@
         <v>60</v>
       </c>
       <c r="H40" t="s">
-        <v>255</v>
+        <v>602</v>
       </c>
       <c r="AA40" t="s">
         <v>110</v>
@@ -14366,7 +15263,7 @@
         <v>61</v>
       </c>
       <c r="H41" t="s">
-        <v>69</v>
+        <v>255</v>
       </c>
       <c r="AA41" t="s">
         <v>326</v>
@@ -14377,7 +15274,7 @@
         <v>62</v>
       </c>
       <c r="H42" t="s">
-        <v>200</v>
+        <v>603</v>
       </c>
       <c r="AA42" t="s">
         <v>420</v>
@@ -14388,7 +15285,7 @@
         <v>574</v>
       </c>
       <c r="H43" t="s">
-        <v>517</v>
+        <v>69</v>
       </c>
       <c r="AA43" t="s">
         <v>530</v>
@@ -14396,7 +15293,7 @@
     </row>
     <row r="44">
       <c r="H44" t="s">
-        <v>277</v>
+        <v>200</v>
       </c>
       <c r="AA44" t="s">
         <v>377</v>
@@ -14404,7 +15301,7 @@
     </row>
     <row r="45">
       <c r="H45" t="s">
-        <v>288</v>
+        <v>517</v>
       </c>
       <c r="AA45" t="s">
         <v>111</v>
@@ -14412,7 +15309,7 @@
     </row>
     <row r="46">
       <c r="H46" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="AA46" t="s">
         <v>112</v>
@@ -14420,7 +15317,7 @@
     </row>
     <row r="47">
       <c r="H47" t="s">
-        <v>331</v>
+        <v>288</v>
       </c>
       <c r="AA47" t="s">
         <v>113</v>
@@ -14428,7 +15325,7 @@
     </row>
     <row r="48">
       <c r="H48" t="s">
-        <v>330</v>
+        <v>289</v>
       </c>
       <c r="AA48" t="s">
         <v>114</v>
@@ -14436,7 +15333,7 @@
     </row>
     <row r="49">
       <c r="H49" t="s">
-        <v>199</v>
+        <v>331</v>
       </c>
       <c r="AA49" t="s">
         <v>115</v>
@@ -14444,7 +15341,7 @@
     </row>
     <row r="50">
       <c r="H50" t="s">
-        <v>308</v>
+        <v>330</v>
       </c>
       <c r="AA50" t="s">
         <v>116</v>
@@ -14452,7 +15349,7 @@
     </row>
     <row r="51">
       <c r="H51" t="s">
-        <v>599</v>
+        <v>199</v>
       </c>
       <c r="AA51" t="s">
         <v>555</v>
@@ -14460,7 +15357,7 @@
     </row>
     <row r="52">
       <c r="H52" t="s">
-        <v>600</v>
+        <v>308</v>
       </c>
       <c r="AA52" t="s">
         <v>201</v>
@@ -14468,7 +15365,7 @@
     </row>
     <row r="53">
       <c r="H53" t="s">
-        <v>327</v>
+        <v>604</v>
       </c>
       <c r="AA53" t="s">
         <v>68</v>
@@ -14476,7 +15373,7 @@
     </row>
     <row r="54">
       <c r="H54" t="s">
-        <v>353</v>
+        <v>605</v>
       </c>
       <c r="AA54" t="s">
         <v>514</v>
@@ -14484,7 +15381,7 @@
     </row>
     <row r="55">
       <c r="H55" t="s">
-        <v>290</v>
+        <v>606</v>
       </c>
       <c r="AA55" t="s">
         <v>117</v>
@@ -14492,7 +15389,7 @@
     </row>
     <row r="56">
       <c r="H56" t="s">
-        <v>341</v>
+        <v>599</v>
       </c>
       <c r="AA56" t="s">
         <v>118</v>
@@ -14500,7 +15397,7 @@
     </row>
     <row r="57">
       <c r="H57" t="s">
-        <v>319</v>
+        <v>600</v>
       </c>
       <c r="AA57" t="s">
         <v>119</v>
@@ -14508,7 +15405,7 @@
     </row>
     <row r="58">
       <c r="H58" t="s">
-        <v>256</v>
+        <v>327</v>
       </c>
       <c r="AA58" t="s">
         <v>474</v>
@@ -14516,7 +15413,7 @@
     </row>
     <row r="59">
       <c r="H59" t="s">
-        <v>280</v>
+        <v>353</v>
       </c>
       <c r="AA59" t="s">
         <v>443</v>
@@ -14524,7 +15421,7 @@
     </row>
     <row r="60">
       <c r="H60" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="AA60" t="s">
         <v>120</v>
@@ -14532,7 +15429,7 @@
     </row>
     <row r="61">
       <c r="H61" t="s">
-        <v>518</v>
+        <v>341</v>
       </c>
       <c r="AA61" t="s">
         <v>334</v>
@@ -14540,7 +15437,7 @@
     </row>
     <row r="62">
       <c r="H62" t="s">
-        <v>282</v>
+        <v>319</v>
       </c>
       <c r="AA62" t="s">
         <v>444</v>
@@ -14548,7 +15445,7 @@
     </row>
     <row r="63">
       <c r="H63" t="s">
-        <v>291</v>
+        <v>256</v>
       </c>
       <c r="AA63" t="s">
         <v>121</v>
@@ -14556,7 +15453,7 @@
     </row>
     <row r="64">
       <c r="H64" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="AA64" t="s">
         <v>122</v>
@@ -14564,7 +15461,7 @@
     </row>
     <row r="65">
       <c r="H65" t="s">
-        <v>325</v>
+        <v>281</v>
       </c>
       <c r="AA65" t="s">
         <v>123</v>
@@ -14572,7 +15469,7 @@
     </row>
     <row r="66">
       <c r="H66" t="s">
-        <v>297</v>
+        <v>518</v>
       </c>
       <c r="AA66" t="s">
         <v>124</v>
@@ -14580,7 +15477,7 @@
     </row>
     <row r="67">
       <c r="H67" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
       <c r="AA67" t="s">
         <v>125</v>
@@ -14588,7 +15485,7 @@
     </row>
     <row r="68">
       <c r="H68" t="s">
-        <v>354</v>
+        <v>291</v>
       </c>
       <c r="AA68" t="s">
         <v>126</v>
@@ -14596,7 +15493,7 @@
     </row>
     <row r="69">
       <c r="H69" t="s">
-        <v>355</v>
+        <v>300</v>
       </c>
       <c r="AA69" t="s">
         <v>127</v>
@@ -14604,7 +15501,7 @@
     </row>
     <row r="70">
       <c r="H70" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="AA70" t="s">
         <v>421</v>
@@ -14612,7 +15509,7 @@
     </row>
     <row r="71">
       <c r="H71" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="AA71" t="s">
         <v>453</v>
@@ -14620,7 +15517,7 @@
     </row>
     <row r="72">
       <c r="H72" t="s">
-        <v>257</v>
+        <v>298</v>
       </c>
       <c r="AA72" t="s">
         <v>202</v>
@@ -14628,7 +15525,7 @@
     </row>
     <row r="73">
       <c r="H73" t="s">
-        <v>504</v>
+        <v>354</v>
       </c>
       <c r="AA73" t="s">
         <v>373</v>
@@ -14636,7 +15533,7 @@
     </row>
     <row r="74">
       <c r="H74" t="s">
-        <v>302</v>
+        <v>355</v>
       </c>
       <c r="AA74" t="s">
         <v>422</v>
@@ -14644,7 +15541,7 @@
     </row>
     <row r="75">
       <c r="H75" t="s">
-        <v>392</v>
+        <v>333</v>
       </c>
       <c r="AA75" t="s">
         <v>128</v>
@@ -14652,7 +15549,7 @@
     </row>
     <row r="76">
       <c r="H76" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="AA76" t="s">
         <v>129</v>
@@ -14660,7 +15557,7 @@
     </row>
     <row r="77">
       <c r="H77" t="s">
-        <v>393</v>
+        <v>257</v>
       </c>
       <c r="AA77" t="s">
         <v>130</v>
@@ -14668,7 +15565,7 @@
     </row>
     <row r="78">
       <c r="H78" t="s">
-        <v>250</v>
+        <v>504</v>
       </c>
       <c r="AA78" t="s">
         <v>131</v>
@@ -14676,7 +15573,7 @@
     </row>
     <row r="79">
       <c r="H79" t="s">
-        <v>489</v>
+        <v>302</v>
       </c>
       <c r="AA79" t="s">
         <v>570</v>
@@ -14684,7 +15581,7 @@
     </row>
     <row r="80">
       <c r="H80" t="s">
-        <v>332</v>
+        <v>392</v>
       </c>
       <c r="AA80" t="s">
         <v>185</v>
@@ -14692,7 +15589,7 @@
     </row>
     <row r="81">
       <c r="H81" t="s">
-        <v>268</v>
+        <v>292</v>
       </c>
       <c r="AA81" t="s">
         <v>186</v>
@@ -14700,7 +15597,7 @@
     </row>
     <row r="82">
       <c r="H82" t="s">
-        <v>274</v>
+        <v>393</v>
       </c>
       <c r="AA82" t="s">
         <v>433</v>
@@ -14708,7 +15605,7 @@
     </row>
     <row r="83">
       <c r="H83" t="s">
-        <v>279</v>
+        <v>250</v>
       </c>
       <c r="AA83" t="s">
         <v>445</v>
@@ -14716,7 +15613,7 @@
     </row>
     <row r="84">
       <c r="H84" t="s">
-        <v>411</v>
+        <v>489</v>
       </c>
       <c r="AA84" t="s">
         <v>132</v>
@@ -14724,7 +15621,7 @@
     </row>
     <row r="85">
       <c r="H85" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="AA85" t="s">
         <v>133</v>
@@ -14732,7 +15629,7 @@
     </row>
     <row r="86">
       <c r="H86" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="AA86" t="s">
         <v>134</v>
@@ -14740,7 +15637,7 @@
     </row>
     <row r="87">
       <c r="H87" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="AA87" t="s">
         <v>475</v>
@@ -14748,7 +15645,7 @@
     </row>
     <row r="88">
       <c r="H88" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="AA88" t="s">
         <v>135</v>
@@ -14756,7 +15653,7 @@
     </row>
     <row r="89">
       <c r="H89" t="s">
-        <v>264</v>
+        <v>411</v>
       </c>
       <c r="AA89" t="s">
         <v>136</v>
@@ -14764,7 +15661,7 @@
     </row>
     <row r="90">
       <c r="H90" t="s">
-        <v>506</v>
+        <v>320</v>
       </c>
       <c r="AA90" t="s">
         <v>187</v>
@@ -14772,7 +15669,7 @@
     </row>
     <row r="91">
       <c r="H91" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AA91" t="s">
         <v>476</v>
@@ -14780,7 +15677,7 @@
     </row>
     <row r="92">
       <c r="H92" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="AA92" t="s">
         <v>537</v>
@@ -14788,7 +15685,7 @@
     </row>
     <row r="93">
       <c r="H93" t="s">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="AA93" t="s">
         <v>188</v>
@@ -14796,7 +15693,7 @@
     </row>
     <row r="94">
       <c r="H94" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="AA94" t="s">
         <v>434</v>
@@ -14804,7 +15701,7 @@
     </row>
     <row r="95">
       <c r="H95" t="s">
-        <v>293</v>
+        <v>506</v>
       </c>
       <c r="AA95" t="s">
         <v>189</v>
@@ -14812,7 +15709,7 @@
     </row>
     <row r="96">
       <c r="H96" t="s">
-        <v>299</v>
+        <v>259</v>
       </c>
       <c r="AA96" t="s">
         <v>190</v>
@@ -14820,7 +15717,7 @@
     </row>
     <row r="97">
       <c r="H97" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="AA97" t="s">
         <v>524</v>
@@ -14828,7 +15725,7 @@
     </row>
     <row r="98">
       <c r="H98" t="s">
-        <v>328</v>
+        <v>260</v>
       </c>
       <c r="AA98" t="s">
         <v>525</v>
@@ -14836,7 +15733,7 @@
     </row>
     <row r="99">
       <c r="H99" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="AA99" t="s">
         <v>203</v>
@@ -14844,33 +15741,48 @@
     </row>
     <row r="100">
       <c r="H100" t="s">
-        <v>266</v>
+        <v>293</v>
       </c>
       <c r="AA100" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="101">
+      <c r="H101" t="s">
+        <v>299</v>
+      </c>
       <c r="AA101" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="102">
+      <c r="H102" t="s">
+        <v>283</v>
+      </c>
       <c r="AA102" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="103">
+      <c r="H103" t="s">
+        <v>328</v>
+      </c>
       <c r="AA103" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="104">
+      <c r="H104" t="s">
+        <v>265</v>
+      </c>
       <c r="AA104" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="105">
+      <c r="H105" t="s">
+        <v>266</v>
+      </c>
       <c r="AA105" t="s">
         <v>424</v>
       </c>

</xml_diff>

<commit_message>
[desktop] - [`screenshotByLocator(locator,file)`]: *NEW* capture the screenshot of the specified locator. - [`screenshot(name,file)`]: *NEW* capture the screenshot of the specified desktop component via its name. - [`clickMenuByLocator(locator,menu)`]: support the triggering of menu via `INDEX:` (same support as in context menu).
[web]
- [`dragAndDrop(fromLocator,toLocator)`]: updated to support native mouse event, which is required when start of a drag-and-drop event also trigger drastic changes to the underlying DOM structure.
- [`dragTo(fromLocator,xOffset,yOffset)`]: updated to support native mouse event, which is required when start of a drag-and-drop event also trigger drastic changes to the underlying DOM structure.

Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -20,7 +20,7 @@
     <definedName name="csv">'#system'!$G$2:$G$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$H$2:$H$101</definedName>
+    <definedName name="desktop">'#system'!$H$2:$H$102</definedName>
     <definedName name="excel">'#system'!$I$2:$I$17</definedName>
     <definedName name="external">'#system'!$J$2:$J$7</definedName>
     <definedName name="image">'#system'!$K$2:$K$8</definedName>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26946" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27568" uniqueCount="611">
   <si>
     <t>description</t>
   </si>
@@ -1904,6 +1904,9 @@
   </si>
   <si>
     <t>saveTableRowsRange(var,beginRow,endRow,csv)</t>
+  </si>
+  <si>
+    <t>screenshotByLocator(locator,file)</t>
   </si>
 </sst>
 </file>
@@ -1911,7 +1914,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="739" x14ac:knownFonts="1">
+  <fonts count="756" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6566,8 +6569,115 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1035">
+  <fills count="1059">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6578,6 +6688,142 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -12458,7 +12704,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="752">
+  <cellXfs count="769">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -14719,6 +14965,57 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="738" fillId="1031" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="739" fillId="1037" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="740" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="741" fillId="1040" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="742" fillId="1043" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="743" fillId="1046" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="744" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="745" fillId="1049" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="746" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="747" fillId="1052" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="748" fillId="1055" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="749" fillId="1043" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="750" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="751" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="752" fillId="1046" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="753" fillId="1058" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="754" fillId="1046" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="755" fillId="1055" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -16798,7 +17095,7 @@
     </row>
     <row r="84">
       <c r="H84" t="s">
-        <v>279</v>
+        <v>610</v>
       </c>
       <c r="AA84" t="s">
         <v>132</v>
@@ -16806,7 +17103,7 @@
     </row>
     <row r="85">
       <c r="H85" t="s">
-        <v>411</v>
+        <v>279</v>
       </c>
       <c r="AA85" t="s">
         <v>133</v>
@@ -16814,7 +17111,7 @@
     </row>
     <row r="86">
       <c r="H86" t="s">
-        <v>320</v>
+        <v>411</v>
       </c>
       <c r="AA86" t="s">
         <v>134</v>
@@ -16822,7 +17119,7 @@
     </row>
     <row r="87">
       <c r="H87" t="s">
-        <v>258</v>
+        <v>320</v>
       </c>
       <c r="AA87" t="s">
         <v>475</v>
@@ -16830,7 +17127,7 @@
     </row>
     <row r="88">
       <c r="H88" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="AA88" t="s">
         <v>135</v>
@@ -16838,7 +17135,7 @@
     </row>
     <row r="89">
       <c r="H89" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="AA89" t="s">
         <v>136</v>
@@ -16846,7 +17143,7 @@
     </row>
     <row r="90">
       <c r="H90" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="AA90" t="s">
         <v>187</v>
@@ -16854,7 +17151,7 @@
     </row>
     <row r="91">
       <c r="H91" t="s">
-        <v>506</v>
+        <v>264</v>
       </c>
       <c r="AA91" t="s">
         <v>476</v>
@@ -16862,7 +17159,7 @@
     </row>
     <row r="92">
       <c r="H92" t="s">
-        <v>259</v>
+        <v>506</v>
       </c>
       <c r="AA92" t="s">
         <v>537</v>
@@ -16870,7 +17167,7 @@
     </row>
     <row r="93">
       <c r="H93" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="AA93" t="s">
         <v>188</v>
@@ -16878,7 +17175,7 @@
     </row>
     <row r="94">
       <c r="H94" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="AA94" t="s">
         <v>434</v>
@@ -16886,7 +17183,7 @@
     </row>
     <row r="95">
       <c r="H95" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AA95" t="s">
         <v>189</v>
@@ -16894,7 +17191,7 @@
     </row>
     <row r="96">
       <c r="H96" t="s">
-        <v>293</v>
+        <v>261</v>
       </c>
       <c r="AA96" t="s">
         <v>190</v>
@@ -16902,7 +17199,7 @@
     </row>
     <row r="97">
       <c r="H97" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="AA97" t="s">
         <v>524</v>
@@ -16910,7 +17207,7 @@
     </row>
     <row r="98">
       <c r="H98" t="s">
-        <v>283</v>
+        <v>299</v>
       </c>
       <c r="AA98" t="s">
         <v>525</v>
@@ -16918,7 +17215,7 @@
     </row>
     <row r="99">
       <c r="H99" t="s">
-        <v>328</v>
+        <v>283</v>
       </c>
       <c r="AA99" t="s">
         <v>203</v>
@@ -16926,7 +17223,7 @@
     </row>
     <row r="100">
       <c r="H100" t="s">
-        <v>265</v>
+        <v>328</v>
       </c>
       <c r="AA100" t="s">
         <v>137</v>
@@ -16934,13 +17231,16 @@
     </row>
     <row r="101">
       <c r="H101" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AA101" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="102">
+      <c r="H102" t="s">
+        <v>266</v>
+      </c>
       <c r="AA102" t="s">
         <v>423</v>
       </c>

</xml_diff>

<commit_message>
[expression] - [LisT &raquo; `item(index)`]: support multiple indices (to concatenate specified items into 1 text) and the use of `random` to randomly select one of the available item.
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -20,7 +20,7 @@
     <definedName name="csv">'#system'!$G$2:$G$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$H$2:$H$102</definedName>
+    <definedName name="desktop">'#system'!$H$2:$H$103</definedName>
     <definedName name="excel">'#system'!$I$2:$I$17</definedName>
     <definedName name="external">'#system'!$J$2:$J$7</definedName>
     <definedName name="image">'#system'!$K$2:$K$8</definedName>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27568" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29437" uniqueCount="612">
   <si>
     <t>description</t>
   </si>
@@ -1907,6 +1907,9 @@
   </si>
   <si>
     <t>screenshotByLocator(locator,file)</t>
+  </si>
+  <si>
+    <t>screenshot(name,file)</t>
   </si>
 </sst>
 </file>
@@ -1914,7 +1917,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="756" x14ac:knownFonts="1">
+  <fonts count="807" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6676,8 +6679,329 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1059">
+  <fills count="1131">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6688,6 +7012,414 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -12704,7 +13436,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="769">
+  <cellXfs count="820">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -15016,6 +15748,159 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="755" fillId="1055" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="756" fillId="1061" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="757" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="758" fillId="1064" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="759" fillId="1067" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="760" fillId="1070" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="761" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="762" fillId="1073" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="763" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="764" fillId="1076" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="765" fillId="1079" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="766" fillId="1067" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="767" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="768" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="769" fillId="1070" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="770" fillId="1082" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="771" fillId="1070" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="772" fillId="1079" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="773" fillId="1085" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="774" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="775" fillId="1088" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="776" fillId="1091" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="777" fillId="1094" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="778" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="779" fillId="1097" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="780" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="781" fillId="1100" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="782" fillId="1103" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="783" fillId="1091" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="784" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="785" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="786" fillId="1094" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="787" fillId="1106" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="788" fillId="1094" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="789" fillId="1103" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="790" fillId="1109" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="791" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="792" fillId="1112" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="793" fillId="1115" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="794" fillId="1118" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="795" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="796" fillId="1121" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="797" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="798" fillId="1124" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="799" fillId="1127" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="800" fillId="1115" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="801" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="802" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="803" fillId="1118" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="804" fillId="1130" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="805" fillId="1118" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="806" fillId="1127" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -17095,7 +17980,7 @@
     </row>
     <row r="84">
       <c r="H84" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="AA84" t="s">
         <v>132</v>
@@ -17103,7 +17988,7 @@
     </row>
     <row r="85">
       <c r="H85" t="s">
-        <v>279</v>
+        <v>610</v>
       </c>
       <c r="AA85" t="s">
         <v>133</v>
@@ -17111,7 +17996,7 @@
     </row>
     <row r="86">
       <c r="H86" t="s">
-        <v>411</v>
+        <v>279</v>
       </c>
       <c r="AA86" t="s">
         <v>134</v>
@@ -17119,7 +18004,7 @@
     </row>
     <row r="87">
       <c r="H87" t="s">
-        <v>320</v>
+        <v>411</v>
       </c>
       <c r="AA87" t="s">
         <v>475</v>
@@ -17127,7 +18012,7 @@
     </row>
     <row r="88">
       <c r="H88" t="s">
-        <v>258</v>
+        <v>320</v>
       </c>
       <c r="AA88" t="s">
         <v>135</v>
@@ -17135,7 +18020,7 @@
     </row>
     <row r="89">
       <c r="H89" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="AA89" t="s">
         <v>136</v>
@@ -17143,7 +18028,7 @@
     </row>
     <row r="90">
       <c r="H90" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="AA90" t="s">
         <v>187</v>
@@ -17151,7 +18036,7 @@
     </row>
     <row r="91">
       <c r="H91" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="AA91" t="s">
         <v>476</v>
@@ -17159,7 +18044,7 @@
     </row>
     <row r="92">
       <c r="H92" t="s">
-        <v>506</v>
+        <v>264</v>
       </c>
       <c r="AA92" t="s">
         <v>537</v>
@@ -17167,7 +18052,7 @@
     </row>
     <row r="93">
       <c r="H93" t="s">
-        <v>259</v>
+        <v>506</v>
       </c>
       <c r="AA93" t="s">
         <v>188</v>
@@ -17175,7 +18060,7 @@
     </row>
     <row r="94">
       <c r="H94" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="AA94" t="s">
         <v>434</v>
@@ -17183,7 +18068,7 @@
     </row>
     <row r="95">
       <c r="H95" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="AA95" t="s">
         <v>189</v>
@@ -17191,7 +18076,7 @@
     </row>
     <row r="96">
       <c r="H96" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AA96" t="s">
         <v>190</v>
@@ -17199,7 +18084,7 @@
     </row>
     <row r="97">
       <c r="H97" t="s">
-        <v>293</v>
+        <v>261</v>
       </c>
       <c r="AA97" t="s">
         <v>524</v>
@@ -17207,7 +18092,7 @@
     </row>
     <row r="98">
       <c r="H98" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="AA98" t="s">
         <v>525</v>
@@ -17215,7 +18100,7 @@
     </row>
     <row r="99">
       <c r="H99" t="s">
-        <v>283</v>
+        <v>299</v>
       </c>
       <c r="AA99" t="s">
         <v>203</v>
@@ -17223,7 +18108,7 @@
     </row>
     <row r="100">
       <c r="H100" t="s">
-        <v>328</v>
+        <v>283</v>
       </c>
       <c r="AA100" t="s">
         <v>137</v>
@@ -17231,7 +18116,7 @@
     </row>
     <row r="101">
       <c r="H101" t="s">
-        <v>265</v>
+        <v>328</v>
       </c>
       <c r="AA101" t="s">
         <v>191</v>
@@ -17239,13 +18124,16 @@
     </row>
     <row r="102">
       <c r="H102" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AA102" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="103">
+      <c r="H103" t="s">
+        <v>266</v>
+      </c>
       <c r="AA103" t="s">
         <v>534</v>
       </c>

</xml_diff>

<commit_message>
[Nexial Interactive] - redesigned execution summary on console to reduce output and to improve readability. - code fix to correctly update execution statistics (esp. on execution duration).
[tn.5250]
- [`waitUntilProcessed(maxWaitMs)`]: **NEW** wait-until command to poll for the current TN5250 session to be unblocked from processing request. Usually, when a request is made to the connected TN5250 session, the server will need some time to completed the requested command/transaction. This command the automation to pause (and poll) until the request is completed and the session is "unblocked" from further interaction.
- reduce poll time from 1000ms to 200ms to improve overall performance.

Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29437" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30683" uniqueCount="612">
   <si>
     <t>description</t>
   </si>
@@ -1917,7 +1917,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="807" x14ac:knownFonts="1">
+  <fonts count="841" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7000,8 +7000,222 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1131">
+  <fills count="1179">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7012,6 +7226,278 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -13436,7 +13922,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="820">
+  <cellXfs count="854">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -15901,6 +16387,108 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="806" fillId="1127" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="807" fillId="1133" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="808" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="809" fillId="1136" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="810" fillId="1139" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="811" fillId="1142" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="812" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="813" fillId="1145" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="814" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="815" fillId="1148" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="816" fillId="1151" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="817" fillId="1139" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="818" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="819" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="820" fillId="1142" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="821" fillId="1154" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="822" fillId="1142" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="823" fillId="1151" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="824" fillId="1157" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="825" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="826" fillId="1160" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="827" fillId="1163" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="828" fillId="1166" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="829" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="830" fillId="1169" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="831" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="832" fillId="1172" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="833" fillId="1175" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="834" fillId="1163" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="835" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="836" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="837" fillId="1166" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="838" fillId="1178" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="839" fillId="1166" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="840" fillId="1175" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[excel commands] - [`xls2xlsx(xlsFile,xlsxFile)`]: **NEW** command to convert XLS to XLSX.
[rdbms commands]
- [`resultToCSV(var,csvFile,delim,showHeader)`]: removed trailing newline character.

[ws commands]
- For BASIC authentication, `nexial.ws.basic.password` is no longer required (edge cases). `nexial.ws.basic.user` is still required for BASIC authentication.

Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -21,7 +21,7 @@
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
     <definedName name="desktop">'#system'!$H$2:$H$103</definedName>
-    <definedName name="excel">'#system'!$I$2:$I$17</definedName>
+    <definedName name="excel">'#system'!$I$2:$I$18</definedName>
     <definedName name="external">'#system'!$J$2:$J$7</definedName>
     <definedName name="image">'#system'!$K$2:$K$8</definedName>
     <definedName name="io">'#system'!$L$2:$L$32</definedName>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30683" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31931" uniqueCount="613">
   <si>
     <t>description</t>
   </si>
@@ -1910,6 +1910,9 @@
   </si>
   <si>
     <t>screenshot(name,file)</t>
+  </si>
+  <si>
+    <t>xls2xlsx(xlsFile,xlsxFile)</t>
   </si>
 </sst>
 </file>
@@ -1917,7 +1920,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="841" x14ac:knownFonts="1">
+  <fonts count="875" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7214,8 +7217,222 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1179">
+  <fills count="1227">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7226,6 +7443,278 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -13922,7 +14411,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="854">
+  <cellXfs count="888">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -16489,6 +16978,108 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="840" fillId="1175" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="841" fillId="1181" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="842" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="843" fillId="1184" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="844" fillId="1187" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="845" fillId="1190" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="846" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="847" fillId="1193" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="848" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="849" fillId="1196" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="850" fillId="1199" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="851" fillId="1187" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="852" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="853" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="854" fillId="1190" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="855" fillId="1202" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="856" fillId="1190" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="857" fillId="1199" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="858" fillId="1205" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="859" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="860" fillId="1208" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="861" fillId="1211" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="862" fillId="1214" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="863" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="864" fillId="1217" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="865" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="866" fillId="1220" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="867" fillId="1223" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="868" fillId="1211" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="869" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="870" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="871" fillId="1214" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="872" fillId="1226" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="873" fillId="1214" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="874" fillId="1223" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -17832,6 +18423,9 @@
       <c r="H18" t="s">
         <v>80</v>
       </c>
+      <c r="I18" t="s">
+        <v>612</v>
+      </c>
       <c r="L18" t="s">
         <v>72</v>
       </c>

</xml_diff>

<commit_message>
[desktop] - [`saveComboOptions(var,name)`]: *NEW* command to capture the available options of a Combo component as a list. - [`selectCombo(name,text)`]: fix flaky automation when dealing with SingleSelectList component that contains nested SingleSelectList components.
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -20,7 +20,7 @@
     <definedName name="csv">'#system'!$G$2:$G$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$H$2:$H$103</definedName>
+    <definedName name="desktop">'#system'!$H$2:$H$104</definedName>
     <definedName name="excel">'#system'!$I$2:$I$18</definedName>
     <definedName name="external">'#system'!$J$2:$J$7</definedName>
     <definedName name="image">'#system'!$K$2:$K$8</definedName>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31931" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32556" uniqueCount="614">
   <si>
     <t>description</t>
   </si>
@@ -1913,6 +1913,9 @@
   </si>
   <si>
     <t>xls2xlsx(xlsFile,xlsxFile)</t>
+  </si>
+  <si>
+    <t>saveComboOptions(var,name)</t>
   </si>
 </sst>
 </file>
@@ -1920,7 +1923,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="875" x14ac:knownFonts="1">
+  <fonts count="892" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7431,8 +7434,115 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1227">
+  <fills count="1251">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7443,6 +7553,142 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -14411,7 +14657,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="888">
+  <cellXfs count="905">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -17080,6 +17326,57 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="874" fillId="1223" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="875" fillId="1229" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="876" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="877" fillId="1232" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="878" fillId="1235" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="879" fillId="1238" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="880" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="881" fillId="1241" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="882" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="883" fillId="1244" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="884" fillId="1247" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="885" fillId="1235" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="886" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="887" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="888" fillId="1238" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="889" fillId="1250" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="890" fillId="1238" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="891" fillId="1247" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -19026,7 +19323,7 @@
     </row>
     <row r="67">
       <c r="H67" t="s">
-        <v>325</v>
+        <v>613</v>
       </c>
       <c r="AA67" t="s">
         <v>125</v>
@@ -19034,7 +19331,7 @@
     </row>
     <row r="68">
       <c r="H68" t="s">
-        <v>297</v>
+        <v>325</v>
       </c>
       <c r="AA68" t="s">
         <v>126</v>
@@ -19042,7 +19339,7 @@
     </row>
     <row r="69">
       <c r="H69" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AA69" t="s">
         <v>127</v>
@@ -19050,7 +19347,7 @@
     </row>
     <row r="70">
       <c r="H70" t="s">
-        <v>354</v>
+        <v>298</v>
       </c>
       <c r="AA70" t="s">
         <v>421</v>
@@ -19058,7 +19355,7 @@
     </row>
     <row r="71">
       <c r="H71" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="AA71" t="s">
         <v>453</v>
@@ -19066,7 +19363,7 @@
     </row>
     <row r="72">
       <c r="H72" t="s">
-        <v>333</v>
+        <v>355</v>
       </c>
       <c r="AA72" t="s">
         <v>202</v>
@@ -19074,7 +19371,7 @@
     </row>
     <row r="73">
       <c r="H73" t="s">
-        <v>301</v>
+        <v>333</v>
       </c>
       <c r="AA73" t="s">
         <v>373</v>
@@ -19082,7 +19379,7 @@
     </row>
     <row r="74">
       <c r="H74" t="s">
-        <v>257</v>
+        <v>301</v>
       </c>
       <c r="AA74" t="s">
         <v>422</v>
@@ -19090,7 +19387,7 @@
     </row>
     <row r="75">
       <c r="H75" t="s">
-        <v>504</v>
+        <v>257</v>
       </c>
       <c r="AA75" t="s">
         <v>128</v>
@@ -19098,7 +19395,7 @@
     </row>
     <row r="76">
       <c r="H76" t="s">
-        <v>302</v>
+        <v>504</v>
       </c>
       <c r="AA76" t="s">
         <v>129</v>
@@ -19106,7 +19403,7 @@
     </row>
     <row r="77">
       <c r="H77" t="s">
-        <v>392</v>
+        <v>302</v>
       </c>
       <c r="AA77" t="s">
         <v>130</v>
@@ -19114,7 +19411,7 @@
     </row>
     <row r="78">
       <c r="H78" t="s">
-        <v>608</v>
+        <v>392</v>
       </c>
       <c r="AA78" t="s">
         <v>131</v>
@@ -19122,7 +19419,7 @@
     </row>
     <row r="79">
       <c r="H79" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AA79" t="s">
         <v>570</v>
@@ -19130,7 +19427,7 @@
     </row>
     <row r="80">
       <c r="H80" t="s">
-        <v>250</v>
+        <v>609</v>
       </c>
       <c r="AA80" t="s">
         <v>185</v>
@@ -19138,7 +19435,7 @@
     </row>
     <row r="81">
       <c r="H81" t="s">
-        <v>489</v>
+        <v>250</v>
       </c>
       <c r="AA81" t="s">
         <v>186</v>
@@ -19146,7 +19443,7 @@
     </row>
     <row r="82">
       <c r="H82" t="s">
-        <v>332</v>
+        <v>489</v>
       </c>
       <c r="AA82" t="s">
         <v>433</v>
@@ -19154,7 +19451,7 @@
     </row>
     <row r="83">
       <c r="H83" t="s">
-        <v>268</v>
+        <v>332</v>
       </c>
       <c r="AA83" t="s">
         <v>445</v>
@@ -19162,7 +19459,7 @@
     </row>
     <row r="84">
       <c r="H84" t="s">
-        <v>611</v>
+        <v>268</v>
       </c>
       <c r="AA84" t="s">
         <v>132</v>
@@ -19170,7 +19467,7 @@
     </row>
     <row r="85">
       <c r="H85" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="AA85" t="s">
         <v>133</v>
@@ -19178,7 +19475,7 @@
     </row>
     <row r="86">
       <c r="H86" t="s">
-        <v>279</v>
+        <v>610</v>
       </c>
       <c r="AA86" t="s">
         <v>134</v>
@@ -19186,7 +19483,7 @@
     </row>
     <row r="87">
       <c r="H87" t="s">
-        <v>411</v>
+        <v>279</v>
       </c>
       <c r="AA87" t="s">
         <v>475</v>
@@ -19194,7 +19491,7 @@
     </row>
     <row r="88">
       <c r="H88" t="s">
-        <v>320</v>
+        <v>411</v>
       </c>
       <c r="AA88" t="s">
         <v>135</v>
@@ -19202,7 +19499,7 @@
     </row>
     <row r="89">
       <c r="H89" t="s">
-        <v>258</v>
+        <v>320</v>
       </c>
       <c r="AA89" t="s">
         <v>136</v>
@@ -19210,7 +19507,7 @@
     </row>
     <row r="90">
       <c r="H90" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="AA90" t="s">
         <v>187</v>
@@ -19218,7 +19515,7 @@
     </row>
     <row r="91">
       <c r="H91" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="AA91" t="s">
         <v>476</v>
@@ -19226,7 +19523,7 @@
     </row>
     <row r="92">
       <c r="H92" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="AA92" t="s">
         <v>537</v>
@@ -19234,7 +19531,7 @@
     </row>
     <row r="93">
       <c r="H93" t="s">
-        <v>506</v>
+        <v>264</v>
       </c>
       <c r="AA93" t="s">
         <v>188</v>
@@ -19242,7 +19539,7 @@
     </row>
     <row r="94">
       <c r="H94" t="s">
-        <v>259</v>
+        <v>506</v>
       </c>
       <c r="AA94" t="s">
         <v>434</v>
@@ -19250,7 +19547,7 @@
     </row>
     <row r="95">
       <c r="H95" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="AA95" t="s">
         <v>189</v>
@@ -19258,7 +19555,7 @@
     </row>
     <row r="96">
       <c r="H96" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="AA96" t="s">
         <v>190</v>
@@ -19266,7 +19563,7 @@
     </row>
     <row r="97">
       <c r="H97" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AA97" t="s">
         <v>524</v>
@@ -19274,7 +19571,7 @@
     </row>
     <row r="98">
       <c r="H98" t="s">
-        <v>293</v>
+        <v>261</v>
       </c>
       <c r="AA98" t="s">
         <v>525</v>
@@ -19282,7 +19579,7 @@
     </row>
     <row r="99">
       <c r="H99" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="AA99" t="s">
         <v>203</v>
@@ -19290,7 +19587,7 @@
     </row>
     <row r="100">
       <c r="H100" t="s">
-        <v>283</v>
+        <v>299</v>
       </c>
       <c r="AA100" t="s">
         <v>137</v>
@@ -19298,7 +19595,7 @@
     </row>
     <row r="101">
       <c r="H101" t="s">
-        <v>328</v>
+        <v>283</v>
       </c>
       <c r="AA101" t="s">
         <v>191</v>
@@ -19306,7 +19603,7 @@
     </row>
     <row r="102">
       <c r="H102" t="s">
-        <v>265</v>
+        <v>328</v>
       </c>
       <c r="AA102" t="s">
         <v>423</v>
@@ -19314,13 +19611,16 @@
     </row>
     <row r="103">
       <c r="H103" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AA103" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="104">
+      <c r="H104" t="s">
+        <v>266</v>
+      </c>
       <c r="AA104" t="s">
         <v>535</v>
       </c>

</xml_diff>

<commit_message>
[desktop] - [`saveComboOptionsByLocator(var,locator)`]: *NEW* command to capture the available options of a ComboBox component as a list.
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -20,7 +20,7 @@
     <definedName name="csv">'#system'!$G$2:$G$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
-    <definedName name="desktop">'#system'!$H$2:$H$104</definedName>
+    <definedName name="desktop">'#system'!$H$2:$H$105</definedName>
     <definedName name="excel">'#system'!$I$2:$I$18</definedName>
     <definedName name="external">'#system'!$J$2:$J$7</definedName>
     <definedName name="image">'#system'!$K$2:$K$8</definedName>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32556" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33182" uniqueCount="615">
   <si>
     <t>description</t>
   </si>
@@ -1916,6 +1916,9 @@
   </si>
   <si>
     <t>saveComboOptions(var,name)</t>
+  </si>
+  <si>
+    <t>saveComboOptionsByLocator(var,locator)</t>
   </si>
 </sst>
 </file>
@@ -1923,7 +1926,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="892" x14ac:knownFonts="1">
+  <fonts count="909" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7541,8 +7544,115 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1251">
+  <fills count="1275">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7553,6 +7663,142 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -14657,7 +14903,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="905">
+  <cellXfs count="922">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -17377,6 +17623,57 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="891" fillId="1247" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="892" fillId="1253" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="893" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="894" fillId="1256" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="895" fillId="1259" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="896" fillId="1262" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="897" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="898" fillId="1265" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="899" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="900" fillId="1268" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="901" fillId="1271" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="902" fillId="1259" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="903" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="904" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="905" fillId="1262" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="906" fillId="1274" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="907" fillId="1262" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="908" fillId="1271" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -19331,7 +19628,7 @@
     </row>
     <row r="68">
       <c r="H68" t="s">
-        <v>325</v>
+        <v>614</v>
       </c>
       <c r="AA68" t="s">
         <v>126</v>
@@ -19339,7 +19636,7 @@
     </row>
     <row r="69">
       <c r="H69" t="s">
-        <v>297</v>
+        <v>325</v>
       </c>
       <c r="AA69" t="s">
         <v>127</v>
@@ -19347,7 +19644,7 @@
     </row>
     <row r="70">
       <c r="H70" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AA70" t="s">
         <v>421</v>
@@ -19355,7 +19652,7 @@
     </row>
     <row r="71">
       <c r="H71" t="s">
-        <v>354</v>
+        <v>298</v>
       </c>
       <c r="AA71" t="s">
         <v>453</v>
@@ -19363,7 +19660,7 @@
     </row>
     <row r="72">
       <c r="H72" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="AA72" t="s">
         <v>202</v>
@@ -19371,7 +19668,7 @@
     </row>
     <row r="73">
       <c r="H73" t="s">
-        <v>333</v>
+        <v>355</v>
       </c>
       <c r="AA73" t="s">
         <v>373</v>
@@ -19379,7 +19676,7 @@
     </row>
     <row r="74">
       <c r="H74" t="s">
-        <v>301</v>
+        <v>333</v>
       </c>
       <c r="AA74" t="s">
         <v>422</v>
@@ -19387,7 +19684,7 @@
     </row>
     <row r="75">
       <c r="H75" t="s">
-        <v>257</v>
+        <v>301</v>
       </c>
       <c r="AA75" t="s">
         <v>128</v>
@@ -19395,7 +19692,7 @@
     </row>
     <row r="76">
       <c r="H76" t="s">
-        <v>504</v>
+        <v>257</v>
       </c>
       <c r="AA76" t="s">
         <v>129</v>
@@ -19403,7 +19700,7 @@
     </row>
     <row r="77">
       <c r="H77" t="s">
-        <v>302</v>
+        <v>504</v>
       </c>
       <c r="AA77" t="s">
         <v>130</v>
@@ -19411,7 +19708,7 @@
     </row>
     <row r="78">
       <c r="H78" t="s">
-        <v>392</v>
+        <v>302</v>
       </c>
       <c r="AA78" t="s">
         <v>131</v>
@@ -19419,7 +19716,7 @@
     </row>
     <row r="79">
       <c r="H79" t="s">
-        <v>608</v>
+        <v>392</v>
       </c>
       <c r="AA79" t="s">
         <v>570</v>
@@ -19427,7 +19724,7 @@
     </row>
     <row r="80">
       <c r="H80" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AA80" t="s">
         <v>185</v>
@@ -19435,7 +19732,7 @@
     </row>
     <row r="81">
       <c r="H81" t="s">
-        <v>250</v>
+        <v>609</v>
       </c>
       <c r="AA81" t="s">
         <v>186</v>
@@ -19443,7 +19740,7 @@
     </row>
     <row r="82">
       <c r="H82" t="s">
-        <v>489</v>
+        <v>250</v>
       </c>
       <c r="AA82" t="s">
         <v>433</v>
@@ -19451,7 +19748,7 @@
     </row>
     <row r="83">
       <c r="H83" t="s">
-        <v>332</v>
+        <v>489</v>
       </c>
       <c r="AA83" t="s">
         <v>445</v>
@@ -19459,7 +19756,7 @@
     </row>
     <row r="84">
       <c r="H84" t="s">
-        <v>268</v>
+        <v>332</v>
       </c>
       <c r="AA84" t="s">
         <v>132</v>
@@ -19467,7 +19764,7 @@
     </row>
     <row r="85">
       <c r="H85" t="s">
-        <v>611</v>
+        <v>268</v>
       </c>
       <c r="AA85" t="s">
         <v>133</v>
@@ -19475,7 +19772,7 @@
     </row>
     <row r="86">
       <c r="H86" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="AA86" t="s">
         <v>134</v>
@@ -19483,7 +19780,7 @@
     </row>
     <row r="87">
       <c r="H87" t="s">
-        <v>279</v>
+        <v>610</v>
       </c>
       <c r="AA87" t="s">
         <v>475</v>
@@ -19491,7 +19788,7 @@
     </row>
     <row r="88">
       <c r="H88" t="s">
-        <v>411</v>
+        <v>279</v>
       </c>
       <c r="AA88" t="s">
         <v>135</v>
@@ -19499,7 +19796,7 @@
     </row>
     <row r="89">
       <c r="H89" t="s">
-        <v>320</v>
+        <v>411</v>
       </c>
       <c r="AA89" t="s">
         <v>136</v>
@@ -19507,7 +19804,7 @@
     </row>
     <row r="90">
       <c r="H90" t="s">
-        <v>258</v>
+        <v>320</v>
       </c>
       <c r="AA90" t="s">
         <v>187</v>
@@ -19515,7 +19812,7 @@
     </row>
     <row r="91">
       <c r="H91" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="AA91" t="s">
         <v>476</v>
@@ -19523,7 +19820,7 @@
     </row>
     <row r="92">
       <c r="H92" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="AA92" t="s">
         <v>537</v>
@@ -19531,7 +19828,7 @@
     </row>
     <row r="93">
       <c r="H93" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="AA93" t="s">
         <v>188</v>
@@ -19539,7 +19836,7 @@
     </row>
     <row r="94">
       <c r="H94" t="s">
-        <v>506</v>
+        <v>264</v>
       </c>
       <c r="AA94" t="s">
         <v>434</v>
@@ -19547,7 +19844,7 @@
     </row>
     <row r="95">
       <c r="H95" t="s">
-        <v>259</v>
+        <v>506</v>
       </c>
       <c r="AA95" t="s">
         <v>189</v>
@@ -19555,7 +19852,7 @@
     </row>
     <row r="96">
       <c r="H96" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="AA96" t="s">
         <v>190</v>
@@ -19563,7 +19860,7 @@
     </row>
     <row r="97">
       <c r="H97" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="AA97" t="s">
         <v>524</v>
@@ -19571,7 +19868,7 @@
     </row>
     <row r="98">
       <c r="H98" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AA98" t="s">
         <v>525</v>
@@ -19579,7 +19876,7 @@
     </row>
     <row r="99">
       <c r="H99" t="s">
-        <v>293</v>
+        <v>261</v>
       </c>
       <c r="AA99" t="s">
         <v>203</v>
@@ -19587,7 +19884,7 @@
     </row>
     <row r="100">
       <c r="H100" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="AA100" t="s">
         <v>137</v>
@@ -19595,7 +19892,7 @@
     </row>
     <row r="101">
       <c r="H101" t="s">
-        <v>283</v>
+        <v>299</v>
       </c>
       <c r="AA101" t="s">
         <v>191</v>
@@ -19603,7 +19900,7 @@
     </row>
     <row r="102">
       <c r="H102" t="s">
-        <v>328</v>
+        <v>283</v>
       </c>
       <c r="AA102" t="s">
         <v>423</v>
@@ -19611,7 +19908,7 @@
     </row>
     <row r="103">
       <c r="H103" t="s">
-        <v>265</v>
+        <v>328</v>
       </c>
       <c r="AA103" t="s">
         <v>534</v>
@@ -19619,13 +19916,16 @@
     </row>
     <row r="104">
       <c r="H104" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AA104" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="105">
+      <c r="H105" t="s">
+        <v>266</v>
+      </c>
       <c r="AA105" t="s">
         <v>424</v>
       </c>

</xml_diff>

<commit_message>
[improvements] - [`nexial.projectProperties.trimKey`]: support leading/trailing spaces in data variable names in the `project.properties`, for aligning variable values to improve readability.
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33182" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33808" uniqueCount="615">
   <si>
     <t>description</t>
   </si>
@@ -1926,7 +1926,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="909" x14ac:knownFonts="1">
+  <fonts count="926" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7651,8 +7651,115 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1275">
+  <fills count="1299">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7663,6 +7770,142 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -14903,7 +15146,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="922">
+  <cellXfs count="939">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -17674,6 +17917,57 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="908" fillId="1271" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="909" fillId="1277" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="910" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="911" fillId="1280" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="912" fillId="1283" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="913" fillId="1286" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="914" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="915" fillId="1289" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="916" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="917" fillId="1292" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="918" fillId="1295" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="919" fillId="1283" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="920" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="921" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="922" fillId="1286" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="923" fillId="1298" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="924" fillId="1286" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="925" fillId="1295" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[web] - [`screenshot(file,locator,removeFixed)`]: additional wait time to offset any visual effect caused by [`nexial.web.highlight`]
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33808" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34434" uniqueCount="615">
   <si>
     <t>description</t>
   </si>
@@ -1926,7 +1926,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="926" x14ac:knownFonts="1">
+  <fonts count="943" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7758,8 +7758,115 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1299">
+  <fills count="1323">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7770,6 +7877,142 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -15146,7 +15389,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="939">
+  <cellXfs count="956">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -17968,6 +18211,57 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="925" fillId="1295" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="926" fillId="1301" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="927" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="928" fillId="1304" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="929" fillId="1307" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="930" fillId="1310" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="931" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="932" fillId="1313" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="933" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="934" fillId="1316" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="935" fillId="1319" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="936" fillId="1307" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="937" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="938" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="939" fillId="1310" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="940" fillId="1322" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="941" fillId="1310" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="942" fillId="1319" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[expression] - [TEXT >> number]: "optimistically" converts text to number by _gently_ removing non-numeric characters.
[web]
- [`assertLocation(search)`]: *NEW* command to assert the current URL with PolyMatcher.
- fixed a "circular reference" issue with collection browser performance metrics over JQuery-laden web page.
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34434" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35060" uniqueCount="615">
   <si>
     <t>description</t>
   </si>
@@ -1926,7 +1926,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="943" x14ac:knownFonts="1">
+  <fonts count="960" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7865,8 +7865,115 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1323">
+  <fills count="1347">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7877,6 +7984,142 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -15389,7 +15632,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="956">
+  <cellXfs count="973">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -18262,6 +18505,57 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="942" fillId="1319" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="943" fillId="1325" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="944" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="945" fillId="1328" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="946" fillId="1331" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="947" fillId="1334" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="948" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="949" fillId="1337" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="950" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="951" fillId="1340" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="952" fillId="1343" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="953" fillId="1331" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="954" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="955" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="956" fillId="1334" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="957" fillId="1346" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="958" fillId="1334" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="959" fillId="1343" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
[base] - [`assertVarsPresent(vars)`]: check that all the specified data variables exist in the current execution. - [`assertVarsNotPresent(vars)`]: check that none of the specified data variables exist in the current execution.
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/template/nexial-macro.xlsx
+++ b/template/nexial-macro.xlsx
@@ -16,7 +16,7 @@
     <definedName name="aws.ses">'#system'!$C$2:$C$3</definedName>
     <definedName name="aws.sqs">'#system'!$D$2:$D$6</definedName>
     <definedName name="aws.vision">'#system'!$E$2:$E$2</definedName>
-    <definedName name="base">'#system'!$F$2:$F$45</definedName>
+    <definedName name="base">'#system'!$F$2:$F$47</definedName>
     <definedName name="csv">'#system'!$G$2:$G$6</definedName>
     <definedName name="date">'#system'!$C$2:$C$14</definedName>
     <definedName name="db">'#system'!$D$2:$D$5</definedName>
@@ -45,7 +45,7 @@
     <definedName name="target">'#system'!$A$2:$A$33</definedName>
     <definedName name="text">'#system'!$Y$2:$Y$2</definedName>
     <definedName name="tn.5250">'#system'!$AA$2:$AA$8</definedName>
-    <definedName name="web">'#system'!$AA$2:$AA$151</definedName>
+    <definedName name="web">'#system'!$AA$2:$AA$152</definedName>
     <definedName name="webalert">'#system'!$AB$2:$AB$8</definedName>
     <definedName name="webcookie">'#system'!$AC$2:$AC$10</definedName>
     <definedName name="ws">'#system'!$AE$2:$AE$17</definedName>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35060" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35689" uniqueCount="618">
   <si>
     <t>description</t>
   </si>
@@ -1919,6 +1919,15 @@
   </si>
   <si>
     <t>saveComboOptionsByLocator(var,locator)</t>
+  </si>
+  <si>
+    <t>assertVarsNotPresent(vars)</t>
+  </si>
+  <si>
+    <t>assertVarsPresent(vars)</t>
+  </si>
+  <si>
+    <t>assertLocation(search)</t>
   </si>
 </sst>
 </file>
@@ -1926,7 +1935,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="960" x14ac:knownFonts="1">
+  <fonts count="977" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -7972,8 +7981,115 @@
       <color rgb="808080"/>
       <u val="none"/>
     </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="3E511F"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="287389"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="6E6E3C"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="5A5A32"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="11.0"/>
+      <color rgb="12284A"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <sz val="10.0"/>
+      <color rgb="0000FF"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="050505"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="006100"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="10.0"/>
+      <color rgb="9C0006"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Tahoma"/>
+      <sz val="11.0"/>
+      <color rgb="808080"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="1347">
+  <fills count="1371">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7984,6 +8100,142 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB4B4B4"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6EFD7"/>
+        <bgColor rgb="E6EFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="DCE1E6"/>
+        <bgColor rgb="DCE1E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="F0F0E1"/>
+        <bgColor rgb="F0F0E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7CE"/>
+        <bgColor rgb="FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="ECECE8"/>
+        <bgColor rgb="ECECE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAFAFA"/>
+        <bgColor rgb="FAFAFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="E6E6E6"/>
+        <bgColor rgb="E6E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="C6EFCE"/>
+        <bgColor rgb="C6EFCE"/>
       </patternFill>
     </fill>
     <fill>
@@ -15632,7 +15884,7 @@
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="973">
+  <cellXfs count="990">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -18556,6 +18808,57 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="959" fillId="1343" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="960" fillId="1349" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="961" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="962" fillId="1352" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="963" fillId="1355" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="964" fillId="1358" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="965" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="966" fillId="1361" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment indent="1" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="967" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="968" fillId="1364" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="969" fillId="1367" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="970" fillId="1355" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="971" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="972" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="973" fillId="1358" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="974" fillId="1370" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="975" fillId="1358" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="976" fillId="1367" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -18853,7 +19156,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH151"/>
+  <dimension ref="A1:AH152"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125"/>
   </sheetViews>
@@ -19923,7 +20226,7 @@
         <v>226</v>
       </c>
       <c r="F19" t="s">
-        <v>397</v>
+        <v>615</v>
       </c>
       <c r="H19" t="s">
         <v>81</v>
@@ -19946,7 +20249,7 @@
         <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>561</v>
+        <v>616</v>
       </c>
       <c r="H20" t="s">
         <v>284</v>
@@ -19969,7 +20272,7 @@
         <v>378</v>
       </c>
       <c r="F21" t="s">
-        <v>562</v>
+        <v>397</v>
       </c>
       <c r="H21" t="s">
         <v>285</v>
@@ -19992,7 +20295,7 @@
         <v>394</v>
       </c>
       <c r="F22" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="H22" t="s">
         <v>286</v>
@@ -20012,7 +20315,7 @@
         <v>395</v>
       </c>
       <c r="F23" t="s">
-        <v>51</v>
+        <v>562</v>
       </c>
       <c r="H23" t="s">
         <v>287</v>
@@ -20032,7 +20335,7 @@
         <v>342</v>
       </c>
       <c r="F24" t="s">
-        <v>52</v>
+        <v>563</v>
       </c>
       <c r="H24" t="s">
         <v>278</v>
@@ -20052,7 +20355,7 @@
         <v>379</v>
       </c>
       <c r="F25" t="s">
-        <v>516</v>
+        <v>51</v>
       </c>
       <c r="H25" t="s">
         <v>267</v>
@@ -20072,7 +20375,7 @@
         <v>551</v>
       </c>
       <c r="F26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H26" t="s">
         <v>67</v>
@@ -20081,7 +20384,7 @@
         <v>376</v>
       </c>
       <c r="AA26" t="s">
-        <v>520</v>
+        <v>617</v>
       </c>
       <c r="AG26" t="s">
         <v>223</v>
@@ -20092,7 +20395,7 @@
         <v>45</v>
       </c>
       <c r="F27" t="s">
-        <v>309</v>
+        <v>516</v>
       </c>
       <c r="H27" t="s">
         <v>270</v>
@@ -20101,7 +20404,7 @@
         <v>571</v>
       </c>
       <c r="AA27" t="s">
-        <v>100</v>
+        <v>520</v>
       </c>
       <c r="AG27" t="s">
         <v>224</v>
@@ -20112,7 +20415,7 @@
         <v>46</v>
       </c>
       <c r="F28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H28" t="s">
         <v>254</v>
@@ -20121,7 +20424,7 @@
         <v>503</v>
       </c>
       <c r="AA28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29">
@@ -20129,7 +20432,7 @@
         <v>47</v>
       </c>
       <c r="F29" t="s">
-        <v>429</v>
+        <v>309</v>
       </c>
       <c r="H29" t="s">
         <v>271</v>
@@ -20138,7 +20441,7 @@
         <v>76</v>
       </c>
       <c r="AA29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30">
@@ -20146,7 +20449,7 @@
         <v>587</v>
       </c>
       <c r="F30" t="s">
-        <v>212</v>
+        <v>54</v>
       </c>
       <c r="H30" t="s">
         <v>272</v>
@@ -20155,7 +20458,7 @@
         <v>416</v>
       </c>
       <c r="AA30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31">
@@ -20163,7 +20466,7 @@
         <v>48</v>
       </c>
       <c r="F31" t="s">
-        <v>213</v>
+        <v>429</v>
       </c>
       <c r="H31" t="s">
         <v>204</v>
@@ -20172,7 +20475,7 @@
         <v>37</v>
       </c>
       <c r="AA31" t="s">
-        <v>315</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32">
@@ -20180,7 +20483,7 @@
         <v>396</v>
       </c>
       <c r="F32" t="s">
-        <v>448</v>
+        <v>212</v>
       </c>
       <c r="H32" t="s">
         <v>263</v>
@@ -20189,7 +20492,7 @@
         <v>38</v>
       </c>
       <c r="AA32" t="s">
-        <v>104</v>
+        <v>315</v>
       </c>
     </row>
     <row r="33">
@@ -20197,139 +20500,145 @@
         <v>214</v>
       </c>
       <c r="F33" t="s">
-        <v>449</v>
+        <v>213</v>
       </c>
       <c r="H33" t="s">
         <v>273</v>
       </c>
       <c r="AA33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34">
       <c r="F34" t="s">
-        <v>398</v>
+        <v>448</v>
       </c>
       <c r="H34" t="s">
         <v>488</v>
       </c>
       <c r="AA34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35">
       <c r="F35" t="s">
-        <v>55</v>
+        <v>449</v>
       </c>
       <c r="H35" t="s">
         <v>248</v>
       </c>
       <c r="AA35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36">
       <c r="F36" t="s">
-        <v>56</v>
+        <v>398</v>
       </c>
       <c r="H36" t="s">
         <v>318</v>
       </c>
       <c r="AA36" t="s">
-        <v>521</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37">
       <c r="F37" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H37" t="s">
         <v>295</v>
       </c>
       <c r="AA37" t="s">
-        <v>108</v>
+        <v>521</v>
       </c>
     </row>
     <row r="38">
       <c r="F38" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H38" t="s">
         <v>249</v>
       </c>
       <c r="AA38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39">
       <c r="F39" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H39" t="s">
         <v>296</v>
       </c>
       <c r="AA39" t="s">
-        <v>198</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40">
       <c r="F40" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H40" t="s">
         <v>255</v>
       </c>
       <c r="AA40" t="s">
-        <v>110</v>
+        <v>198</v>
       </c>
     </row>
     <row r="41">
       <c r="F41" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H41" t="s">
         <v>603</v>
       </c>
       <c r="AA41" t="s">
-        <v>326</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42">
       <c r="F42" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H42" t="s">
         <v>69</v>
       </c>
       <c r="AA42" t="s">
-        <v>420</v>
+        <v>326</v>
       </c>
     </row>
     <row r="43">
       <c r="F43" t="s">
-        <v>574</v>
+        <v>61</v>
       </c>
       <c r="H43" t="s">
         <v>200</v>
       </c>
       <c r="AA43" t="s">
-        <v>530</v>
+        <v>420</v>
       </c>
     </row>
     <row r="44">
+      <c r="F44" t="s">
+        <v>62</v>
+      </c>
       <c r="H44" t="s">
         <v>517</v>
       </c>
       <c r="AA44" t="s">
-        <v>377</v>
+        <v>530</v>
       </c>
     </row>
     <row r="45">
+      <c r="F45" t="s">
+        <v>574</v>
+      </c>
       <c r="H45" t="s">
         <v>277</v>
       </c>
       <c r="AA45" t="s">
-        <v>111</v>
+        <v>377</v>
       </c>
     </row>
     <row r="46">
@@ -20337,7 +20646,7 @@
         <v>288</v>
       </c>
       <c r="AA46" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47">
@@ -20345,7 +20654,7 @@
         <v>289</v>
       </c>
       <c r="AA47" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48">
@@ -20353,7 +20662,7 @@
         <v>331</v>
       </c>
       <c r="AA48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49">
@@ -20361,7 +20670,7 @@
         <v>330</v>
       </c>
       <c r="AA49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50">
@@ -20369,7 +20678,7 @@
         <v>199</v>
       </c>
       <c r="AA50" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51">
@@ -20377,7 +20686,7 @@
         <v>308</v>
       </c>
       <c r="AA51" t="s">
-        <v>555</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52">
@@ -20385,7 +20694,7 @@
         <v>605</v>
       </c>
       <c r="AA52" t="s">
-        <v>201</v>
+        <v>555</v>
       </c>
     </row>
     <row r="53">
@@ -20393,7 +20702,7 @@
         <v>606</v>
       </c>
       <c r="AA53" t="s">
-        <v>68</v>
+        <v>201</v>
       </c>
     </row>
     <row r="54">
@@ -20401,7 +20710,7 @@
         <v>599</v>
       </c>
       <c r="AA54" t="s">
-        <v>514</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55">
@@ -20409,7 +20718,7 @@
         <v>600</v>
       </c>
       <c r="AA55" t="s">
-        <v>117</v>
+        <v>514</v>
       </c>
     </row>
     <row r="56">
@@ -20417,7 +20726,7 @@
         <v>327</v>
       </c>
       <c r="AA56" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="57">
@@ -20425,7 +20734,7 @@
         <v>353</v>
       </c>
       <c r="AA57" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="58">
@@ -20433,7 +20742,7 @@
         <v>290</v>
       </c>
       <c r="AA58" t="s">
-        <v>474</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59">
@@ -20441,7 +20750,7 @@
         <v>319</v>
       </c>
       <c r="AA59" t="s">
-        <v>443</v>
+        <v>474</v>
       </c>
     </row>
     <row r="60">
@@ -20449,7 +20758,7 @@
         <v>256</v>
       </c>
       <c r="AA60" t="s">
-        <v>120</v>
+        <v>443</v>
       </c>
     </row>
     <row r="61">
@@ -20457,7 +20766,7 @@
         <v>280</v>
       </c>
       <c r="AA61" t="s">
-        <v>334</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62">
@@ -20465,7 +20774,7 @@
         <v>281</v>
       </c>
       <c r="AA62" t="s">
-        <v>444</v>
+        <v>334</v>
       </c>
     </row>
     <row r="63">
@@ -20473,7 +20782,7 @@
         <v>518</v>
       </c>
       <c r="AA63" t="s">
-        <v>121</v>
+        <v>444</v>
       </c>
     </row>
     <row r="64">
@@ -20481,7 +20790,7 @@
         <v>282</v>
       </c>
       <c r="AA64" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65">
@@ -20489,7 +20798,7 @@
         <v>607</v>
       </c>
       <c r="AA65" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66">
@@ -20497,7 +20806,7 @@
         <v>300</v>
       </c>
       <c r="AA66" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="67">
@@ -20505,7 +20814,7 @@
         <v>613</v>
       </c>
       <c r="AA67" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="68">
@@ -20513,7 +20822,7 @@
         <v>614</v>
       </c>
       <c r="AA68" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="69">
@@ -20521,7 +20830,7 @@
         <v>325</v>
       </c>
       <c r="AA69" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="70">
@@ -20529,7 +20838,7 @@
         <v>297</v>
       </c>
       <c r="AA70" t="s">
-        <v>421</v>
+        <v>127</v>
       </c>
     </row>
     <row r="71">
@@ -20537,7 +20846,7 @@
         <v>298</v>
       </c>
       <c r="AA71" t="s">
-        <v>453</v>
+        <v>421</v>
       </c>
     </row>
     <row r="72">
@@ -20545,7 +20854,7 @@
         <v>354</v>
       </c>
       <c r="AA72" t="s">
-        <v>202</v>
+        <v>453</v>
       </c>
     </row>
     <row r="73">
@@ -20553,7 +20862,7 @@
         <v>355</v>
       </c>
       <c r="AA73" t="s">
-        <v>373</v>
+        <v>202</v>
       </c>
     </row>
     <row r="74">
@@ -20561,7 +20870,7 @@
         <v>333</v>
       </c>
       <c r="AA74" t="s">
-        <v>422</v>
+        <v>373</v>
       </c>
     </row>
     <row r="75">
@@ -20569,7 +20878,7 @@
         <v>301</v>
       </c>
       <c r="AA75" t="s">
-        <v>128</v>
+        <v>422</v>
       </c>
     </row>
     <row r="76">
@@ -20577,7 +20886,7 @@
         <v>257</v>
       </c>
       <c r="AA76" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="77">
@@ -20585,7 +20894,7 @@
         <v>504</v>
       </c>
       <c r="AA77" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="78">
@@ -20593,7 +20902,7 @@
         <v>302</v>
       </c>
       <c r="AA78" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="79">
@@ -20601,7 +20910,7 @@
         <v>392</v>
       </c>
       <c r="AA79" t="s">
-        <v>570</v>
+        <v>131</v>
       </c>
     </row>
     <row r="80">
@@ -20609,7 +20918,7 @@
         <v>608</v>
       </c>
       <c r="AA80" t="s">
-        <v>185</v>
+        <v>570</v>
       </c>
     </row>
     <row r="81">
@@ -20617,7 +20926,7 @@
         <v>609</v>
       </c>
       <c r="AA81" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="82">
@@ -20625,7 +20934,7 @@
         <v>250</v>
       </c>
       <c r="AA82" t="s">
-        <v>433</v>
+        <v>186</v>
       </c>
     </row>
     <row r="83">
@@ -20633,7 +20942,7 @@
         <v>489</v>
       </c>
       <c r="AA83" t="s">
-        <v>445</v>
+        <v>433</v>
       </c>
     </row>
     <row r="84">
@@ -20641,7 +20950,7 @@
         <v>332</v>
       </c>
       <c r="AA84" t="s">
-        <v>132</v>
+        <v>445</v>
       </c>
     </row>
     <row r="85">
@@ -20649,7 +20958,7 @@
         <v>268</v>
       </c>
       <c r="AA85" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="86">
@@ -20657,7 +20966,7 @@
         <v>611</v>
       </c>
       <c r="AA86" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="87">
@@ -20665,7 +20974,7 @@
         <v>610</v>
       </c>
       <c r="AA87" t="s">
-        <v>475</v>
+        <v>134</v>
       </c>
     </row>
     <row r="88">
@@ -20673,7 +20982,7 @@
         <v>279</v>
       </c>
       <c r="AA88" t="s">
-        <v>135</v>
+        <v>475</v>
       </c>
     </row>
     <row r="89">
@@ -20681,7 +20990,7 @@
         <v>411</v>
       </c>
       <c r="AA89" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="90">
@@ -20689,7 +20998,7 @@
         <v>320</v>
       </c>
       <c r="AA90"